<commit_message>
Calibrated both behavior and fear
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747554B2-5DB2-42AE-9343-A2A60F9163CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5E1029-671B-4A6D-9234-1376633EF072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Graphics" sheetId="2" r:id="rId2"/>
     <sheet name="Calibration2" sheetId="3" r:id="rId3"/>
     <sheet name="Graphics2" sheetId="4" r:id="rId4"/>
+    <sheet name="Behavior" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>[0.0</t>
   </si>
@@ -187,6 +188,15 @@
   </si>
   <si>
     <t>WO 0.4</t>
+  </si>
+  <si>
+    <t>Fear/35</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>fear*ℯ^(-time/300)</t>
   </si>
 </sst>
 </file>
@@ -692,16 +702,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>343714</xdr:colOff>
-      <xdr:row>170</xdr:row>
-      <xdr:rowOff>162453</xdr:rowOff>
+      <xdr:colOff>296089</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>38628</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -724,7 +734,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="28765500"/>
+          <a:off x="1028700" y="29022675"/>
           <a:ext cx="5830114" cy="3781953"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -781,15 +791,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>372293</xdr:colOff>
-      <xdr:row>192</xdr:row>
-      <xdr:rowOff>86242</xdr:rowOff>
+      <xdr:colOff>467543</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>105292</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -812,7 +822,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="32956500"/>
+          <a:off x="1171575" y="33166050"/>
           <a:ext cx="5858693" cy="3705742"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1490,6 +1500,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>172240</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152926</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79751C4F-6E8A-4025-8E8F-1BFE29051BA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="5658640" cy="3772426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1790,12 +1849,12 @@
   <dimension ref="A2:DI35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
@@ -6148,11 +6207,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A28FB15-96AC-4A27-8F42-1357F430FE8B}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O181" sqref="O181"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P77" sqref="P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6235,10 +6297,13 @@
   <dimension ref="A1:DI38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10214,7 +10279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0FAAD7-3AC8-479E-A3BF-9FE1F66B31C5}">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A148" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z100" sqref="Z100"/>
     </sheetView>
   </sheetViews>
@@ -10306,6 +10371,418 @@
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A765E4A-43AC-48A3-9F55-45170F1E0FC2}">
+  <dimension ref="A1:DW23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:127" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0.25</v>
+      </c>
+      <c r="D1">
+        <v>0.25</v>
+      </c>
+      <c r="E1">
+        <v>0.5</v>
+      </c>
+      <c r="F1">
+        <v>0.75</v>
+      </c>
+      <c r="G1">
+        <v>0.75</v>
+      </c>
+      <c r="H1">
+        <v>0.875</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>1</v>
+      </c>
+      <c r="P1">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>1.25</v>
+      </c>
+      <c r="R1">
+        <v>1.5</v>
+      </c>
+      <c r="S1">
+        <v>1.75</v>
+      </c>
+      <c r="T1">
+        <v>1.875</v>
+      </c>
+      <c r="U1">
+        <v>2.875</v>
+      </c>
+      <c r="V1">
+        <v>3.125</v>
+      </c>
+      <c r="W1">
+        <v>4.125</v>
+      </c>
+      <c r="X1">
+        <v>5.875</v>
+      </c>
+      <c r="Y1">
+        <v>8</v>
+      </c>
+      <c r="Z1">
+        <v>10.375</v>
+      </c>
+      <c r="AA1">
+        <v>13.125</v>
+      </c>
+      <c r="AB1">
+        <v>17.125</v>
+      </c>
+      <c r="AC1">
+        <v>18.5</v>
+      </c>
+      <c r="AD1">
+        <v>22.375</v>
+      </c>
+      <c r="AE1">
+        <v>29.125</v>
+      </c>
+      <c r="AF1">
+        <v>33.125</v>
+      </c>
+      <c r="AG1">
+        <v>37.125</v>
+      </c>
+      <c r="AH1">
+        <v>41.125</v>
+      </c>
+      <c r="AI1">
+        <v>44.5</v>
+      </c>
+      <c r="AJ1">
+        <v>43.875</v>
+      </c>
+      <c r="AK1">
+        <v>47</v>
+      </c>
+      <c r="AL1">
+        <v>55.25</v>
+      </c>
+      <c r="AM1">
+        <v>58.875</v>
+      </c>
+      <c r="AN1">
+        <v>62.75</v>
+      </c>
+      <c r="AO1">
+        <v>65.375</v>
+      </c>
+      <c r="AP1">
+        <v>65.5</v>
+      </c>
+      <c r="AQ1">
+        <v>62</v>
+      </c>
+      <c r="AR1">
+        <v>60.375</v>
+      </c>
+      <c r="AS1">
+        <v>58.75</v>
+      </c>
+      <c r="AT1">
+        <v>57.5</v>
+      </c>
+      <c r="AU1">
+        <v>56.25</v>
+      </c>
+      <c r="AV1">
+        <v>55.75</v>
+      </c>
+      <c r="AW1">
+        <v>54.5</v>
+      </c>
+      <c r="AX1">
+        <v>54</v>
+      </c>
+      <c r="AY1">
+        <v>54.25</v>
+      </c>
+      <c r="AZ1">
+        <v>53.625</v>
+      </c>
+      <c r="BA1">
+        <v>53.5</v>
+      </c>
+      <c r="BB1">
+        <v>53.375</v>
+      </c>
+      <c r="BC1">
+        <v>52.75</v>
+      </c>
+      <c r="BD1">
+        <v>52.375</v>
+      </c>
+      <c r="BE1">
+        <v>51.75</v>
+      </c>
+      <c r="BF1">
+        <v>52</v>
+      </c>
+      <c r="BG1">
+        <v>51.875</v>
+      </c>
+      <c r="BH1">
+        <v>51.75</v>
+      </c>
+      <c r="BI1">
+        <v>51.625</v>
+      </c>
+      <c r="BJ1">
+        <v>51.25</v>
+      </c>
+      <c r="BK1">
+        <v>50.75</v>
+      </c>
+      <c r="BL1">
+        <v>50</v>
+      </c>
+      <c r="BM1">
+        <v>50.375</v>
+      </c>
+      <c r="BN1">
+        <v>50.25</v>
+      </c>
+      <c r="BO1">
+        <v>50</v>
+      </c>
+      <c r="BP1">
+        <v>49.75</v>
+      </c>
+      <c r="BQ1">
+        <v>49.75</v>
+      </c>
+      <c r="BR1">
+        <v>48.75</v>
+      </c>
+      <c r="BS1">
+        <v>48.375</v>
+      </c>
+      <c r="BT1">
+        <v>49.375</v>
+      </c>
+      <c r="BU1">
+        <v>49.5</v>
+      </c>
+      <c r="BV1">
+        <v>49.375</v>
+      </c>
+      <c r="BW1">
+        <v>49.25</v>
+      </c>
+      <c r="BX1">
+        <v>48.875</v>
+      </c>
+      <c r="BY1">
+        <v>47.875</v>
+      </c>
+      <c r="BZ1">
+        <v>46.875</v>
+      </c>
+      <c r="CA1">
+        <v>47.625</v>
+      </c>
+      <c r="CB1">
+        <v>47.625</v>
+      </c>
+      <c r="CC1">
+        <v>47.375</v>
+      </c>
+      <c r="CD1">
+        <v>47</v>
+      </c>
+      <c r="CE1">
+        <v>46.875</v>
+      </c>
+      <c r="CF1">
+        <v>45.875</v>
+      </c>
+      <c r="CG1">
+        <v>45</v>
+      </c>
+      <c r="CH1">
+        <v>45.25</v>
+      </c>
+      <c r="CI1">
+        <v>45.25</v>
+      </c>
+      <c r="CJ1">
+        <v>45.25</v>
+      </c>
+      <c r="CK1">
+        <v>44.875</v>
+      </c>
+      <c r="CL1">
+        <v>44.375</v>
+      </c>
+      <c r="CM1">
+        <v>43.5</v>
+      </c>
+      <c r="CN1">
+        <v>43</v>
+      </c>
+      <c r="CO1">
+        <v>43.125</v>
+      </c>
+      <c r="CP1">
+        <v>42.75</v>
+      </c>
+      <c r="CQ1">
+        <v>42.625</v>
+      </c>
+      <c r="CR1">
+        <v>42.5</v>
+      </c>
+      <c r="CS1">
+        <v>42.125</v>
+      </c>
+      <c r="CT1">
+        <v>41.5</v>
+      </c>
+      <c r="CU1">
+        <v>41.25</v>
+      </c>
+      <c r="CV1">
+        <v>41</v>
+      </c>
+      <c r="CW1">
+        <v>40.75</v>
+      </c>
+      <c r="CX1">
+        <v>40.5</v>
+      </c>
+      <c r="CY1">
+        <v>40.375</v>
+      </c>
+      <c r="CZ1">
+        <v>39.875</v>
+      </c>
+      <c r="DA1">
+        <v>39.5</v>
+      </c>
+      <c r="DB1">
+        <v>39.125</v>
+      </c>
+      <c r="DC1">
+        <v>39</v>
+      </c>
+      <c r="DD1">
+        <v>39</v>
+      </c>
+      <c r="DE1">
+        <v>38.625</v>
+      </c>
+      <c r="DF1">
+        <v>38.5</v>
+      </c>
+      <c r="DG1">
+        <v>38</v>
+      </c>
+      <c r="DH1">
+        <v>37.75</v>
+      </c>
+      <c r="DI1">
+        <v>37.5</v>
+      </c>
+      <c r="DJ1">
+        <v>37.375</v>
+      </c>
+      <c r="DK1">
+        <v>37.125</v>
+      </c>
+      <c r="DL1">
+        <v>37</v>
+      </c>
+      <c r="DM1">
+        <v>36.75</v>
+      </c>
+      <c r="DN1">
+        <v>36.25</v>
+      </c>
+      <c r="DO1">
+        <v>36.125</v>
+      </c>
+      <c r="DP1">
+        <v>35.875</v>
+      </c>
+      <c r="DQ1">
+        <v>35.75</v>
+      </c>
+      <c r="DR1">
+        <v>35.625</v>
+      </c>
+      <c r="DS1">
+        <v>35.375</v>
+      </c>
+      <c r="DT1">
+        <v>35</v>
+      </c>
+      <c r="DU1">
+        <v>34.875</v>
+      </c>
+      <c r="DV1">
+        <v>34.75</v>
+      </c>
+      <c r="DW1">
+        <v>34.375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:127" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further calibration and peek in to message governed behavior
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5E1029-671B-4A6D-9234-1376633EF072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C5B258-0638-4406-84BC-39CA564D5CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Graphics" sheetId="2" r:id="rId2"/>
     <sheet name="Calibration2" sheetId="3" r:id="rId3"/>
     <sheet name="Graphics2" sheetId="4" r:id="rId4"/>
-    <sheet name="Behavior" sheetId="5" r:id="rId5"/>
+    <sheet name="Calib2" sheetId="5" r:id="rId5"/>
+    <sheet name="Conclusion" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>[0.0</t>
   </si>
@@ -196,7 +196,136 @@
     <t>Binary</t>
   </si>
   <si>
-    <t>fear*ℯ^(-time/300)</t>
+    <t>fear*(1-ℯ^(-time/10))</t>
+  </si>
+  <si>
+    <t>Fear/xY, Time/300</t>
+  </si>
+  <si>
+    <t>fear*ℯ^(-(time/250))</t>
+  </si>
+  <si>
+    <t>Error 17.27</t>
+  </si>
+  <si>
+    <t>Decay 250, growth 1.45</t>
+  </si>
+  <si>
+    <t>Fear-0.5, growth 1.3</t>
+  </si>
+  <si>
+    <t>Behavior 30.88, Fear 19.97</t>
+  </si>
+  <si>
+    <t>Growth 1.3, Fear -0.5 from Day 20 105</t>
+  </si>
+  <si>
+    <t>Growth 1.3, Fear -0.5 from Day 15 105</t>
+  </si>
+  <si>
+    <t>Fear 26.29</t>
+  </si>
+  <si>
+    <t>Behavior 26.21</t>
+  </si>
+  <si>
+    <t>fear*(1-ℯ^(-time/10)), Growth 1.4</t>
+  </si>
+  <si>
+    <t>W 0.4 decay</t>
+  </si>
+  <si>
+    <t>Growth 1.3, from Day 15 105, no Decay</t>
+  </si>
+  <si>
+    <t>error behavior is 48.357773372401155</t>
+  </si>
+  <si>
+    <t>error fear is 34.426016737444655</t>
+  </si>
+  <si>
+    <t>Day 30</t>
+  </si>
+  <si>
+    <t>error behavior is 34.74563407944974</t>
+  </si>
+  <si>
+    <t>error fear is 24.658918835546512</t>
+  </si>
+  <si>
+    <t>Day 25</t>
+  </si>
+  <si>
+    <t>error behavior is 39.35432556128484</t>
+  </si>
+  <si>
+    <t>error fear is 26.722525721509417</t>
+  </si>
+  <si>
+    <t>Growth 1.3, Fear -0.4 from 10 109, if decay else growth</t>
+  </si>
+  <si>
+    <t>error behavior is 32.738740040670336</t>
+  </si>
+  <si>
+    <t>error fear is 14.655055421999947</t>
+  </si>
+  <si>
+    <t>Infection Curve</t>
+  </si>
+  <si>
+    <t>Behavior&gt;100</t>
+  </si>
+  <si>
+    <t>Behavior &gt;50</t>
+  </si>
+  <si>
+    <t>Using Norms(Social Distancing) and Attitude (Health Facts)</t>
+  </si>
+  <si>
+    <t>Validation for other behavior</t>
+  </si>
+  <si>
+    <t>Fear=norms*14</t>
+  </si>
+  <si>
+    <t>behavior=norm+attitude/2*fear/110+attitude*1500</t>
+  </si>
+  <si>
+    <t>error behavior is 58.738736911719634</t>
+  </si>
+  <si>
+    <t>error fear is 20.036458713563174</t>
+  </si>
+  <si>
+    <t>Reasons for this:</t>
+  </si>
+  <si>
+    <t>Behavior is governed by media, messages on social distancing+norms</t>
+  </si>
+  <si>
+    <t>First fear by COVID unknown, thi s is accompanied by guidelines how we should behave - SD etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This needs some time to process, adaption is slow and also governed by regular norms we see+attitude, is then further supported by facts. </t>
+  </si>
+  <si>
+    <t>H1 - The model can replicate the trends of infection in Germany</t>
+  </si>
+  <si>
+    <t>H2 - The model can replicate the trends of behavior and fear in Germany</t>
+  </si>
+  <si>
+    <t>H3 - Fear can explain the behavior - is our prediction better than the tell me model</t>
+  </si>
+  <si>
+    <t>H4 - The course of the epidemic is significantly influenced by individual behavior change</t>
+  </si>
+  <si>
+    <t>H5 - The course of the epidemic is significantly influenced by the communication strategy</t>
+  </si>
+  <si>
+    <t>Fear+Norm+Attitude/3</t>
   </si>
 </sst>
 </file>
@@ -1546,6 +1675,759 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>105555</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>133874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70297372-9B48-4760-9275-E5EB667087E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="4572000"/>
+          <a:ext cx="5591955" cy="3753374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>391345</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>95768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1783644-62D7-4A50-8A40-DC728376879E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8763000"/>
+          <a:ext cx="5877745" cy="3715268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>343714</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>114821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED828B5B-A408-4F5E-A02F-7559A6F002F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12763500"/>
+          <a:ext cx="5830114" cy="3734321"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>124608</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>171979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FC33496-60BA-4602-BA14-EF19F2475EDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16954500"/>
+          <a:ext cx="5611008" cy="3791479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>238924</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>76733</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE21B33D-EC8B-4007-B6D5-470CB6ECCC17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="17021175"/>
+          <a:ext cx="5725324" cy="3820058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>238924</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>19584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F2A0DAC-51E0-4929-BA1A-A43182B1943E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15240000" y="16954500"/>
+          <a:ext cx="5725324" cy="3829584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>172240</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>171979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4D029C6-C07C-48C3-9E91-0458CF9B9733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23774400" y="16954500"/>
+          <a:ext cx="5658640" cy="3791479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>296082</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>143400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{650F50EB-363A-4B47-86A5-C43E93F6912F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="5782482" cy="3762900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>571405</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2AE90D6-A692-4C5A-B414-BD6D20DCC589}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7124701" y="200026"/>
+          <a:ext cx="5638704" cy="3752850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>334165</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A802E3-E305-4828-AE31-5A49130A13FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573125" y="171450"/>
+          <a:ext cx="5658640" cy="3772426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>372274</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>105308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90561DB9-B29C-4E92-958F-237C38C9A97D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="8858250"/>
+          <a:ext cx="5725324" cy="3820058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>277029</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C0DE5DD-5453-4640-9B7B-38A86291E9BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4619625"/>
+          <a:ext cx="5763429" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>115082</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>162453</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F18E401-DFF5-44F0-B37B-A42D5C11A3FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12954000"/>
+          <a:ext cx="5601482" cy="3781953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>383121</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADEE0950-50CC-4CAB-8317-C8C0913249FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="17145000"/>
+          <a:ext cx="5869520" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>108024</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>57464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{323B66C8-E942-4186-A761-881679BDD9BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="31337250"/>
+          <a:ext cx="3781953" cy="2248214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>550011</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05B4EADB-72AC-4181-8D22-E026BEB139F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21635357"/>
+          <a:ext cx="6060904" cy="3959679"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>307058</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>180220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1985F2CB-B00F-4E5F-B477-4F28EC23AA08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="26697214"/>
+          <a:ext cx="6430272" cy="4344006"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1848,7 +2730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF31E81-C5FF-4FF4-91BB-CCFB43A88A47}">
   <dimension ref="A2:DI35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -6207,8 +7089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A28FB15-96AC-4A27-8F42-1357F430FE8B}">
   <dimension ref="A1:M174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P77" sqref="P77"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6297,7 +7179,7 @@
   <dimension ref="A1:DI38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10279,8 +11161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0FAAD7-3AC8-479E-A3BF-9FE1F66B31C5}">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z100" sqref="Z100"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10381,10 +11263,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A765E4A-43AC-48A3-9F55-45170F1E0FC2}">
-  <dimension ref="A1:DW23"/>
+  <dimension ref="A1:DW92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="K70" workbookViewId="0">
+      <selection activeCell="AY99" sqref="AY99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10780,9 +11662,582 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="3" spans="1:127" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:126" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" t="s">
+        <v>54</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0.25</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0.5</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0.5</v>
+      </c>
+      <c r="AD24">
+        <v>1.25</v>
+      </c>
+      <c r="AE24">
+        <v>1.25</v>
+      </c>
+      <c r="AF24">
+        <v>2</v>
+      </c>
+      <c r="AG24">
+        <v>3.5</v>
+      </c>
+      <c r="AH24">
+        <v>4</v>
+      </c>
+      <c r="AI24">
+        <v>3.5</v>
+      </c>
+      <c r="AJ24">
+        <v>5.75</v>
+      </c>
+      <c r="AK24">
+        <v>10</v>
+      </c>
+      <c r="AL24">
+        <v>14.5</v>
+      </c>
+      <c r="AM24">
+        <v>17.25</v>
+      </c>
+      <c r="AN24">
+        <v>23.75</v>
+      </c>
+      <c r="AO24">
+        <v>30.75</v>
+      </c>
+      <c r="AP24">
+        <v>30.25</v>
+      </c>
+      <c r="AQ24">
+        <v>33</v>
+      </c>
+      <c r="AR24">
+        <v>49</v>
+      </c>
+      <c r="AS24">
+        <v>56</v>
+      </c>
+      <c r="AT24">
+        <v>63.75</v>
+      </c>
+      <c r="AU24">
+        <v>69.25</v>
+      </c>
+      <c r="AV24">
+        <v>79.25</v>
+      </c>
+      <c r="AW24">
+        <v>69.5</v>
+      </c>
+      <c r="AX24">
+        <v>79</v>
+      </c>
+      <c r="AY24">
+        <v>100</v>
+      </c>
+      <c r="AZ24">
+        <v>102</v>
+      </c>
+      <c r="BA24">
+        <v>108</v>
+      </c>
+      <c r="BB24">
+        <v>109.5</v>
+      </c>
+      <c r="BC24">
+        <v>117.75</v>
+      </c>
+      <c r="BD24">
+        <v>103.25</v>
+      </c>
+      <c r="BE24">
+        <v>103.5</v>
+      </c>
+      <c r="BF24">
+        <v>110</v>
+      </c>
+      <c r="BG24">
+        <v>111.75</v>
+      </c>
+      <c r="BH24">
+        <v>113</v>
+      </c>
+      <c r="BI24">
+        <v>114.5</v>
+      </c>
+      <c r="BJ24">
+        <v>116</v>
+      </c>
+      <c r="BK24">
+        <v>111.75</v>
+      </c>
+      <c r="BL24">
+        <v>113.5</v>
+      </c>
+      <c r="BM24">
+        <v>116.5</v>
+      </c>
+      <c r="BN24">
+        <v>116.75</v>
+      </c>
+      <c r="BO24">
+        <v>116</v>
+      </c>
+      <c r="BP24">
+        <v>116</v>
+      </c>
+      <c r="BQ24">
+        <v>115.75</v>
+      </c>
+      <c r="BR24">
+        <v>114.5</v>
+      </c>
+      <c r="BS24">
+        <v>113.75</v>
+      </c>
+      <c r="BT24">
+        <v>115</v>
+      </c>
+      <c r="BU24">
+        <v>114.75</v>
+      </c>
+      <c r="BV24">
+        <v>114</v>
+      </c>
+      <c r="BW24">
+        <v>113.75</v>
+      </c>
+      <c r="BX24">
+        <v>113</v>
+      </c>
+      <c r="BY24">
+        <v>111</v>
+      </c>
+      <c r="BZ24">
+        <v>110.25</v>
+      </c>
+      <c r="CA24">
+        <v>111.75</v>
+      </c>
+      <c r="CB24">
+        <v>110.5</v>
+      </c>
+      <c r="CC24">
+        <v>110.25</v>
+      </c>
+      <c r="CD24">
+        <v>109</v>
+      </c>
+      <c r="CE24">
+        <v>108.75</v>
+      </c>
+      <c r="CF24">
+        <v>105.25</v>
+      </c>
+      <c r="CG24">
+        <v>103.75</v>
+      </c>
+      <c r="CH24">
+        <v>109</v>
+      </c>
+      <c r="CI24">
+        <v>107.5</v>
+      </c>
+      <c r="CJ24">
+        <v>106.5</v>
+      </c>
+      <c r="CK24">
+        <v>106</v>
+      </c>
+      <c r="CL24">
+        <v>104.5</v>
+      </c>
+      <c r="CM24">
+        <v>92.5</v>
+      </c>
+      <c r="CN24">
+        <v>91.5</v>
+      </c>
+      <c r="CO24">
+        <v>103.25</v>
+      </c>
+      <c r="CP24">
+        <v>99.75</v>
+      </c>
+      <c r="CQ24">
+        <v>99.5</v>
+      </c>
+      <c r="CR24">
+        <v>97</v>
+      </c>
+      <c r="CS24">
+        <v>96.25</v>
+      </c>
+      <c r="CT24">
+        <v>79.5</v>
+      </c>
+      <c r="CU24">
+        <v>77.5</v>
+      </c>
+      <c r="CV24">
+        <v>97.25</v>
+      </c>
+      <c r="CW24">
+        <v>93.75</v>
+      </c>
+      <c r="CX24">
+        <v>94</v>
+      </c>
+      <c r="CY24">
+        <v>90</v>
+      </c>
+      <c r="CZ24">
+        <v>88.25</v>
+      </c>
+      <c r="DA24">
+        <v>67</v>
+      </c>
+      <c r="DB24">
+        <v>64.5</v>
+      </c>
+      <c r="DC24">
+        <v>90.5</v>
+      </c>
+      <c r="DD24">
+        <v>83.75</v>
+      </c>
+      <c r="DE24">
+        <v>83.25</v>
+      </c>
+      <c r="DF24">
+        <v>79</v>
+      </c>
+      <c r="DG24">
+        <v>75.75</v>
+      </c>
+      <c r="DH24">
+        <v>56.25</v>
+      </c>
+      <c r="DI24">
+        <v>50.5</v>
+      </c>
+      <c r="DJ24">
+        <v>73.5</v>
+      </c>
+      <c r="DK24">
+        <v>65.5</v>
+      </c>
+      <c r="DL24">
+        <v>63.75</v>
+      </c>
+      <c r="DM24">
+        <v>62.25</v>
+      </c>
+      <c r="DN24">
+        <v>67</v>
+      </c>
+      <c r="DO24">
+        <v>42</v>
+      </c>
+      <c r="DP24">
+        <v>41</v>
+      </c>
+      <c r="DQ24">
+        <v>58.25</v>
+      </c>
+      <c r="DR24">
+        <v>54.25</v>
+      </c>
+      <c r="DS24">
+        <v>52.5</v>
+      </c>
+      <c r="DT24">
+        <v>46.25</v>
+      </c>
+      <c r="DU24">
+        <v>41.75</v>
+      </c>
+      <c r="DV24">
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:126" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="K46">
+        <v>33.75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>59</v>
+      </c>
+      <c r="M89" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z89" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN89" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="90" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="K90">
+        <v>32.840000000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="K91">
+        <v>24.905000000000001</v>
+      </c>
+      <c r="W91" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ91" t="s">
+        <v>69</v>
+      </c>
+      <c r="AX91" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="W92" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ92" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
+  <dimension ref="A1:AG164"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>26.88</v>
+      </c>
+      <c r="V2">
+        <v>24.58</v>
+      </c>
+      <c r="AG2">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K69" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K70" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" t="s">
+        <v>78</v>
+      </c>
+      <c r="K90" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N95" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N103" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="106" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N106" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>80</v>
+      </c>
+      <c r="G113" t="s">
+        <v>82</v>
+      </c>
+      <c r="H113" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L115" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L116" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q118" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q119" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing for HPC and further Validation
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C5B258-0638-4406-84BC-39CA564D5CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C42117-0031-467C-87E1-526B9CA8ED7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
@@ -12086,7 +12086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
   <dimension ref="A1:AG164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ready to try HPC
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C42117-0031-467C-87E1-526B9CA8ED7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D169FAA-B1D4-4EB3-A2AF-3D316B8F046E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
   <si>
     <t>[0.0</t>
   </si>
@@ -327,12 +327,84 @@
   <si>
     <t>Fear+Norm+Attitude/3</t>
   </si>
+  <si>
+    <t>-&gt; behavior = norms+attitude messages + perceived norm+my old attitude</t>
+  </si>
+  <si>
+    <t>Behavior &gt; 30, Risk 0.5</t>
+  </si>
+  <si>
+    <t>Risk 1, Behavior 50, Small Behavior True Risk</t>
+  </si>
+  <si>
+    <t>export LD_LIBRARY_PATH=$HOME/bin/julia-v0.6/lib:$LD_LIBRARY_PATH</t>
+  </si>
+  <si>
+    <t>export CPATH=$HOME/bin/julia-v0.6/include:$CPATH</t>
+  </si>
+  <si>
+    <t>export PATH=$~/bin/julia-1.5.0/bin:$PATH</t>
+  </si>
+  <si>
+    <t>Behavior 70, Risk 0.7</t>
+  </si>
+  <si>
+    <t>If Behavior Risk/10</t>
+  </si>
+  <si>
+    <t>error behavior is 42.96230664485535</t>
+  </si>
+  <si>
+    <t>error fear is 29.43449361204646</t>
+  </si>
+  <si>
+    <t>error infected is 636.1314598220791</t>
+  </si>
+  <si>
+    <t>If Behavior Risk/10 also in :Q</t>
+  </si>
+  <si>
+    <t>error behavior is 32.17801723541984</t>
+  </si>
+  <si>
+    <t>error fear is 29.739989900782476</t>
+  </si>
+  <si>
+    <t>error infected is 167.95065102186467</t>
+  </si>
+  <si>
+    <t>All behavior leads to no Inf Risk</t>
+  </si>
+  <si>
+    <t>Contacts/2</t>
+  </si>
+  <si>
+    <t>error behavior is 37.65369540817264</t>
+  </si>
+  <si>
+    <t>error fear is 35.45577318141028</t>
+  </si>
+  <si>
+    <t>error infected is 1884.744060387621</t>
+  </si>
+  <si>
+    <t>error behavior is 30.80015398195664</t>
+  </si>
+  <si>
+    <t>error fear is 28.058950945826588</t>
+  </si>
+  <si>
+    <t>error infected is 606.5801717568814</t>
+  </si>
+  <si>
+    <t>Risk*0.65, Behavior 70, If behavior Risk/10, 3days infection delay,max 40% increase and 10% daily decrease fear</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +417,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,9 +444,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2035,15 +2115,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>571405</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9430</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2066,7 +2146,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7124701" y="200026"/>
+          <a:off x="7172326" y="428626"/>
           <a:ext cx="5638704" cy="3752850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2428,6 +2508,480 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D73816A6-6B30-4A29-8672-FDDFECB98AE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5629275" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6802A5-FDA5-4410-9F6A-1C5AC71FFD25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5629275" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>134339</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7CAED8C-8F0B-4876-9B63-5CC2BC825FF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7900147" y="23834912"/>
+          <a:ext cx="6331324" cy="4112427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>60159</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>143400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E86207-F0A4-48FE-9238-3F7B2CA3A64C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7866529" y="28384500"/>
+          <a:ext cx="5506218" cy="3762900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88738</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>181505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A52B8AB-1600-494B-A67C-F69A07EEBF6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="34290000"/>
+          <a:ext cx="5534797" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>87609</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>170299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95469E4D-2571-499F-94B4-BF9A8DD67802}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6107205" y="34278794"/>
+          <a:ext cx="5477639" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>593003</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01C5F41-91AF-4A25-99F8-3F737A6CC3E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14421971" y="34290000"/>
+          <a:ext cx="5534797" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>250687</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>143400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC61CEF-C8AE-4E47-8207-6F4CD6BCC5CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14522824" y="38481000"/>
+          <a:ext cx="5696745" cy="3762900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>512855</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>171953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CDFFC53-D44D-4383-A94B-35B83C4D7B0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="38481000"/>
+          <a:ext cx="5353797" cy="3600953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>346341</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>57583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6FB0EBF-00A3-4276-B721-CB3BCDF33F1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14522824" y="42672000"/>
+          <a:ext cx="4582164" cy="3105583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2734,7 +3288,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
@@ -2784,12 +3338,12 @@
     <col min="82" max="82" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3046,12 +3600,12 @@
         <v>10024</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -3305,7 +3859,7 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -3313,7 +3867,7 @@
         <v>205.27437525948699</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3570,7 +4124,7 @@
         <v>9699.625</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -3578,7 +4132,7 @@
         <v>1599.18</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3835,7 +4389,7 @@
         <v>9201.25</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -3843,7 +4397,7 @@
         <v>1256.78</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4100,12 +4654,12 @@
         <v>7841</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -4362,12 +4916,12 @@
         <v>6833.5</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85">
       <c r="B16">
         <v>779.62</v>
       </c>
     </row>
-    <row r="18" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:113">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -4624,7 +5178,7 @@
         <v>93.5</v>
       </c>
     </row>
-    <row r="19" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:113">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -4632,7 +5186,7 @@
         <v>42.923092111405701</v>
       </c>
     </row>
-    <row r="20" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:113">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4973,7 +5527,7 @@
         <v>36.625</v>
       </c>
     </row>
-    <row r="21" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:113">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -4981,7 +5535,7 @@
         <v>46.31</v>
       </c>
     </row>
-    <row r="22" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:113">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -5322,12 +5876,12 @@
         <v>41.375</v>
       </c>
     </row>
-    <row r="23" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:113">
       <c r="B23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:113">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -5668,12 +6222,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:113">
       <c r="B25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:113">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -6014,7 +6568,7 @@
         <v>38.625</v>
       </c>
     </row>
-    <row r="27" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:113">
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -6022,17 +6576,17 @@
         <v>50.26</v>
       </c>
     </row>
-    <row r="28" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:113">
       <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:113">
       <c r="B29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:113">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -6373,7 +6927,7 @@
         <v>37.75</v>
       </c>
     </row>
-    <row r="31" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:113">
       <c r="B31" t="s">
         <v>4</v>
       </c>
@@ -6381,7 +6935,7 @@
         <v>16.84</v>
       </c>
     </row>
-    <row r="32" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:113">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -6722,7 +7276,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:113">
       <c r="B33" t="s">
         <v>4</v>
       </c>
@@ -6730,7 +7284,7 @@
         <v>17.95</v>
       </c>
     </row>
-    <row r="34" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:113">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -7071,7 +7625,7 @@
         <v>43.375</v>
       </c>
     </row>
-    <row r="35" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:113">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -7093,77 +7647,77 @@
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="M2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="M23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="13:13">
       <c r="M44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1">
       <c r="A111" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1">
       <c r="A131" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1">
       <c r="A152" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1">
       <c r="A172" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1">
       <c r="A174" t="s">
         <v>30</v>
       </c>
@@ -7182,12 +7736,12 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -7195,7 +7749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -7452,12 +8006,12 @@
         <v>21.125</v>
       </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85">
       <c r="B3">
         <v>44.052939072790302</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -7630,12 +8184,12 @@
         <v>45.375</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85">
       <c r="B5">
         <v>25.03</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -7808,7 +8362,7 @@
         <v>47.125</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -7981,12 +8535,12 @@
         <v>141.375</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85">
       <c r="B9">
         <v>33.729999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -8159,12 +8713,12 @@
         <v>113.25</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85">
       <c r="B11">
         <v>31.35</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -8337,12 +8891,12 @@
         <v>129.75</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85">
       <c r="B13">
         <v>22.41</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -8515,12 +9069,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85">
       <c r="B15">
         <v>9.17</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -8693,12 +9247,12 @@
         <v>108.625</v>
       </c>
     </row>
-    <row r="17" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:113">
       <c r="B17">
         <v>13.268000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:113">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -8871,12 +9425,12 @@
         <v>118.25</v>
       </c>
     </row>
-    <row r="19" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:113">
       <c r="B19">
         <v>23.65</v>
       </c>
     </row>
-    <row r="20" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:113">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -9049,12 +9603,12 @@
         <v>96.25</v>
       </c>
     </row>
-    <row r="21" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:113">
       <c r="B21">
         <v>56.04</v>
       </c>
     </row>
-    <row r="22" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:113">
       <c r="B22">
         <v>0</v>
       </c>
@@ -9224,12 +9778,12 @@
         <v>109.125</v>
       </c>
     </row>
-    <row r="23" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:113">
       <c r="B23">
         <v>17.079999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:113">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -9402,17 +9956,17 @@
         <v>98.625</v>
       </c>
     </row>
-    <row r="25" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:113">
       <c r="B25">
         <v>14.08</v>
       </c>
     </row>
-    <row r="26" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:113">
       <c r="A26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:113">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -9753,12 +10307,12 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="28" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:113">
       <c r="B28">
         <v>14.81</v>
       </c>
     </row>
-    <row r="29" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:113">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -10099,17 +10653,17 @@
         <v>87.25</v>
       </c>
     </row>
-    <row r="30" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:113">
       <c r="B30">
         <v>18.59</v>
       </c>
     </row>
-    <row r="31" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:113">
       <c r="A31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:113">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -10450,12 +11004,12 @@
         <v>69.125</v>
       </c>
     </row>
-    <row r="33" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:113">
       <c r="B33">
         <v>33.42</v>
       </c>
     </row>
-    <row r="34" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:113">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -10733,7 +11287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:113">
       <c r="B35">
         <v>78</v>
       </c>
@@ -10801,12 +11355,12 @@
         <v>69.625</v>
       </c>
     </row>
-    <row r="36" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:113">
       <c r="B36">
         <v>24.58</v>
       </c>
     </row>
-    <row r="37" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:113">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -11147,7 +11701,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:113">
       <c r="B38">
         <v>26.88</v>
       </c>
@@ -11165,9 +11719,9 @@
       <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -11175,82 +11729,82 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="L2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="L24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="L25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="L46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="L67" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12">
       <c r="L89" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1">
       <c r="A108" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1">
       <c r="A130" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1">
       <c r="A151" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1">
       <c r="A152" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1">
       <c r="A173" t="s">
         <v>42</v>
       </c>
@@ -11269,9 +11823,9 @@
       <selection activeCell="AY99" sqref="AY99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:127">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -11654,7 +12208,7 @@
         <v>34.375</v>
       </c>
     </row>
-    <row r="2" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:127">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -11662,12 +12216,12 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="3" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:127">
       <c r="L3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:126">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -12011,12 +12565,12 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="25" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:126">
       <c r="L25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -12024,7 +12578,7 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -12032,7 +12586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:50">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -12046,12 +12600,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:50">
       <c r="K90">
         <v>32.840000000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:50">
       <c r="K91">
         <v>24.905000000000001</v>
       </c>
@@ -12065,7 +12619,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="92" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:50">
       <c r="W92" t="s">
         <v>62</v>
       </c>
@@ -12084,15 +12638,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
-  <dimension ref="A1:AG164"/>
+  <dimension ref="A1:AI227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="G197" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y224" sqref="Y224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -12103,7 +12657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="K2">
         <v>26.88</v>
       </c>
@@ -12114,7 +12668,7 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -12122,42 +12676,57 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="K47" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="K48" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21">
       <c r="A68" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21">
       <c r="K69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21">
       <c r="K70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21">
+      <c r="U77" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
+      <c r="U78" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21">
+      <c r="U79" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -12168,32 +12737,32 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14">
       <c r="N92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14">
       <c r="N95" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="14:14">
       <c r="N99" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="14:14">
       <c r="N103" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="14:14">
       <c r="N106" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -12204,7 +12773,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17">
       <c r="L115" t="s">
         <v>84</v>
       </c>
@@ -12212,7 +12781,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17">
       <c r="L116" t="s">
         <v>85</v>
       </c>
@@ -12220,29 +12789,123 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17">
       <c r="Q118" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17">
       <c r="Q119" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17">
+      <c r="Q120" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="N125" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
       <c r="A140" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="14:14">
+      <c r="N149" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
       <c r="A164" t="s">
         <v>81</v>
       </c>
     </row>
+    <row r="180" spans="1:34">
+      <c r="A180" t="s">
+        <v>102</v>
+      </c>
+      <c r="K180" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y180" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="181" spans="1:34">
+      <c r="U181" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH181" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="182" spans="1:34">
+      <c r="U182" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH182" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="183" spans="1:34">
+      <c r="U183" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH183" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="202" spans="11:25">
+      <c r="K202" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y202" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="203" spans="11:25">
+      <c r="U203" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="204" spans="11:25">
+      <c r="U204" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="205" spans="11:25">
+      <c r="U205" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="224" spans="25:25">
+      <c r="Y224" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="225" spans="35:35">
+      <c r="AI225" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="226" spans="35:35">
+      <c r="AI226" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="227" spans="35:35">
+      <c r="AI227" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cleaned up code and ready to start with messages
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C42117-0031-467C-87E1-526B9CA8ED7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D169FAA-B1D4-4EB3-A2AF-3D316B8F046E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
   <si>
     <t>[0.0</t>
   </si>
@@ -327,12 +327,84 @@
   <si>
     <t>Fear+Norm+Attitude/3</t>
   </si>
+  <si>
+    <t>-&gt; behavior = norms+attitude messages + perceived norm+my old attitude</t>
+  </si>
+  <si>
+    <t>Behavior &gt; 30, Risk 0.5</t>
+  </si>
+  <si>
+    <t>Risk 1, Behavior 50, Small Behavior True Risk</t>
+  </si>
+  <si>
+    <t>export LD_LIBRARY_PATH=$HOME/bin/julia-v0.6/lib:$LD_LIBRARY_PATH</t>
+  </si>
+  <si>
+    <t>export CPATH=$HOME/bin/julia-v0.6/include:$CPATH</t>
+  </si>
+  <si>
+    <t>export PATH=$~/bin/julia-1.5.0/bin:$PATH</t>
+  </si>
+  <si>
+    <t>Behavior 70, Risk 0.7</t>
+  </si>
+  <si>
+    <t>If Behavior Risk/10</t>
+  </si>
+  <si>
+    <t>error behavior is 42.96230664485535</t>
+  </si>
+  <si>
+    <t>error fear is 29.43449361204646</t>
+  </si>
+  <si>
+    <t>error infected is 636.1314598220791</t>
+  </si>
+  <si>
+    <t>If Behavior Risk/10 also in :Q</t>
+  </si>
+  <si>
+    <t>error behavior is 32.17801723541984</t>
+  </si>
+  <si>
+    <t>error fear is 29.739989900782476</t>
+  </si>
+  <si>
+    <t>error infected is 167.95065102186467</t>
+  </si>
+  <si>
+    <t>All behavior leads to no Inf Risk</t>
+  </si>
+  <si>
+    <t>Contacts/2</t>
+  </si>
+  <si>
+    <t>error behavior is 37.65369540817264</t>
+  </si>
+  <si>
+    <t>error fear is 35.45577318141028</t>
+  </si>
+  <si>
+    <t>error infected is 1884.744060387621</t>
+  </si>
+  <si>
+    <t>error behavior is 30.80015398195664</t>
+  </si>
+  <si>
+    <t>error fear is 28.058950945826588</t>
+  </si>
+  <si>
+    <t>error infected is 606.5801717568814</t>
+  </si>
+  <si>
+    <t>Risk*0.65, Behavior 70, If behavior Risk/10, 3days infection delay,max 40% increase and 10% daily decrease fear</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +417,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,9 +444,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2035,15 +2115,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>571405</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9430</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2066,7 +2146,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7124701" y="200026"/>
+          <a:off x="7172326" y="428626"/>
           <a:ext cx="5638704" cy="3752850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2428,6 +2508,480 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D73816A6-6B30-4A29-8672-FDDFECB98AE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5629275" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6802A5-FDA5-4410-9F6A-1C5AC71FFD25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5629275" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>134339</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7CAED8C-8F0B-4876-9B63-5CC2BC825FF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7900147" y="23834912"/>
+          <a:ext cx="6331324" cy="4112427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>60159</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>143400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E86207-F0A4-48FE-9238-3F7B2CA3A64C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7866529" y="28384500"/>
+          <a:ext cx="5506218" cy="3762900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88738</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>181505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A52B8AB-1600-494B-A67C-F69A07EEBF6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="34290000"/>
+          <a:ext cx="5534797" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>87609</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>170299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95469E4D-2571-499F-94B4-BF9A8DD67802}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6107205" y="34278794"/>
+          <a:ext cx="5477639" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>593003</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01C5F41-91AF-4A25-99F8-3F737A6CC3E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14421971" y="34290000"/>
+          <a:ext cx="5534797" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>250687</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>143400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC61CEF-C8AE-4E47-8207-6F4CD6BCC5CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14522824" y="38481000"/>
+          <a:ext cx="5696745" cy="3762900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>512855</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>171953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CDFFC53-D44D-4383-A94B-35B83C4D7B0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="38481000"/>
+          <a:ext cx="5353797" cy="3600953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>346341</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>57583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6FB0EBF-00A3-4276-B721-CB3BCDF33F1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14522824" y="42672000"/>
+          <a:ext cx="4582164" cy="3105583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2734,7 +3288,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
@@ -2784,12 +3338,12 @@
     <col min="82" max="82" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3046,12 +3600,12 @@
         <v>10024</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -3305,7 +3859,7 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -3313,7 +3867,7 @@
         <v>205.27437525948699</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3570,7 +4124,7 @@
         <v>9699.625</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -3578,7 +4132,7 @@
         <v>1599.18</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3835,7 +4389,7 @@
         <v>9201.25</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -3843,7 +4397,7 @@
         <v>1256.78</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4100,12 +4654,12 @@
         <v>7841</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -4362,12 +4916,12 @@
         <v>6833.5</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85">
       <c r="B16">
         <v>779.62</v>
       </c>
     </row>
-    <row r="18" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:113">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -4624,7 +5178,7 @@
         <v>93.5</v>
       </c>
     </row>
-    <row r="19" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:113">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -4632,7 +5186,7 @@
         <v>42.923092111405701</v>
       </c>
     </row>
-    <row r="20" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:113">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4973,7 +5527,7 @@
         <v>36.625</v>
       </c>
     </row>
-    <row r="21" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:113">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -4981,7 +5535,7 @@
         <v>46.31</v>
       </c>
     </row>
-    <row r="22" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:113">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -5322,12 +5876,12 @@
         <v>41.375</v>
       </c>
     </row>
-    <row r="23" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:113">
       <c r="B23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:113">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -5668,12 +6222,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:113">
       <c r="B25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:113">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -6014,7 +6568,7 @@
         <v>38.625</v>
       </c>
     </row>
-    <row r="27" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:113">
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -6022,17 +6576,17 @@
         <v>50.26</v>
       </c>
     </row>
-    <row r="28" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:113">
       <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:113">
       <c r="B29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:113">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -6373,7 +6927,7 @@
         <v>37.75</v>
       </c>
     </row>
-    <row r="31" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:113">
       <c r="B31" t="s">
         <v>4</v>
       </c>
@@ -6381,7 +6935,7 @@
         <v>16.84</v>
       </c>
     </row>
-    <row r="32" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:113">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -6722,7 +7276,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:113">
       <c r="B33" t="s">
         <v>4</v>
       </c>
@@ -6730,7 +7284,7 @@
         <v>17.95</v>
       </c>
     </row>
-    <row r="34" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:113">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -7071,7 +7625,7 @@
         <v>43.375</v>
       </c>
     </row>
-    <row r="35" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:113">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -7093,77 +7647,77 @@
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="M2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="M23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="13:13">
       <c r="M44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1">
       <c r="A111" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1">
       <c r="A131" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1">
       <c r="A152" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1">
       <c r="A172" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1">
       <c r="A174" t="s">
         <v>30</v>
       </c>
@@ -7182,12 +7736,12 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -7195,7 +7749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -7452,12 +8006,12 @@
         <v>21.125</v>
       </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85">
       <c r="B3">
         <v>44.052939072790302</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -7630,12 +8184,12 @@
         <v>45.375</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85">
       <c r="B5">
         <v>25.03</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -7808,7 +8362,7 @@
         <v>47.125</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -7981,12 +8535,12 @@
         <v>141.375</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85">
       <c r="B9">
         <v>33.729999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -8159,12 +8713,12 @@
         <v>113.25</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85">
       <c r="B11">
         <v>31.35</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -8337,12 +8891,12 @@
         <v>129.75</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85">
       <c r="B13">
         <v>22.41</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -8515,12 +9069,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85">
       <c r="B15">
         <v>9.17</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -8693,12 +9247,12 @@
         <v>108.625</v>
       </c>
     </row>
-    <row r="17" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:113">
       <c r="B17">
         <v>13.268000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:113">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -8871,12 +9425,12 @@
         <v>118.25</v>
       </c>
     </row>
-    <row r="19" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:113">
       <c r="B19">
         <v>23.65</v>
       </c>
     </row>
-    <row r="20" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:113">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -9049,12 +9603,12 @@
         <v>96.25</v>
       </c>
     </row>
-    <row r="21" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:113">
       <c r="B21">
         <v>56.04</v>
       </c>
     </row>
-    <row r="22" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:113">
       <c r="B22">
         <v>0</v>
       </c>
@@ -9224,12 +9778,12 @@
         <v>109.125</v>
       </c>
     </row>
-    <row r="23" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:113">
       <c r="B23">
         <v>17.079999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:113">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -9402,17 +9956,17 @@
         <v>98.625</v>
       </c>
     </row>
-    <row r="25" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:113">
       <c r="B25">
         <v>14.08</v>
       </c>
     </row>
-    <row r="26" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:113">
       <c r="A26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:113">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -9753,12 +10307,12 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="28" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:113">
       <c r="B28">
         <v>14.81</v>
       </c>
     </row>
-    <row r="29" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:113">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -10099,17 +10653,17 @@
         <v>87.25</v>
       </c>
     </row>
-    <row r="30" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:113">
       <c r="B30">
         <v>18.59</v>
       </c>
     </row>
-    <row r="31" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:113">
       <c r="A31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:113">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -10450,12 +11004,12 @@
         <v>69.125</v>
       </c>
     </row>
-    <row r="33" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:113">
       <c r="B33">
         <v>33.42</v>
       </c>
     </row>
-    <row r="34" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:113">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -10733,7 +11287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:113">
       <c r="B35">
         <v>78</v>
       </c>
@@ -10801,12 +11355,12 @@
         <v>69.625</v>
       </c>
     </row>
-    <row r="36" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:113">
       <c r="B36">
         <v>24.58</v>
       </c>
     </row>
-    <row r="37" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:113">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -11147,7 +11701,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:113">
       <c r="B38">
         <v>26.88</v>
       </c>
@@ -11165,9 +11719,9 @@
       <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -11175,82 +11729,82 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="L2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="L24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="L25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="L46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="L67" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12">
       <c r="L89" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1">
       <c r="A108" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1">
       <c r="A130" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1">
       <c r="A151" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1">
       <c r="A152" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1">
       <c r="A173" t="s">
         <v>42</v>
       </c>
@@ -11269,9 +11823,9 @@
       <selection activeCell="AY99" sqref="AY99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:127">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -11654,7 +12208,7 @@
         <v>34.375</v>
       </c>
     </row>
-    <row r="2" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:127">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -11662,12 +12216,12 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="3" spans="1:127" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:127">
       <c r="L3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:126">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -12011,12 +12565,12 @@
         <v>32.75</v>
       </c>
     </row>
-    <row r="25" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:126">
       <c r="L25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -12024,7 +12578,7 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -12032,7 +12586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:50">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -12046,12 +12600,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:50">
       <c r="K90">
         <v>32.840000000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:50">
       <c r="K91">
         <v>24.905000000000001</v>
       </c>
@@ -12065,7 +12619,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="92" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:50">
       <c r="W92" t="s">
         <v>62</v>
       </c>
@@ -12084,15 +12638,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
-  <dimension ref="A1:AG164"/>
+  <dimension ref="A1:AI227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="G197" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y224" sqref="Y224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -12103,7 +12657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="K2">
         <v>26.88</v>
       </c>
@@ -12114,7 +12668,7 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -12122,42 +12676,57 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="K47" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="K48" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21">
       <c r="A68" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21">
       <c r="K69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21">
       <c r="K70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21">
+      <c r="U77" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
+      <c r="U78" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21">
+      <c r="U79" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -12168,32 +12737,32 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14">
       <c r="N92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14">
       <c r="N95" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="14:14">
       <c r="N99" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="14:14">
       <c r="N103" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="14:14">
       <c r="N106" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -12204,7 +12773,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17">
       <c r="L115" t="s">
         <v>84</v>
       </c>
@@ -12212,7 +12781,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17">
       <c r="L116" t="s">
         <v>85</v>
       </c>
@@ -12220,29 +12789,123 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17">
       <c r="Q118" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17">
       <c r="Q119" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17">
+      <c r="Q120" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="N125" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
       <c r="A140" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="14:14">
+      <c r="N149" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
       <c r="A164" t="s">
         <v>81</v>
       </c>
     </row>
+    <row r="180" spans="1:34">
+      <c r="A180" t="s">
+        <v>102</v>
+      </c>
+      <c r="K180" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y180" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="181" spans="1:34">
+      <c r="U181" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH181" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="182" spans="1:34">
+      <c r="U182" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH182" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="183" spans="1:34">
+      <c r="U183" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH183" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="202" spans="11:25">
+      <c r="K202" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y202" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="203" spans="11:25">
+      <c r="U203" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="204" spans="11:25">
+      <c r="U204" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="205" spans="11:25">
+      <c r="U205" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="224" spans="25:25">
+      <c r="Y224" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="225" spans="35:35">
+      <c r="AI225" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="226" spans="35:35">
+      <c r="AI226" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="227" spans="35:35">
+      <c r="AI227" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reworked spatial setup for bigger maps
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D169FAA-B1D4-4EB3-A2AF-3D316B8F046E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB07CA0-49FB-4142-BD1A-2819A5A4B118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
+    <workbookView xWindow="7905" yWindow="4020" windowWidth="20895" windowHeight="11835" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="144">
   <si>
     <t>[0.0</t>
   </si>
@@ -398,6 +398,78 @@
   </si>
   <si>
     <t>Risk*0.65, Behavior 70, If behavior Risk/10, 3days infection delay,max 40% increase and 10% daily decrease fear</t>
+  </si>
+  <si>
+    <t>Risk 0.65, Behavior 60, same as above</t>
+  </si>
+  <si>
+    <t>error behavior is 33.64572317230976</t>
+  </si>
+  <si>
+    <t>error fear is 25.022909552258287</t>
+  </si>
+  <si>
+    <t>error infected is 531.6281490055067</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>PropertyGrowth 1.7, Scale 0-2</t>
+  </si>
+  <si>
+    <t>Above+Max Daily Fear Decay 0.7</t>
+  </si>
+  <si>
+    <t>PropertyGrowth 130,Scale 0-2</t>
+  </si>
+  <si>
+    <t>PropertyGrowth 1.7, Scale 0-3</t>
+  </si>
+  <si>
+    <t>error behavior is 30.157608135128488</t>
+  </si>
+  <si>
+    <t>error fear is 26.07005412058058</t>
+  </si>
+  <si>
+    <t>error infected is 1574.846266257025</t>
+  </si>
+  <si>
+    <t>Growth 170, 0-3, daily cases/210</t>
+  </si>
+  <si>
+    <t>error behavior is 26.596096128049485</t>
+  </si>
+  <si>
+    <t>error fear is 27.301443645729965</t>
+  </si>
+  <si>
+    <t>error infected is 124.88224306693621</t>
+  </si>
+  <si>
+    <t>attitude difference/3</t>
+  </si>
+  <si>
+    <t>attitude difference/1</t>
+  </si>
+  <si>
+    <t>error behavior is 29.572680679411462</t>
+  </si>
+  <si>
+    <t>error fear is 28.81874756587898</t>
+  </si>
+  <si>
+    <t>error infected is 299.2557105102875</t>
+  </si>
+  <si>
+    <t>norm time/200</t>
+  </si>
+  <si>
+    <t>/2 that since best fit for all</t>
+  </si>
+  <si>
+    <t>Norm time/350</t>
   </si>
 </sst>
 </file>
@@ -2510,128 +2582,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D73816A6-6B30-4A29-8672-FDDFECB98AE3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="5629275" cy="3619500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6802A5-FDA5-4410-9F6A-1C5AC71FFD25}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="5629275" cy="3619500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>33618</xdr:colOff>
       <xdr:row>125</xdr:row>
@@ -2657,7 +2607,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2701,7 +2651,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2745,7 +2695,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2789,7 +2739,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2833,7 +2783,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2877,7 +2827,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2921,7 +2871,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2941,22 +2891,66 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>192401</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>89051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC13A795-8FA1-451B-AD2B-7A16D9B06F79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14578854" y="42817677"/>
+          <a:ext cx="5582429" cy="3753374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>224</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>346341</xdr:colOff>
-      <xdr:row>240</xdr:row>
-      <xdr:rowOff>57583</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>317371</xdr:colOff>
+      <xdr:row>266</xdr:row>
+      <xdr:rowOff>29111</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
+        <xdr:cNvPr id="24" name="Picture 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6FB0EBF-00A3-4276-B721-CB3BCDF33F1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97A66997-57FA-4ADC-B502-FAC37716733F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2972,8 +2966,404 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14522824" y="42672000"/>
-          <a:ext cx="4582164" cy="3105583"/>
+          <a:off x="14522824" y="46863000"/>
+          <a:ext cx="5763429" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>422160</xdr:colOff>
+      <xdr:row>247</xdr:row>
+      <xdr:rowOff>22970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62EF7838-0E1B-46D8-9597-82BFF3E2336C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="43075412"/>
+          <a:ext cx="5868219" cy="4001058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>249</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>412634</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>114821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{702B1FAC-7E0F-49D3-86F3-FA63801C85B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="47434500"/>
+          <a:ext cx="5858693" cy="3734321"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>275328</xdr:colOff>
+      <xdr:row>269</xdr:row>
+      <xdr:rowOff>184864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC522214-CCE4-4797-A72A-3E5933BA21F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6152029" y="47647411"/>
+          <a:ext cx="5620534" cy="3781953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>260212</xdr:colOff>
+      <xdr:row>245</xdr:row>
+      <xdr:rowOff>124347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFB680C-9D23-4780-88CE-E6BC959D2577}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="43053000"/>
+          <a:ext cx="5706271" cy="3743847"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>272</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>126844</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>162453</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CA94AD0-9FEC-4C55-B0E1-0F5D7B90869F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="51816000"/>
+          <a:ext cx="5572903" cy="3781953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>294</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>299997</xdr:colOff>
+      <xdr:row>314</xdr:row>
+      <xdr:rowOff>97475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85A0766A-DDA8-4D09-9E04-62331F999E7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6062382" y="56018206"/>
+          <a:ext cx="5734850" cy="3896269"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>593913</xdr:colOff>
+      <xdr:row>294</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>325219</xdr:colOff>
+      <xdr:row>314</xdr:row>
+      <xdr:rowOff>158542</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E1EDD6-E697-4E2F-A119-6D392291A1BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14511619" y="56107852"/>
+          <a:ext cx="5782482" cy="3867690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>317</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>126844</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C801C7-F639-4FC2-A70E-0A9676472E80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="60388500"/>
+          <a:ext cx="5572903" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>339</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>241160</xdr:colOff>
+      <xdr:row>359</xdr:row>
+      <xdr:rowOff>19584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAC3044D-1747-4F45-B230-4655A3B24298}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="64579500"/>
+          <a:ext cx="5687219" cy="3829584"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12638,10 +13028,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
-  <dimension ref="A1:AI227"/>
+  <dimension ref="A1:AI339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G197" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y224" sqref="Y224"/>
+    <sheetView tabSelected="1" topLeftCell="I317" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K340" sqref="K340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12887,19 +13277,125 @@
         <v>119</v>
       </c>
     </row>
-    <row r="225" spans="35:35">
+    <row r="225" spans="1:35">
+      <c r="A225" t="s">
+        <v>124</v>
+      </c>
       <c r="AI225" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="226" spans="35:35">
+    <row r="226" spans="1:35">
+      <c r="A226" t="s">
+        <v>125</v>
+      </c>
+      <c r="L226" t="s">
+        <v>128</v>
+      </c>
       <c r="AI226" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="227" spans="35:35">
+    <row r="227" spans="1:35">
+      <c r="V227" t="s">
+        <v>129</v>
+      </c>
       <c r="AI227" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="228" spans="1:35">
+      <c r="V228" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="229" spans="1:35">
+      <c r="V229" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="246" spans="1:35">
+      <c r="Y246" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="247" spans="1:35">
+      <c r="AI247" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="248" spans="1:35">
+      <c r="AI248" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="249" spans="1:35">
+      <c r="A249" t="s">
+        <v>126</v>
+      </c>
+      <c r="K249" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI249" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="272" spans="11:11">
+      <c r="K272" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="273" spans="21:21">
+      <c r="U273" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="274" spans="21:21">
+      <c r="U274" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="275" spans="21:21">
+      <c r="U275" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="294" spans="11:25">
+      <c r="K294" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y294" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="295" spans="11:25">
+      <c r="U295" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="296" spans="11:25">
+      <c r="U296" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="297" spans="11:25">
+      <c r="U297" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="302" spans="11:25">
+      <c r="U302" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="317" spans="11:11">
+      <c r="K317" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="339" spans="11:11">
+      <c r="K339" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thats it. I hereby pronounce you happily calibrated ever after.
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB07CA0-49FB-4142-BD1A-2819A5A4B118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503DC244-1AB3-4686-89D1-BE3CFAED9D1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="4020" windowWidth="20895" windowHeight="11835" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="179">
   <si>
     <t>[0.0</t>
   </si>
@@ -470,6 +470,111 @@
   </si>
   <si>
     <t>Norm time/350</t>
+  </si>
+  <si>
+    <t>Infection Risk - General</t>
+  </si>
+  <si>
+    <t>Quarantine (Behavior)</t>
+  </si>
+  <si>
+    <t>Quarantine (No Behavior)</t>
+  </si>
+  <si>
+    <t>General (No PB)</t>
+  </si>
+  <si>
+    <t>General (PB)</t>
+  </si>
+  <si>
+    <t>Travel (PB)</t>
+  </si>
+  <si>
+    <t>Travel (No PB)</t>
+  </si>
+  <si>
+    <t>Fear Growth</t>
+  </si>
+  <si>
+    <t>Fear Decay</t>
+  </si>
+  <si>
+    <t>Fear Decay Trigger</t>
+  </si>
+  <si>
+    <t>Fear Decay Delay</t>
+  </si>
+  <si>
+    <t>PB Activation Threshold</t>
+  </si>
+  <si>
+    <t>Fear Influence on PB</t>
+  </si>
+  <si>
+    <t>Attitude/Norms Growth</t>
+  </si>
+  <si>
+    <t>Attitude Decay</t>
+  </si>
+  <si>
+    <t>Norm Decay</t>
+  </si>
+  <si>
+    <t>Calibrated Value</t>
+  </si>
+  <si>
+    <t>Risk*0.65</t>
+  </si>
+  <si>
+    <t>100*1.3*(1-e^(-case_growth*personal_cases))</t>
+  </si>
+  <si>
+    <t>fear-0.5</t>
+  </si>
+  <si>
+    <t>If 3 days growth &lt; 105%</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>PB  &gt; 65</t>
+  </si>
+  <si>
+    <t>Fear*1.1</t>
+  </si>
+  <si>
+    <t>norm*e^(-(time/340))</t>
+  </si>
+  <si>
+    <t>property*(1+e^(-property_factor), Scale Property (0,170)-&gt;(0,3)</t>
+  </si>
+  <si>
+    <t>unscaled_attitude*(e^(-difference/2)), Scale Attitude (0,158) -&gt; (0,2)</t>
+  </si>
+  <si>
+    <t>error behavior is 27.98637926543676</t>
+  </si>
+  <si>
+    <t>error fear is 33.26911856094239</t>
+  </si>
+  <si>
+    <t>error infected is 186.33064324083537</t>
+  </si>
+  <si>
+    <t>Final Params</t>
+  </si>
+  <si>
+    <t>error behavior is 26.638244210553736</t>
+  </si>
+  <si>
+    <t>error fear is 31.825906272342596</t>
+  </si>
+  <si>
+    <t>error infected is 146.9276651225957</t>
+  </si>
+  <si>
+    <t>Risk 0.64 Behavior 60</t>
   </si>
 </sst>
 </file>
@@ -3372,6 +3477,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>399171</xdr:colOff>
+      <xdr:row>380</xdr:row>
+      <xdr:rowOff>101385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5996C0B9-A055-45BB-82A2-153E143D31F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6152029" y="68680853"/>
+          <a:ext cx="5744377" cy="3810532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>382</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>193528</xdr:colOff>
+      <xdr:row>402</xdr:row>
+      <xdr:rowOff>114848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90F08B43-DFDE-441E-A107-BDE2C2409776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="72771000"/>
+          <a:ext cx="5639587" cy="3924848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13028,10 +13221,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
-  <dimension ref="A1:AI339"/>
+  <dimension ref="A1:AI384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I317" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K340" sqref="K340"/>
+    <sheetView tabSelected="1" topLeftCell="F358" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB371" sqref="AB371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13393,9 +13586,180 @@
         <v>141</v>
       </c>
     </row>
-    <row r="339" spans="11:11">
+    <row r="322" spans="26:27">
+      <c r="AA322" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="323" spans="26:27">
+      <c r="Z323" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA323" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="324" spans="26:27">
+      <c r="Z324" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA324">
+        <v>1.6299999999999999E-3</v>
+      </c>
+    </row>
+    <row r="325" spans="26:27">
+      <c r="Z325" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA325">
+        <v>1.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="326" spans="26:27">
+      <c r="Z326" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA326">
+        <v>3.6600000000000001E-3</v>
+      </c>
+    </row>
+    <row r="327" spans="26:27">
+      <c r="Z327" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA327">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="328" spans="26:27">
+      <c r="Z328" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA328">
+        <v>0.36599999999999999</v>
+      </c>
+    </row>
+    <row r="329" spans="26:27">
+      <c r="Z329" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA329">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="330" spans="26:27">
+      <c r="Z330" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA330" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="331" spans="26:27">
+      <c r="Z331" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA331" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="332" spans="26:27">
+      <c r="Z332" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA332" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="333" spans="26:27">
+      <c r="Z333" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA333" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="334" spans="26:27">
+      <c r="Z334" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA334" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="335" spans="26:27">
+      <c r="Z335" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA335" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="336" spans="26:27">
+      <c r="Z336" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA336" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="337" spans="11:27">
+      <c r="Z337" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA337" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="338" spans="11:27">
+      <c r="Z338" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA338" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="339" spans="11:27">
       <c r="K339" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="360" spans="11:21">
+      <c r="K360" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="361" spans="11:21">
+      <c r="U361" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="362" spans="11:21">
+      <c r="U362" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="363" spans="11:21">
+      <c r="U363" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="382" spans="11:21">
+      <c r="K382" t="s">
+        <v>178</v>
+      </c>
+      <c r="U382" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="383" spans="11:21">
+      <c r="U383" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="384" spans="11:21">
+      <c r="U384" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First tests for goodness of fit
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503DC244-1AB3-4686-89D1-BE3CFAED9D1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB562D4-CE6A-451B-8FB2-17788DBA0281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Graphics2" sheetId="4" r:id="rId4"/>
     <sheet name="Calib2" sheetId="5" r:id="rId5"/>
     <sheet name="Conclusion" sheetId="6" r:id="rId6"/>
+    <sheet name="ChiSqu Test" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="214">
   <si>
     <t>[0.0</t>
   </si>
@@ -575,6 +576,111 @@
   </si>
   <si>
     <t>Risk 0.64 Behavior 60</t>
+  </si>
+  <si>
+    <t>Behavior:</t>
+  </si>
+  <si>
+    <t>Pearson's Chi-square Test</t>
+  </si>
+  <si>
+    <t>-------------------------</t>
+  </si>
+  <si>
+    <t>Population details:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    parameter of interest:   Multinomial Probabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    value under h_0:         [6.421521222854386e-5, 6.421521222854386e-5, 6.421521222854386e-5, 6.421521222854386e-5, 6.421521222854386e-5, 6.421521222854386e-5, 6.421521222854386e-5, 6.421521222854386e-5, 0.0001284304244570877, 0.0001284304244570877  …  0.004918748628595335, 0.004852279052533236, 0.004852279052533236, 0.004719339900409038, 0.0045864007482848395, 0.004320522444036443, 0.004719339900409038, 0.004453461596160641, 0.004320522444036443, 0.004187583291912244]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0  …  0.004704652378463147, 0.004573967590172504, 0.004443282801881861, 0.004181913225300575, 0.004181913225300575, 0.004051228437009932, 0.004312598013591218, 0.004051228437009932, 0.003920543648719289, 0.003789858860428646]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    95% confidence interval: [(0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035), (0.0, 0.0035)  …  (0.0014, 0.0082), (0.0013, 0.0081), (0.0012, 0.0079), (0.0009, 0.0077), (0.0009, 0.0077), (0.0008, 0.0075), (0.001, 0.0078), (0.0008, 0.0075), (0.0007, 0.0074), (0.0005, 0.0073)]</t>
+  </si>
+  <si>
+    <t>Test summary:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    outcome with 95% confidence: fail to reject h_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    one-sided p-value:           0.6788</t>
+  </si>
+  <si>
+    <t>Details:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sample size:        7652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    statistic:          103.58420489431465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    degrees of freedom: 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    residuals:          [-0.700981314995498, -0.700981314995498, -0.700981314995498, -0.700981314995498, -0.700981314995498, -0.700981314995498, -0.700981314995498, -0.700981314995498, -0.9913372826367599, -0.9913372826367599  …  -0.26703563915741074, -0.3494988004158997, -0.5136105346318093, -0.6843307743603704, -0.5224642881172417, -0.35838187431853474, -0.5179236596595457, -0.5272498863899506, -0.5322998158637798, -0.5376356037764811]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std. residuals:     [-0.9829600930135668, -0.9829600930135668, -0.9829600930135668, -0.9829600930135668, -0.9829600930135668, -0.9829600930135668, -0.9829600930135668, -0.9829600930135668, -1.390206349064192, -1.390206349064192  …  -0.3828009135467793, -0.5009804457298044, -0.7362223683319435, -0.9808076876735916, -0.7487160127553111, -0.5134427588599031, -0.7423069750106223, -0.7554743804066804, -0.76260967862119, -0.770152596083419]</t>
+  </si>
+  <si>
+    <t>Infections:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    value under h_0:         [3.640666076181563e-7, 3.640666076181563e-7, 3.640666076181563e-7, 3.640666076181563e-7, 7.281332152363126e-7, 7.281332152363126e-7, 1.0921998228544687e-6, 1.4562664304726252e-6, 2.5484662533270938e-6, 3.276599468563407e-6  …  0.009451621104509535, 0.009492782425392973, 0.009517705794001291, 0.009550181698551525, 0.009600028435768165, 0.009634770101100974, 0.00967139990041926, 0.009706519192549166, 0.009742771365070358, 0.009766939480084485]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          [0.0, 0.0, 0.0, 0.0, 7.416934047139066e-7, 7.416934047139066e-7, 1.4833868094278132e-6, 2.2250802141417197e-6, 4.4501604282834395e-6, 5.933547237711253e-6  …  0.008850627398451048, 0.008869169733568895, 0.008886228681877315, 0.008923313352113011, 0.008959656328943992, 0.008973748503633555, 0.008990065758537263, 0.009000449466203257, 0.009017508414511677, 0.009036792443034238]       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    95% confidence interval: [(0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003), (0.0, 0.0003)  …  (0.0086, 0.0091), (0.0086, 0.0091), (0.0086, 0.0092), (0.0086, 0.0092), (0.0087, 0.0092), (0.0087, 0.0092), (0.0087, 0.0093), (0.0087, 0.0093), (0.0087, 0.0093), (0.0088, 0.0093)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    outcome with 95% confidence: reject h_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    one-sided p-value:           &lt;1e-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sample size:        1348266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    statistic:          12450.040075537145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    residuals:          [-0.7006130378367942, -0.7006130378367942, -0.7006130378367942, -0.7006130378367942, 0.01845219893162042, 0.01845219893162042, 0.43463144066936726, 0.7397560628138501, 1.3832128793766483, 1.7043513549117302  …  -7.178018339048342, -7.43200466062883, -7.515870137840213, -7.4483197969364054, -7.588989264092661, -7.819568035233294, -8.044578110816033, -8.321538437726877, -8.531826758067197, -8.57864843596887]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std. residuals:     [-0.9818817365979624, -0.9818817365979624, -0.9818817365979624, -0.9818817365979624, 0.025860043806685117, 0.025860043806685117, 0.6091193957585496, 1.0367403066833776, 1.9385229973577338, 2.3885887681131504  …  -10.34178064851564, -10.708154280755146, -10.829259131439072, -10.732277872808288, -10.935513951750513, -11.26816313045955, -11.59283248468878, -11.992374433289937, -12.29587238661733, -12.363649880902676]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    value under h_0:         [6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5, 6.685618918059582e-5  …  0.004943664884343022, 0.004860810165611016, 0.004971283123920358, 0.004916046644765687, 0.00466748248856967, 0.004446536571950987, 0.004916046644765687, 0.004750337207301675, 0.004584627769837664, 0.004612246009414999]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          [6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5, 6.104633416763323e-5  …  0.004517428728404859, 0.004395336060069593, 0.004395336060069593, 0.004273243391734327, 0.004273243391734327, 0.004273243391734327, 0.004273243391734327, 0.004273243391734327, 0.0041511507233990596, 0.0041511507233990596]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    95% confidence interval: [(0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024), (0.0, 0.0024)  …  (0.0023, 0.0068), (0.0022, 0.0067), (0.0022, 0.0067), (0.0021, 0.0066), (0.0021, 0.0066), (0.0021, 0.0066), (0.0021, 0.0066), (0.0021, 0.0066), (0.002, 0.0065), (0.002, 0.0065)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    one-sided p-value:           &lt;1e-42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sample size:        16381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    statistic:          453.15951632877704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    residuals:          [-0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718, -0.09094203971925718  …  -0.7758825416407858, -0.8544986894977437, -1.0454867301497144, -1.1733843016355048, -0.7385647020940129, -0.3326141666249464, -1.1733843016355048, -0.885955222093754, -0.8193779458056663, -0.8689697443724833]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std. residuals:     [-0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453  …  -1.0542797251221054, -1.1609969320602966, -1.4206653975462857, -1.5943613082456878, -1.0032621755625761, -0.45170979342082757, -1.5943613082456878, -1.2035880025708865, -1.112935466936198, -1.1803308545384814]</t>
   </si>
 </sst>
 </file>
@@ -13223,7 +13329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
   <dimension ref="A1:AI384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F358" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F358" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB371" sqref="AB371"/>
     </sheetView>
   </sheetViews>
@@ -13766,6 +13872,276 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7E5F9E-BF0B-42B4-91DE-C6002CD98041}">
+  <dimension ref="A1:A59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Saving and loading workspace works now
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB562D4-CE6A-451B-8FB2-17788DBA0281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219C83B2-22FF-4D40-9153-E6FAA43044EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
@@ -19,7 +19,8 @@
     <sheet name="Graphics2" sheetId="4" r:id="rId4"/>
     <sheet name="Calib2" sheetId="5" r:id="rId5"/>
     <sheet name="Conclusion" sheetId="6" r:id="rId6"/>
-    <sheet name="ChiSqu Test" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId7"/>
+    <sheet name="ChiSqu Test" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="245">
   <si>
     <t>[0.0</t>
   </si>
@@ -681,6 +682,99 @@
   </si>
   <si>
     <t xml:space="preserve">    std. residuals:     [-0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453, -0.13521441791672453  …  -1.0542797251221054, -1.1609969320602966, -1.4206653975462857, -1.5943613082456878, -1.0032621755625761, -0.45170979342082757, -1.5943613082456878, -1.2035880025708865, -1.112935466936198, -1.1803308545384814]</t>
+  </si>
+  <si>
+    <t>All Runs in Average</t>
+  </si>
+  <si>
+    <t>Run1</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>Infected</t>
+  </si>
+  <si>
+    <t>Run2</t>
+  </si>
+  <si>
+    <t>Run3</t>
+  </si>
+  <si>
+    <t>Run4</t>
+  </si>
+  <si>
+    <t>Run5</t>
+  </si>
+  <si>
+    <t>Run6</t>
+  </si>
+  <si>
+    <t>Run7</t>
+  </si>
+  <si>
+    <t>Run8</t>
+  </si>
+  <si>
+    <t>Run9</t>
+  </si>
+  <si>
+    <t>Run10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.125; 0.125; 0.125; 0.625; 0.875; 1.0; 1.125; 1.75; 1.875; 2.125; 3.25; 4.25; 6.125; 8.375; 11.75; 15.375; 21.0; 28.375; 37.0; 46.375; 56.375; 67.625; 69.0; </t>
+  </si>
+  <si>
+    <t>75.25; 87.875; 92.625; 95.125; 103.125; 107.5; 100.625; 100.25; 111.75; 116.125; 117.0; 117.125; 118.25; 110.375; 107.75; 118.75; 124.5; 125.25; 124.0; 118.625; 109.125; 104.5; 125.125; 127.625; 127.375; 124.5; 116.75; 107.375; 104.5; 127.0; 128.25; 127.875; 125.75; 118.875; 109.5; 106.375; 127.25; 128.125; 128.0; 125.625; 119.875; 110.25; 110.125; 129.625; 129.75; 129.625; 127.75; 124.125; 114.125; 106.125; 128.25; 128.5; 127.625; 125.0; 120.125; 110.5; 103.125; 124.625; 121.25; 117.625; 115.75; 112.375; 103.5; 95.875; 108.75; 104.375; 100.75; 99.75; 99.25; 91.5; 84.875; 94.125; 89.625; 91.5; 95.125; 96.75; 89.375; 82.75; 94.75; 89.875; 85.125; 83.375</t>
+  </si>
+  <si>
+    <t>16 steps, 50 its run</t>
+  </si>
+  <si>
+    <t>error behavior is 38.69552760785954</t>
+  </si>
+  <si>
+    <t>behavior data is [0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.02; 0.04; 0.06; 0.12; 0.18; 0.3; 0.52; 0.76; 1.12; 1.58; 2.14; 2.66; 3.3200000000000003; 4.5200000000000005; 5.9; 7.2; 8.78; 10.82; 11.56; 12.620000000000001; 15.700000000000001; 18.2; 20.34; 22.84; 26.2; 26.32; 27.080000000000002; 31.62; 34.84; 37.04; 39.18; 41.68; 40.2; 39.660000000000004; 44.56; 47.52; 49.58; 50.52; 50.9; 47.84; 45.84; 50.84; 54.06; 55.72; 55.74; 54.86; 51.1; 48.26; 53.34; 56.54; 57.82; 57.72; 56.34; 52.14; 49.96; 56.480000000000004; 58.88; 59.86; 59.300000000000004; 58.38; 54.0; 51.08; 55.7; 57.800000000000004; 58.14; 57.620000000000005; 56.02; 51.82; 48.42; 53.42; 55.14; 54.980000000000004; 53.68; 51.68; 47.86; 44.300000000000004; 48.4; 48.54; 47.06; 45.58; 44.14; 40.94; 38.04; 40.94; 40.04; 39.26; 39.78; 40.7; 37.9; 35.32; 39.08; 38.06; 36.42; 35.64]</t>
+  </si>
+  <si>
+    <t>error fear is 37.31021987628112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fear data is [0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.04; 0.04; 0.06; 0.16; 0.2; 0.2; 0.38; 0.68; 0.9; 1.24; 1.8; 2.12; 2.68; 3.64; 4.94; 6.36; 8.38; 11.0; 12.52; 15.040000000000001; 19.7; 23.86; 28.0; 32.62; 37.72; 37.56; 40.92; 50.82; 55.56; 60.56; 65.9; 72.54; 69.38; 71.78; 83.92; 87.5; 91.24; 94.64; 98.84; 93.04; 93.86; 106.22; 108.96000000000001; 111.34; 112.3; 112.62; 105.10000000000001; </t>
+  </si>
+  <si>
+    <t>104.14; 117.88; 120.78; 121.74000000000001; 121.22; 119.66; 110.76; 108.66; 123.66; 125.94; 126.44; 125.58; 123.06; 113.76; 114.26; 129.74; 129.88; 129.9; 129.08; 127.62; 118.22; 115.66; 129.18; 129.9; 129.74; 128.4; 125.86; 116.42; 111.12; 128.34; 128.3; 126.68; 124.60000000000001; 121.38; 111.76; 104.78; 122.52; 119.48; 116.06; 114.16; 112.16; 103.26; 96.28; 111.60000000000001; 107.06; 105.8; 108.66; 110.4; 101.66; 94.02; 110.44; 104.74000000000001; 100.92; 100.72]</t>
+  </si>
+  <si>
+    <t>error infected is 276.59482817646125</t>
+  </si>
+  <si>
+    <t>infected data is [0.0; 1.0; 2.0; 2.0; 2.0; 6.0; 6.0; 6.0; 11.0; 17.0; 19.0; 24.0; 31.0; 44.0; 52.0; 69.0; 91.0; 124.0; 156.0; 196.0; 215.0; 252.0; 312.0; 374.0; 443.0; 510.0; 587.0; 640.0; 710.0; 816.0; 936.0; 1045.0; 1186.0; 1333.0; 1446.0; 1543.0; 1727.0; 1908.0; 2071.0; 2246.0; 2464.0; 2615.0; 2784.0; 3018.0; 3250.0; 3508.0; 3746.0; 3956.0; 4107.0; 4253.0; 4497.0; 4748.0; 5007.0; 5217.0; 5397.0; 5511.0; 5631.0; 5890.0; 6149.0; 6406.0; 6629.0; 6774.0; 6858.0; 6958.0; 7208.0; 7494.0; 7764.0; 7970.0; 8120.0; 8198.0; 8315.0; 8696.0; 9125.0; 9455.0; 9713.0; 9907.0; 9989.0; 10067.0; 10295.0; 10652.0; 10963.0; 11171.0; 11313.0; 11373.0; 11424.0; 11634.0; 11834.0; 12002.0; 12127.0; 12239.0; 12286.0; 12343.0; 12468.0; 12583.0; 12669.0; 12766.0; 12845.0; 12900.0; 12948.0; 13044.0; 13112.0; 13180.0; 13255.0; 13351.0; 13394.0; 13435.0; 13523.0; 13592.0; 13654.0; 13709.0; 13771.0; 13802.0]</t>
+  </si>
+  <si>
+    <t>1768.226422 seconds (20.05 M allocations: 1.245 GiB, 0.02% gc time)</t>
+  </si>
+  <si>
+    <t>16 steps 16 run</t>
+  </si>
+  <si>
+    <t>error behavior is 26.39305200153952</t>
+  </si>
+  <si>
+    <t>behavior data is [0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0625; 0.125; 0.3125; 0.5625; 0.9375; 1.3125; 1.9375; 2.6875; 3.75; 5.3125; 7.125; 9.125; 10.8125; 14.375; 17.875; 20.8125; 24.1875; 28.4375; 29.0625; 30.0; 35.25; 39.25; 41.8125; 44.8125; 47.1875; 45.5; 44.4375; 49.875; 53.3125; 55.5625; 56.5625; 56.625; 53.125; 50.25; 54.6875; 58.375; 60.1875; 59.6875; 57.5625; 53.0625; 49.75; 55.5; 59.0625; 60.4375; 59.625; 56.6875; 52.3125; 48.75; 55.125; 58.25; 59.125; 58.75; 56.1875; 51.75; 49.1875; 56.0625; 59.0; 59.75; 59.0; 57.625; 53.25; 49.4375; 54.75; 57.1875; 57.5; 56.5625; 53.9375; 49.875; 46.125; 51.875; 53.375; 52.0; 50.5; 48.3125; 44.8125; 41.5; 44.8125; 43.75; 41.625; 40.4375; 39.375; 36.8125; 34.25; 36.125; 35.125; 34.6875; 34.5; 35.6875; 33.6875; 31.4375; 34.0625; 33.125; 31.5625; 30.5625]</t>
+  </si>
+  <si>
+    <t>error fear is 27.977829646686406</t>
+  </si>
+  <si>
+    <t>fear data is [0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0; 0.0625; 0.1875; 0.3125; 0.4375; 0.75; 0.75; 0.9375; 1.5; 1.9375; 2.4375; 3.4375; 4.4375; 5.625; 7.5625; 10.6875; 14.25; 18.875; 24.8125; 31.9375; 36.5; 41.4375; 52.125; 59.25; 65.8125; 72.625; 80.25; 76.875; 78.9375; 93.0; 97.8125; 100.75; 105.5; 108.25; 101.8125; 101.125; 114.9375; 117.4375; 119.4375; 120.125; 119.6875; 110.9375; 108.0625; 121.5625; 125.3125; 126.1875; 124.1875; 120.625; 111.0; 107.6875; 125.25; 127.75; 127.875; 125.8125; 120.5; 110.8125; 108.1875; 127.0; 128.1875; 128.0; 126.5625; 121.75; 112.3125; 112.1875; 130.0; 129.9375; 129.9375; 128.6875; 126.5; 116.1875; 110.5; 128.5; 129.4375; 128.8125; 126.75; 122.375; 112.5625; 105.125; 126.6875; 125.75; 122.0; 119.875; 116.75; 107.5625; 99.625; 116.6875; 111.375; 107.3125; 106.1875; 104.8125; 96.625; 89.4375; 103.125; 99.0625; 98.1875; 99.0; 102.5625; 94.5625; 87.4375; 100.75; 96.5; 91.75; 90.625]</t>
+  </si>
+  <si>
+    <t>error infected is 253.18278771202952</t>
+  </si>
+  <si>
+    <t>infected data is [0.0; 0.0; 1.0; 2.0; 4.0; 6.0; 6.0; 9.0; 12.0; 13.0; 16.0; 20.0; 29.0; 32.0; 42.0; 62.0; 91.0; 116.0; 147.0; 181.0; 209.0; 252.0; 304.0; 347.0; 396.0; 457.0; 572.0; 642.0; 708.0; 811.0; 919.0; 1050.0; 1173.0; 1320.0; 1441.0; 1559.0; 1725.0; 1886.0; 2062.0; 2259.0; 2479.0; 2629.0; 2786.0; 3025.0; 3259.0; 3478.0; 3720.0; 3983.0; 4146.0; 4319.0; 4542.0; 4794.0; 5045.0; 5270.0; 5474.0; 5596.0; 5698.0; 5888.0; 6159.0; 6399.0; 6638.0; 6786.0; 6883.0; 6974.0; 7234.0; 7509.0; 7781.0; 8021.0; 8196.0; 8284.0; 8386.0; 8731.0; 9181.0; 9539.0; 9788.0; 9981.0; 10064.0; 10166.0; 10419.0; 10786.0; 11060.0; 11264.0; 11392.0; 11456.0; 11520.0; 11738.0; 11923.0; 12055.0; 12177.0; 12289.0; 12356.0; 12401.0; 12515.0; 12605.0; 12695.0; 12784.0; 12855.0; 12900.0; 12953.0; 13059.0; 13107.0; 13182.0; 13245.0; 13319.0; 13365.0; 13402.0; 13471.0; 13537.0; 13582.0; 13643.0; 13700.0; 13731.0]</t>
   </si>
 </sst>
 </file>
@@ -13327,10 +13421,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
-  <dimension ref="A1:AI384"/>
+  <dimension ref="A1:AI412"/>
   <sheetViews>
-    <sheetView topLeftCell="F358" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB371" sqref="AB371"/>
+    <sheetView topLeftCell="I370" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB385" sqref="AB385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13850,22 +13944,218 @@
         <v>173</v>
       </c>
     </row>
-    <row r="382" spans="11:21">
+    <row r="381" spans="11:29">
+      <c r="AA381" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="382" spans="11:29">
       <c r="K382" t="s">
         <v>178</v>
       </c>
       <c r="U382" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="383" spans="11:21">
+      <c r="AB382" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="11:29">
       <c r="U383" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="384" spans="11:21">
+      <c r="Z383" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA383" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB383">
+        <v>27.1400097067907</v>
+      </c>
+      <c r="AC383" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="384" spans="11:29">
       <c r="U384" t="s">
         <v>177</v>
+      </c>
+      <c r="AA384" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB384">
+        <v>38.94</v>
+      </c>
+      <c r="AC384" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="385" spans="26:27">
+      <c r="AA385" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="386" spans="26:27">
+      <c r="Z386" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA386" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="387" spans="26:27">
+      <c r="AA387" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="388" spans="26:27">
+      <c r="AA388" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="389" spans="26:27">
+      <c r="Z389" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA389" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="390" spans="26:27">
+      <c r="AA390" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="391" spans="26:27">
+      <c r="AA391" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="392" spans="26:27">
+      <c r="Z392" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA392" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="393" spans="26:27">
+      <c r="AA393" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="394" spans="26:27">
+      <c r="AA394" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="395" spans="26:27">
+      <c r="Z395" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA395" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="396" spans="26:27">
+      <c r="AA396" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="397" spans="26:27">
+      <c r="AA397" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="398" spans="26:27">
+      <c r="Z398" t="s">
+        <v>222</v>
+      </c>
+      <c r="AA398" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="399" spans="26:27">
+      <c r="AA399" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="400" spans="26:27">
+      <c r="AA400" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="401" spans="26:27">
+      <c r="Z401" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA401" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="402" spans="26:27">
+      <c r="AA402" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="403" spans="26:27">
+      <c r="AA403" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="404" spans="26:27">
+      <c r="Z404" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA404" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="405" spans="26:27">
+      <c r="AA405" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="406" spans="26:27">
+      <c r="AA406" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="407" spans="26:27">
+      <c r="Z407" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA407" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="408" spans="26:27">
+      <c r="AA408" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="409" spans="26:27">
+      <c r="AA409" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="410" spans="26:27">
+      <c r="Z410" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA410" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="411" spans="26:27">
+      <c r="AA411" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="412" spans="26:27">
+      <c r="AA412" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -13876,11 +14166,106 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61788BDA-4C45-44A2-BFF7-0EB5F25B5DC0}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7E5F9E-BF0B-42B4-91DE-C6002CD98041}">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Big model for LK Rostock
</commit_message>
<xml_diff>
--- a/ExcelCharts/calibration.xlsx
+++ b/ExcelCharts/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\github\julia\ExcelCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FC8F4D-D019-47C5-BF4F-C1BE511D8E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506A2A6B-F7EB-4FC5-9A13-E9EEA388D3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="7" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
+    <workbookView xWindow="2055" yWindow="1965" windowWidth="21600" windowHeight="11835" firstSheet="6" activeTab="9" xr2:uid="{D0E74750-6A6F-4651-8F75-8F1C67891960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Hyp3" sheetId="9" r:id="rId7"/>
     <sheet name="Hyp4" sheetId="10" r:id="rId8"/>
     <sheet name="Hyp5" sheetId="11" r:id="rId9"/>
+    <sheet name="Sens_Contact_Rate" sheetId="12" r:id="rId10"/>
+    <sheet name="Sens_Inf_Risk" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="482">
   <si>
     <t>[0.0</t>
   </si>
@@ -1076,6 +1078,417 @@
   </si>
   <si>
     <t>F-Test Difference</t>
+  </si>
+  <si>
+    <t>Städteregion</t>
+  </si>
+  <si>
+    <t>Rostock</t>
+  </si>
+  <si>
+    <t>Updated with better average and CI:</t>
+  </si>
+  <si>
+    <t>error fear is 29.30729972712159</t>
+  </si>
+  <si>
+    <t>error behavior is 26.840180211506222</t>
+  </si>
+  <si>
+    <t>error infected is 411.79262403779404</t>
+  </si>
+  <si>
+    <t>RMSE Fear is 0.20276969522579072</t>
+  </si>
+  <si>
+    <t>RMSE Behavior is 0.06571242278882417</t>
+  </si>
+  <si>
+    <t>RMSE Infected is 0.06957368516162281</t>
+  </si>
+  <si>
+    <t>MAE% Fear is 0.3337801834614866</t>
+  </si>
+  <si>
+    <t>MAE% Behavior is 0.09168027239374525</t>
+  </si>
+  <si>
+    <t>MAE% Infected is 0.1284379676776192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           &lt;1e-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          1.0289460684214389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.8808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            1.0289460684214389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          1.034468208565099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.8586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            1.034468208565099</t>
+  </si>
+  <si>
+    <t>Updated with CI and random</t>
+  </si>
+  <si>
+    <t>error behavior is 544.5765037069582</t>
+  </si>
+  <si>
+    <t>error infected is 463.6170882699901</t>
+  </si>
+  <si>
+    <t>RMSE Behavior is 0.35962144343792973</t>
+  </si>
+  <si>
+    <t>RMSE Infected is 0.3985508591822592</t>
+  </si>
+  <si>
+    <t>MAE% Behavior is 0.5486737044203217</t>
+  </si>
+  <si>
+    <t>MAE% Infected is 0.4518233903634981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          0.6129456526008813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.0105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            0.6129456526008813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          0.3166650808107994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            0.3166650808107994</t>
+  </si>
+  <si>
+    <t>(ignore fear, its previous data)</t>
+  </si>
+  <si>
+    <t>F-Test between infections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          1.678690539781731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.0068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            1.678690539781731</t>
+  </si>
+  <si>
+    <t>Tests with CI and random</t>
+  </si>
+  <si>
+    <t>error fear is 34.514690121122264</t>
+  </si>
+  <si>
+    <t>error infected is 306.99673514265356</t>
+  </si>
+  <si>
+    <t>RMSE Fear is 0.2489163797875442</t>
+  </si>
+  <si>
+    <t>RMSE Behavior is Inf</t>
+  </si>
+  <si>
+    <t>RMSE Infected is 0.10173203027913377</t>
+  </si>
+  <si>
+    <t>MAE% Behavior is 0.5684229784987295</t>
+  </si>
+  <si>
+    <t>MAE% Infected is 0.16090704936150627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          1.0459440945189094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.8134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            1.0459440945189094</t>
+  </si>
+  <si>
+    <t>Fest Infected old model new model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          1.0110935124528653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.9538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            1.0110935124528653</t>
+  </si>
+  <si>
+    <t>F-Test CI and new</t>
+  </si>
+  <si>
+    <t>error fear is 20.606175719854132</t>
+  </si>
+  <si>
+    <t>error behavior is 29.207194919934444</t>
+  </si>
+  <si>
+    <t>error infected is 556.279240193365</t>
+  </si>
+  <si>
+    <t>RMSE Fear is 0.1551580133623384</t>
+  </si>
+  <si>
+    <t>RMSE Behavior is 0.09160439693571544</t>
+  </si>
+  <si>
+    <t>RMSE Infected is 0.0651252109777371</t>
+  </si>
+  <si>
+    <t>MAE% Fear is 0.23380379063806825</t>
+  </si>
+  <si>
+    <t>MAE% Behavior is 0.11276630858940125</t>
+  </si>
+  <si>
+    <t>MAE% Infected is 0.1109341206422522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          0.8844333912886818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.5187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            0.8844333912886818</t>
+  </si>
+  <si>
+    <t>F-Test old vs new Infected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    point estimate:          0.8852689844216468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    two-sided p-value:           0.5220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    F statistic:            0.8852689844216468</t>
+  </si>
+  <si>
+    <t>Contacts * 0.9</t>
+  </si>
+  <si>
+    <t>Contacts * 0.8</t>
+  </si>
+  <si>
+    <t>Contacts * 1.1</t>
+  </si>
+  <si>
+    <t>Contacts * 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.125, 0.25, 0.5, 0.625, 0.625, 1.0625, 1.25, 1.75, 2.6875, 3.4375, 4.1875, 5.6875, 7.9375, 10.623437500000007, 14.3125, 18.93593750000001, 24.37343750000001, 27.62343750000001, 32.8125, 41.0, 45.0, 49.3125, 53.8125, 59.06093750000001, 56.81093750000001, 59.875, 69.3125, 73.625, 75.375, 79.05781250000003, 82.9375, 78.25, 79.125, 90.125, 93.62343750000001, 96.56093750000001, 98.12031250000003, 99.87343750000001, 93.12187500000002, 90.3125, 106.875, 111.25, 112.4375, 112.8125, 111.62343750000001, 103.25, 101.5625, 119.24843750000001, 121.6875, 122.93593750000001, 122.4375, 117.9375, 108.75, 105.875, 124.8125, 126.8125, 127.0625, 125.4375, 121.625, 111.6875, 109.75, 129.4375, 130.0, 129.625, 128.3125, 124.8125, 114.875, 107.3125, 128.25, 129.0625, 127.8125, 125.75, 121.4375, 111.6875, 104.5625, 125.0, 122.1875, 118.75, 115.625, 112.93593750000001, 104.0625, 96.8125, 112.6875, 107.0625, 103.5625, 101.125, 98.75, 91.9375, 85.3125, 99.0, 96.25, 93.06093750000001, 96.5625, 95.625, 88.4375, 81.9375, 97.625, 92.5, 88.3125, 88.0625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.3125, 0.375, 0.5625, 0.875, 1.0625, 1.125, 1.75, 2.25, 3.125, 4.5, 5.9375, 7.4375, 9.875, 13.4375, 17.625, 22.625, 28.8125, 35.9375, 39.3125, 44.9375, 55.25, 60.0, 64.875, 70.5625, 75.75, 72.3125, 75.75, 87.0625, 91.125, 92.75, 97.0, 100.8125, 94.625, 94.375, 105.75, 109.5, 111.625, 112.125, 111.125, 103.125, 99.0625, 116.6875, 120.1875, 121.0625, 119.875, 116.8125, 107.6875, 104.875, 123.0, 125.5, 125.9375, 124.75, 119.1875, 109.875, 107.75, 126.125, 127.625, 127.8125, 125.9375, 122.5625, 112.6875, 111.875, 129.6875, 130.0, 129.8125, 128.6875, 125.9375, 115.875, 109.3125, 128.625, 129.4375, 128.5, 126.5625, 122.9375, 113.375, 107.0, 126.0625, 124.0625, 121.5, 118.5, 115.625, 106.5, 99.6875, 115.625, 110.75, 107.5, 105.75, 102.625, 95.25, 88.5, 102.375, 99.5, 96.875, 100.75, 100.0625, 92.375, 85.625, 101.4375, 96.625, 92.125, 92.5], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.375, 0.5625, 0.6875, 0.875, 1.3125, 1.625, 1.8125, 2.625, 3.5, 4.9375, 6.875, 9.375, 11.625, 15.0625, 20.439062499999977, 25.8125, 32.0625, 39.75156249999998, 48.1875, 50.9375, 56.8125, 69.375, 74.125, 79.0, 84.875, 90.12656249999998, 85.62656249999998, 89.6875, 102.1875, 105.8125, 106.875, 111.125, 114.25, 106.6875, 105.625, 117.25, 121.375, 122.1875, 122.1875, 119.5625, 110.5625, 105.4375, 123.4375, 126.4375, 127.0, 124.6875, 120.375, 110.625, 107.75156249999998, 125.8125, 127.875, 127.9375, 126.375, 120.4375, 111.0625, 109.75, 127.125, 128.1875, 128.375, 126.4375, 123.5, 113.625, 113.6875, 129.875, 130.0, 130.0, 129.0625, 126.9375, 116.8125, 111.75, 129.0, 129.75, 129.125, 127.375, 124.375, 115.125, 109.875, 127.125, 125.9375, 124.25, 121.3125, 118.43906249999998, 109.0625, 102.9375, 118.75, 114.9375, 111.6875, 110.5625, 106.6875, 98.8125, 91.93906249999998, 106.125, 103.375, 100.75, 105.0625, 104.6875, 96.625, 89.4375, 105.1875, 100.5625, 96.5, 97.75]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.125, 0.4375, 0.75, 1.0, 1.5, 2.0, 2.8125, 3.75, 5.435937500000007, 6.623437500000007, 8.25, 11.123437500000007, 13.685937500000007, 16.0, 18.4375, 20.93593750000001, 21.375, 22.5625, 26.3125, 29.125, 30.62343750000001, 32.875, 35.3125, 34.4375, 34.0, 37.6875, 40.5, 42.6875, 43.99843750000001, 43.9375, 41.5, 39.43593750000001, 44.9375, 48.6875, 50.49843750000001, 50.9375, 50.1875, 47.0625, 44.9375, 51.0, 54.5625, 56.12343750000001, 56.125, 54.625, 50.75, 48.125, 53.9375, 57.125, 58.1875, 57.9375, 56.0625, 51.5625, 48.5, 55.6875, 58.6875, 59.4375, 58.875, 56.6875, 52.4375, 48.62343750000001, 54.4375, 56.6875, 57.0, 55.75, 53.3125, 49.1875, 45.75, 50.75, 51.3125, 49.875, 48.1875, 46.06093750000001, 42.625, 39.625, 42.375, 41.3125, 39.5, 37.625, 36.375, 34.0625, 31.75, 33.875, 33.5625, 32.5625, 33.1875, 33.0, 31.125, 29.1875, 32.25, 31.375, 29.9375, 28.875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.0625, 0.1875, 0.4375, 0.5625, 1.0, 1.375, 1.875, 2.75, 3.6875, 5.0, 6.5625, 9.0, 10.625, 12.6875, 16.5, 19.6875, 22.4375, 25.375, 28.6875, 28.6875, 29.875, 34.5625, 37.8125, 39.6875, 42.0625, 44.625, 42.8125, 41.75, 45.875, 49.4375, 51.5, 52.1875, 51.8125, 48.3125, 45.5, 50.9375, 54.875, 56.5625, 56.1875, 54.5, 50.625, 47.8125, 53.625, 57.4375, 58.75, 58.4375, 55.8125, 51.6875, 48.5625, 54.625, 57.75, 58.8125, 58.3125, 56.4375, 51.9375, 49.125, 56.0, 58.875, 59.6875, 59.125, 57.3125, 52.9375, 49.25, 54.875, 57.0, 57.4375, 56.25, 54.0625, 50.0, 46.625, 51.5625, 52.5, 51.5625, 49.8125, 47.75, 44.1875, 41.0625, 44.1875, 43.4375, 41.75, 40.1875, 38.625, 36.1875, 33.5625, 35.8125, 35.375, 34.4375, 35.25, 35.375, 33.125, 31.0, 34.125, 33.4375, 31.875, 31.1875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.1875, 0.5, 0.875, 1.125, 1.6875, 2.3125, 3.0625, 4.3125, 5.814062499999977, 7.6875, 10.0, 13.0625, 15.3125, 17.689062499999977, 22.1875, 26.064062499999977, 29.125, 32.4375, 35.87656249999998, 35.625, 36.875, 42.0, 45.3125, 47.3125, 49.6875, 52.0625, 49.50156249999998, 47.875, 52.0625, 56.375, 58.25, 58.56406249999998, 57.4375, 53.125, 49.625, 55.1875, 59.1875, 60.875, 60.0625, 57.5, 53.0625, 49.6875, 55.5625, 59.375, 60.4375, 59.9375, 56.6875, 52.375, 49.0, 55.1875, 58.25, 59.25, 58.625, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">56.8125, 52.3125, 49.75, 56.3125, 59.0, 59.875, 59.375, 57.875, 53.4375, 50.0625, 55.375, 57.3125, 57.875, 56.75, 54.9375, 50.875, 47.75, 52.4375, 53.6875, 53.1875, 51.5625, 49.5625, 45.8125, 42.625, 46.125, 45.875, 44.3125, 43.0, 41.25, 38.5625, 35.62656249999998, 38.0625, 37.4375, 36.625, 37.625, 38.0, 35.3125, 33.0625, 36.1875, 35.5625, 34.0625, 33.9375]), ([0.0, 0.375, 0.75, 1.5625, 3.1875, 5.0, 6.0625, 8.1875, 12.625, 18.43593750000001, 25.4375, 33.68593750000001, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">47.0, 54.31093750000001, 64.0, 90.3125, 115.5625, 146.6875, 188.0, 236.0625, 273.875, 307.48437500000006, 371.2484375, 433.240625, 507.8703125, 583.9359375, 672.9328125000001, 744.996875, 809.7296875000001, 925.875, 1030.9281250000001, 1148.4890625, 1279.0921875000001, 1408.1156250000001, 1529.11875, 1635.1140625, 1793.1921875000003, 1952.4359375000004, 2108.89375, 2274.7734375, 2463.1734375, 2595.409375, 2707.78125, 2899.9328125, 3103.365625, 3320.2781250000003, 3525.2859375000003, 3682.6828125, 3795.8921875, 3950.4812500000003, 4154.618750000001, 4371.3546875, 4627.2953125, 4808.314062500001, 4988.05625, 5129.40625, 5234.8078125, 5495.4609375, 5706.83125, 5974.096875, 6185.056250000001, 6380.109375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6457.6796875, 6584.126562500001, 6806.5984375, 7072.1796875, 7335.2734375, 7563.6765625, 7757.475, 7821.040625000001, 7968.0203125, 8316.80625, 8764.3921875, 9149.428125, 9421.5703125, 9629.16875, 9690.803125, 9771.4828125, 10055.1953125, 10367.8, 10663.5546875, 10874.659375, 11054.0578125, 11125.4875, 11188.7953125, 11387.3703125, 11577.9859375, 11768.109375, 11892.3171875, 12033.1796875, 12079.4, 12147.6859375, 12274.0484375, 12380.6046875, 12474.309375, 12565.625, 12663.6828125, 12711.3046875, 12759.6734375, 12838.1828125, 12920.6875, 12982.9328125, 13064.3734375, 13162.2078125, 13196.91875, 13238.0546875, 13324.5546875, 13400.8546875, 13464.7453125, 13535.8109375, 13608.496875, 13640.25], [0.0, 0.9375, 1.625, 3.0, 5.6875, 8.75, 10.5625, 13.3125, 20.25, 28.875, 39.0, 51.75, 71.0, 81.0, 96.0, 129.75, 164.8125, 210.375, 263.5, 331.0, 377.125, 429.1875, 510.625, 595.4375, 688.6875, 792.3125, 906.875, 997.6875, 1094.625, 1233.1875, 1372.625, 1517.5, 1673.125, 1840.0, 1964.6875, 2098.875, 2286.9375, 2480.6875, 2666.5, 2862.125, 3068.4375, 3208.4375, 3349.0, 3550.0625, 3778.75, 4011.4375, 4229.4375, 4419.375, 4535.875, 4645.8125, 4860.375, 5112.9375, 5369.875, 5584.75, </t>
+  </si>
+  <si>
+    <t>5754.875, 5849.25, 5953.0625, 6173.5625, 6444.0625, 6713.8125, 6933.75, 7090.5625, 7182.375, 7283.5625, 7512.875, 7781.25, 8045.875, 8253.25, 8416.4375, 8501.375, 8603.625, 8967.25, 9376.6875, 9734.625, 9998.0, 10180.1875, 10257.0625, 10333.0625, 10576.875, 10883.4375, 11139.0625, 11326.1875, 11466.875, 11536.75, 11605.6875, 11783.25, 11949.75, 12095.4375, 12217.0, 12322.0625, 12375.0, 12430.3125, 12543.6875, 12635.25, 12719.5, 12802.125, 12877.5, 12924.125, 12964.9375, 13041.75, 13109.625, 13174.875, 13250.5625, 13325.9375, 13366.125, 13403.5, 13482.125, 13548.875, 13608.25, 13671.1875, 13731.5, 13760.125], [0.0, 1.625, 2.6875, 4.625, 8.75, 13.3125, 16.0, 19.626562499999977, 29.3125, 41.75156249999998, 55.375, 72.6875, 98.62656249999998, 112.18906249999998, 131.81406249999998, 175.19062499999995, 221.00468749999993, 275.1312499999999, 345.0703124999999, 431.0625, 490.0062499999999, 557.2062499999997, 659.9390625, 768.4453124999999, 876.3796874999999, 1015.0718749999999, 1146.3828125, 1252.7781249999996, 1378.8859374999997, 1533.125, 1702.0171874999996, 1876.5046874999998, 2060.078125, 2246.4546874999996, 2399.1546874999995, 2540.8203125, 2771.325, 2965.8968749999995, 3189.8890625, 3400.9812499999994, 3620.1124999999993, 3759.8140625, 3906.7062499999997, 4096.151562499999, 4340.940625, 4598.0640625, 4832.6890625, 5029.326562499999, 5136.1734375, 5253.639062499998, 5470.690625, 5732.289062499999, 6011.210937499999, 6228.21875, 6373.146874999999, 6469.226562499999, 6547.4453125, 6776.264062499999, 7039.2671875, 7310.304687499999, 7545.5046875, 7682.5078125, 7763.201562499999, 7849.956249999999, 8072.440625, 8350.396874999999, 8598.0015625, 8807.515625, 8956.690625, 9038.1546875, 9138.884375, 9495.770312499999, 9888.7515625, 10215.5484375, 10485.128125, 10632.259375, 10714.4625, 10778.384375, 11002.896875, 11265.44375, 11512.94375, 11672.31875, 11806.6984375, 11869.009375, 11939.9421875, 12103.5, 12239.375, 12357.375, 12472.3859375, 12559.128125, 12611.065625, 12662.8796875, 12760.25625, 12841.378125, 12915.1921875, 12984.390625, 13054.8203125, 13095.8203125, 13130.753125, 13201.1296875, 13264.5015625, 13324.321875, 13392.190625, 13461.5, 13496.3765625, 13532.13125, 13604.384375, 13664.6265625, 13718.2515625, 13772.503125, 13829.5015625, 13853.3125]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.12343750000000675, 0.1875, 0.25, 0.25, 0.25, 0.625, 1.0, 1.3125, 1.9375, 2.5, 3.125, 4.125, 5.75, 8.0625, 10.748437500000007, 14.0625, 18.37343750000001, 20.93593750000001, 23.9375, 31.49843750000001, 36.6875, 41.6875, 48.12343750000001, 53.06093750000001, 52.1875, 55.81093750000001, 67.49843750000001, 71.49843750000001, 75.87343750000001, 81.3125, 86.875, 82.1875, 83.99843750000001, 97.87343750000001, 100.5, 104.4375, 107.18593750000001, 108.375, 101.99843750000001, 100.12343750000001, 114.8125, 118.3125, 119.25, 119.56093750000001, 117.875, 109.125, 105.375, 123.4375, 125.875, 125.8125, 124.6875, 119.8125, 110.0, 105.24843750000001, 125.9375, 127.75, 127.5, 126.0625, 121.6875, 112.3125, 109.9375, 129.5625, 130.0, 129.6875, 128.5, 125.625, 115.6875, 108.9375, 128.125, 129.0, 128.125, 125.875, 122.5625, 112.6875, 105.5, 125.6875, 124.6875, 120.25, 118.5625, 115.0625, 106.25, 98.5, 114.75, 109.8125, 105.625, 104.4375, 104.9375, 96.9375, 89.49843750000001, 101.375, 96.5, 95.6875, 100.6875, 100.0, 92.5, 85.75, 100.3125, 95.87343750000001, 91.4375, 90.0], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.3125, 0.4375, 0.5, 0.5, 0.5625, 1.0, 1.5, 2.0625, 2.75, 3.6875, 4.75, 6.3125, 8.875, 12.0625, 16.25, 21.4375, 27.8125, 30.6875, 35.1875, 44.0625, 49.75, 55.75, 62.375, 67.5, 65.5625, 68.6875, 82.5, 85.625, 89.1875, 94.375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.5625, 94.1875, 93.9375, 108.5, 110.5625, 113.5625, 114.625, 114.75, 107.0625, 105.1875, 119.625, 122.8125, 123.75, 122.4375, 119.75, 110.625, 107.5, 124.5625, 127.1875, 127.0, 125.5625, 120.6875, 111.0625, 107.0625, 126.6875, 128.125, 127.8125, 126.5, 122.5625, 113.25, 111.4375, 129.75, 130.0, 129.875, 128.75, 126.375, 116.4375, 110.5625, 128.5, 129.375, 128.6875, 126.6875, 123.625, 113.875, 106.875, 126.5, 125.875, 122.3125, 120.5625, 117.0625, 107.9375, 100.5625, 117.25, 112.4375, 108.5625, 107.4375, 107.9375, 99.4375, 91.875, 104.5, 99.5, 99.0, 103.25, 103.0, 95.125, 88.1875, 103.875, 98.5, 94.125, 93.3125], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.5625, 0.6875, 0.75, 0.75, 0.875, 1.375, 2.0, 2.8125, 3.625, 4.9375, 6.4375, 8.5625, 12.1875, 16.3125, 22.314062499999977, 29.75, 37.4375, 40.8125, 46.00156249999998, 56.75156249999998, 62.125, 68.6875, 75.75, 81.1875, 78.0, 80.68906249999998, 95.375, 98.0625, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.87656249999998, 105.68906249999998, 110.0625, 103.75, 101.87656249999998, 116.5625, 118.4375, 120.375, 120.1875, 119.0625, 110.75, 108.6875, 122.875, 125.75, 126.625, 124.5, 121.125, 111.9375, 109.5, 125.50156249999998, 128.125, 127.8125, 126.25, 121.5625, 112.12656249999998, 108.875, 127.25, 128.4375, 128.0, 126.875, 123.5, 114.1875, 112.9375, 129.9375, 130.0, 130.0, 129.0, 127.0625, 117.25, 112.25156249999998, 128.875, 129.6875, 129.25, 127.5, 124.6875, 115.125, 108.5, 127.25, 127.0625, 124.3125, 122.5625, 119.0625, 109.8125, 102.8125, 119.8125, 115.31406249999998, 111.8125, 110.5625, 110.9375, 101.9375, 94.375, 107.8125, 102.8125, 102.375, 105.6875, 105.875, 97.68906249999998, 90.5, 107.5625, 101.3125, 96.875, 96.8125]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.25, 0.3125, 0.5625, 0.9375, 1.25, 1.9375, 2.6234375000000068, 3.8125, 4.75, 5.8125, 7.8125, 10.125, 12.0625, 14.498437500000007, 17.0, 17.87343750000001, 19.375, 22.9375, 26.0625, 28.4375, 31.18593750000001, 34.4375, 34.0, 33.93593750000001, 39.5, 42.1875, 45.0625, 46.8125, 48.06093750000001, 45.75, 44.0625, 49.375, 53.0, 55.0, 55.4375, 54.8125, 50.9375, 48.25, 54.0, 57.5625, 58.9375, 58.6875, 56.375, 51.9375, 48.125, 54.6875, 57.6875, 58.8125, 58.5, 56.0, 51.75, 48.375, 55.625, 58.6875, 59.375, 59.0, 57.1875, 52.8125, 48.8125, 54.375, 56.9375, 57.0625, 56.0625, 53.8125, 49.5, 46.0625, 51.25, 52.625, 51.0625, 49.625, 47.625, 44.0625, 40.875, 43.6875, 42.75, 40.6875, 39.4375, 39.0625, 36.4375, 34.0, 35.5625, 34.3125, 33.625, 34.75, 35.375, 33.125, 31.0, 33.8125, 33.0, 31.5625, 30.625], [0.0, 0.0, 0.0, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.1875, 0.5625, 0.6875, 1.0, 1.5, 2.125, 3.1875, 4.3125, 6.0, 7.625, 9.375, 12.125, 14.9375, 17.5, 20.4375, 23.4375, 24.125, 25.1875, 30.375, 33.5, 35.875, 38.6875, 42.0, 40.875, 40.0, 45.8125, 48.9375, 51.3125, 52.4375, 52.8125, 49.6875, 47.5, 52.75, 56.3125, 58.25, 58.125, 56.5625, 52.4375, 49.25, 54.9375, 58.625, 59.875, 59.375, 56.6875, 52.3125, 48.5625, 55.0, 58.0, 59.0, 58.75, 56.4375, 52.1875, 48.875, 55.9375, 58.875, 59.625, 59.1875, 57.6875, 53.25, 49.3125, 54.6875, 57.1875, 57.375, 56.5, 54.5, 50.1875, 46.6875, 51.8125, 53.4375, 52.3125, 50.875, 48.8125, 45.1875, 41.875, 45.1875, 44.375, 42.375, 41.125, 40.75, 37.9375, 35.3125, 37.1875, 35.875, 35.1875, 36.1875, 36.75, 34.4375, 32.1875, 35.5, 34.4375, 32.875, 31.9375], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.375, 0.875, 1.0625, 1.4375, 2.0625, 3.0625, 4.5, 6.125, 8.4375, 10.6875, 13.1875, 16.75, 19.75, 22.8125, 26.3125, 29.875, 30.1875, 31.125, 36.93906249999998, 40.3125, 42.9375, 45.5, 48.625, 46.8125, 45.1875, 51.125, 54.375, 56.5, 56.9375, 56.4375, 52.6875, 49.875, 55.0625, 58.625, 60.5625, 59.9375, 57.75, 53.375, 50.0, 55.625, 59.375, 60.5625, 59.875, 57.0, 52.6875, 49.0, 55.25, 58.25, 59.1875, 58.9375, 56.875, 52.625, 49.375, 56.25, 59.0, 59.875, 59.375, 58.125, 53.75, 49.8125, 55.0, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">57.4375, 57.6875, 56.9375, 55.25, 50.8125, 47.3125, 52.375, 54.1875, 53.5625, 52.1875, 50.125, 46.375, 43.00156249999998, 46.75, 46.1875, 44.3125, 43.00156249999998, 42.56406249999998, 39.43906249999998, 36.75, 38.9375, 37.625, 36.9375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.5625, 38.1875, 35.75, 33.375, 37.25, 36.0625, 34.3125, 33.4375]), ([0.0, 0.25, 0.375, 1.1875, 1.875, 3.4375, 4.5625, 5.5, 8.1875, 12.623437500000007, 17.75, 24.875, 34.3125, 39.93593750000001, 47.25, 66.87343750000001, 87.18593750000001, 115.3125, 144.3125, 188.3734375, 218.4375, 250.4328125, 299.61875000000003, 353.18125000000003, 414.621875, 483.371875, 557.559375, 623.2968750000001, 697.0609375, 797.24375, 882.3015625, 1009.4593750000001, 1142.234375, 1268.6203125, 1351.621875, 1466.496875, 1617.7375, 1795.3125, 1955.9125000000001, 2139.2765625, 2336.2265625, 2440.7203125, 2609.55, 2812.990625, 3035.2156250000003, 3230.51875, 3450.115625, 3664.121875, 3795.4046875000004, 3965.234375, 4161.7453125, 4415.478125000001, 4660.3625, 4894.175, 5092.9359375, 5220.4265625, 5327.8109375, 5576.2390625, 5838.428125, 6099.140625, 6322.240625, 6491.290625000001, 6609.75625, 6732.8640625, 6954.015625, 7214.640625, 7478.559375, 7714.8109375, 7885.4296875, 8005.05625, 8087.8703125, 8461.5296875, 8878.4671875, 9261.7875, 9549.875, 9764.746875, 9824.415625, 9930.6234375, 10171.159375, 10507.175, 10786.18125, 10989.9359375, 11143.8734375, 11227.2828125, 11289.0796875, 11474.746875, 11680.0546875, 11837.74375, 11977.9984375, 12087.4359375, 12143.8671875, 12211.1796875, 12345.7484375, 12446.478125, 12550.05625, 12635.3109375, 12732.684375, 12780.1171875, 12819.5875, 12916.3109375, 12987.61875, 13059.6234375, 13150.18125, 13231.4375, 13276.3109375, 13317.5515625, 13407.6875, 13486.1828125, 13549.871875, 13610.559375, 13680.5609375, 13714.7453125], [0.0, 0.5, 1.0, 2.25, 3.3125, 5.6875, 7.125, 8.625, 12.625, 19.0, 26.875, 37.25, 49.875, 58.8125, 69.5, 95.3125, 123.25, 160.375, 203.0625, 259.375, 298.625, 343.25, 407.125, 476.9375, 556.9375, 645.0, 746.6875, 825.5, 911.5625, 1032.875, 1161.4375, 1296.5, 1445.125, 1598.8125, 1716.1875, 1839.5, 2030.125, 2213.3125, 2397.5625, 2592.5625, 2802.6875, 2953.4375, 3097.5, 3322.25, 3549.3125, 3783.6875, 4004.875, 4211.0, 4343.875, 4475.0, 4695.125, 4952.4375, 5216.6875, 5440.9375, 5624.875, 5728.5625, 5839.75, 6063.75, 6347.9375, 6618.25, 6843.3125, 7004.625, 7097.625, 7191.75, 7422.3125, 7694.875, 7959.125, 8174.125, 8334.3125, 8425.125, 8524.4375, 8900.25, 9312.6875, 9680.125, 9949.0625, 10134.4375, 10214.6875, 10294.3125, 10530.6875, 10836.0625, 11092.8125, 11278.1875, 11420.5, 11485.75, 11551.6875, 11732.5, 11910.75, 12052.625, 12181.5625, 12292.5, 12349.9375, 12407.125, 12525.1875, 12620.25, 12707.375, 12792.8125, 12880.25, 12925.9375, 12970.625, 13052.4375, 13120.0, 13189.6875, 13269.25, 13349.0625, 13389.6875, 13429.25, 13514.75, 13582.4375, 13643.3125, 13706.1875, 13764.5625, 13793.875], [0.0, 0.8125, 1.9375, 3.5, 5.0, 8.1875, 10.0, 11.875, 17.1875, 25.4375, 35.875, 49.875, 66.00156249999998, 78.68906249999998, 91.87656249999998, 125.87656249999998, 161.37656249999998, 208.00156249999998, 262.125, 333.44062499999995, 379.1265625, 433.82343749999984, 516.7015624999998, 602.1343749999999, 701.2671874999997, 805.125, 927.8140625, 1028.81875, 1124.5625, 1277.3171874999998, 1427.1265625, 1583.253125, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1755.94375, 1919.190625, 2054.5140625, 2191.173437499999, 2401.7593749999996, 2602.8765625, 2807.825, 3020.0625, 3236.265625, 3426.5, 3553.7078125, 3802.5, 4032.5671875, 4270.6328125, 4504.799999999999, 4697.590625, 4812.043749999999, 4954.414062499999, 5164.3140625, 5428.521874999999, 5711.2609375, 5912.19375, 6089.8796875, 6180.63125, 6283.9, 6509.6296875, 6795.8203125, 7078.015625, 7282.0671875, 7432.0078125, 7524.9375, 7611.018749999999, 7861.3453125, 8122.789062499999, 8367.71875, 8571.7546875, 8729.075, 8810.8765625, 8908.7625, 9284.3140625, 9683.978125, 10037.8796875, 10286.3234375, 10458.76875, 10531.815625, 10612.5890625, 10839.946875, 11118.731249999999, 11347.65, 11529.503125, 11658.898437, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11725.0078125, 11787.128125, 11949.5703125, 12108.6875, 12243.1984375, 12356.315625, 12464.0, 12523.390625, 12575.1296875, 12683.690625, 12767.44375, 12845.1875, 12929.8765625, 13007.5703125, 13050.63125, 13098.5046875, 13170.3171875, 13232.6265625, 13300.9375, 13375.1875, 13450.9390625, 13489.5, 13520.7515625, 13601.253125, 13665.9375, 13724.253125, 13782.1921875, 13836.0, 13862.6265625]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.25, 0.5625, 0.5625, 0.6875, 1.0625, 1.5625, 2.0, 2.75, 3.875, 4.875, 6.375, 8.9375, 12.0, 15.9375, 20.8125, 26.31093750000001, 29.81093750000001, 34.25, 42.56093750000001, 49.12343750000001, 53.625, 60.375, 65.3125, 63.43593750000001, 65.125, 77.625, 81.18593750000001, 87.25, 90.93593750000001, 95.30937500000002, 90.1875, 91.68593750000001, 103.3125, 107.125, 110.9375, 112.37343750000001, 114.1875, 106.125, 104.8125, 118.5625, 122.625, 123.0, 122.1875, 118.875, 109.5625, 105.6875, 124.625, 127.1875, 126.0625, 124.625, 119.5, 110.0, 104.99843750000001, 126.3125, 127.75, 127.4375, 125.8125, 120.9375, 111.375, 109.9375, 129.4375, 130.0, 129.5, 128.375, 124.375, 114.625, 107.4375, 128.1875, 129.0, 128.0, 126.0625, 121.9375, 112.0, 104.5, 125.75, 123.0, 120.875, 116.5625, 114.0625, 105.25, 98.0, 113.8125, 108.6875, 105.4375, 104.0625, 100.6875, 93.12343750000001, 86.0, 99.125, 94.125, 94.875, 98.625, 99.4375, 92.0, 85.0625, 95.875, 92.375, 88.0625, 86.0], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.1875, 0.4375, 0.5625, 0.875, 0.9375, 1.125, 1.625, 2.25, 2.9375, 4.125, 5.8125, 7.5625, 9.875, 13.75, 18.375, 23.75, 29.625, 36.5625, 39.9375, 44.25, 55.125, 61.5625, 66.6875, 73.5625, 79.125, 75.6875, 76.9375, 90.875, 94.4375, 98.9375, 102.6875, 106.0625, 99.625, 99.75, 111.5625, 115.125, 118.125, 117.4375, 118.0625, 109.4375, 107.4375, 121.0, 124.9375, 125.1875, 123.75, 120.0, 110.625, 107.5625, 125.5625, 127.6875, 127.0, 125.375, 120.4375, 110.8125, 106.625, 126.8125, 128.0, 127.75, 126.1875, 121.75, 112.125, 111.25, 129.6875, 130.0, 129.75, 128.625, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">125.6875, 115.875, 109.0625, 128.5, 129.3125, 128.5, 126.75, 123.125, 113.0625, 105.9375, 126.375, 124.5625, 122.5, 118.6875, 116.0625, 106.9375, 99.75, 115.9375, 111.3125, 108.25, 106.5625, 103.375, 95.4375, 88.25, 102.0625, 97.125, 97.0625, 101.25, 102.75, 94.875, 87.6875, 100.125, 95.75, 91.6875, 89.5625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.375, 0.6875, 0.875, 1.1875, 1.3125, 1.5625, 2.1875, 3.0, 4.0, 5.6875, 8.0, 10.5625, 13.875, 19.125, 25.375, 32.25, 38.56406249999998, 47.00156249999998, 49.625, 53.75, 66.9375, 73.25, 78.6875, 85.875, 91.31406249999998, 86.8125, 87.56406249999998, 101.6875, 105.00156249999998, 108.5625, 111.5625, 114.3125, 106.6875, 105.625, 117.125, 120.75, 122.875, 121.25, 120.625, 111.625, 109.875, 122.9375, 126.625, 126.6875, 125.125, 121.0, 111.5625, 109.4375, 126.375, 128.125, 127.6875, 125.9375, 121.375, 111.6875, 108.4375, 127.25, 128.25, 128.0, 126.5625, 122.625, 112.9375, 112.375, 129.875, 130.0, 129.9375, 128.875, 126.75, 117.0625, 110.75, 128.8125, 129.5625, 129.0, 127.375, 124.375, 114.25, 107.5625, 127.0, 126.0, 124.125, 120.8125, 118.125, 108.75, 101.5, 118.3125, 114.0625, 111.3125, 109.125, 106.25156249999998, 98.0625, 90.8125, 105.1875, 100.5, 99.875, 104.0, 106.0, 97.75, 90.375, 104.5625, 99.0625, 95.37656249999998, 93.4375]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.25, 0.5625, 0.6875, 1.0, 1.75, 2.25, 3.125, 4.375, 5.748437500000007, 7.3125, 8.8125, 11.685937500000007, 14.6875, 16.9375, 19.8125, 22.74843750000001, 23.25, 24.0, 28.3125, 31.8125, 34.375, 37.1875, 40.0625, 38.74843750000001, 38.5625, 43.25, 46.5625, 49.375, 50.5, 51.9375, 48.875, 47.5625, 52.3125, 56.125, 57.6875, 57.875, 56.1875, 52.375, 49.1875, 55.0625, 58.8125, 59.25, 58.75, 56.3125, 51.625, 48.125, 54.75, 57.8125, 58.8125, 58.3125, 55.625, 51.375, 48.4375, 55.6875, 58.8125, 59.25, 58.75, 56.625, 52.375, 48.4375, 54.25, 56.8125, 57.0, 55.9375, 53.6875, 49.56093750000001, 45.8125, 51.3125, 51.9375, 51.125, 48.8125, 46.9375, 43.3125, 40.3125, 43.1875, 42.0625, 40.375, 39.125, 37.5, 34.9375, 32.5625, 34.3125, 33.125, 32.625, 33.6875, 34.6875, 32.625, 30.5, 32.125, 31.125, 29.8125, 28.6875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.125, 0.375, 0.5625, 1.0, 1.1875, 1.75, 2.75, 3.6875, 5.0, 6.75, 8.875, 10.75, 12.5625, 16.1875, 19.875, 22.5, 25.875, 29.375, 29.75, 30.1875, 35.0625, 38.5625, 41.4375, 44.0, 46.5, 44.75, 43.8125, 48.4375, 51.9375, 54.5625, 54.9375, 55.4375, 51.75, 49.625, 54.1875, 58.0, 59.5, 59.3125, 56.9375, 52.8125, 49.625, 55.5, 59.1875, 59.875, 59.25, 56.6875, 52.0, 48.5625, 54.9375, 57.9375, 58.9375, 58.5625, 56.0, 51.75, 48.8125, 55.875, 58.9375, 59.5, 58.9375, 57.3125, 53.0, 49.125, 54.5625, 57.125, 57.3125, 56.3125, 54.3125, 50.125, 46.4375, 51.8125, 52.8125, 52.125, 50.0625, 48.0625, 44.375, 41.3125, 44.4375, 43.5, 42.0, 40.625, 38.9375, 36.25, 33.75, 35.75, 34.625, 33.9375, 35.125, 36.25, 34.0625, 31.8125, 34.0625, 33.0, 31.5625, 30.25], [0.0, 0.0, 0.0, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.3125, 0.6875, 0.9375, 1.4375, 1.8125, 2.5625, 3.875, 5.375, 7.1875, 9.5, 12.25, 14.5, 16.4375, 20.8125, 25.001562499999977, 27.9375, 32.0625, 35.43906249999998, 35.75156249999998, 35.875, 41.25, 44.8125, 47.75, 49.875, 52.0625, 49.625, 47.9375, 52.4375, 55.875, 58.4375, 58.3125, 57.8125, 53.5625, 51.0, 55.4375, 59.3125, 60.75, 60.4375, 57.5625, 53.25, 50.0625, 55.8125, 59.5, 60.3125, 59.6875, 57.125, 52.375, 49.0, 55.125, 58.0, 59.0, 58.8125, 56.4375, 52.125, 49.1875, 56.0, 59.0, 59.75, 59.125, 57.875, 53.5625, 49.8125, 54.875, 57.4375, 57.625, 56.6875, 55.0, 50.75, 47.125, 52.3125, 53.62656249999998, 53.125, 51.3125, 49.375, 45.5625, 42.375, 45.8125, 45.0, 43.8125, 42.25, 40.5625, 37.625, 35.0, 37.3125, 36.3125, 35.5, 36.75, 37.9375, 35.5625, 33.125, 36.0, 34.75, 33.3125, 31.875]), ([0.0, 0.125, 0.5, 1.1875, 2.875, 4.75, 6.25, 7.873437500000007, 12.75, 17.8125, 25.5625, 35.375, 49.1875, 57.625, 67.62343750000001, 94.18593750000001, 121.625, 156.0609375, 194.75, 251.11875000000003, 289.5, 326.8109375, 394.3109375, 467.4984375, 544.678125, 628.371875, 720.9875000000001, 798.4953125000001, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">885.1656250000001, 1000.678125, 1133.371875, 1261.5578125, 1404.43125, 1571.9359375, 1683.3484375, 1792.1140625, 1962.496875, 2138.1125, 2321.2265625, 2513.4328125, 2723.6109375, 2856.6875000000005, 3001.309375, 3219.428125, 3452.6109375, 3678.8109375, 3896.6765625000003, 4107.6109375, 4256.4125, 4376.26875, 4601.1859375, 4877.4984375, 5116.3078125, 5348.103125000001, 5526.740625, 5650.0484375, 5770.1765625, 5982.48125, 6277.7421875, 6521.421875, 6733.0453125, 6919.1, 7001.4921875, 7088.8125, 7330.775000000001, 7596.5625, 7853.5546875, 8073.6734375, 8229.10625, 8305.5, 8409.4359375, 8795.198437500001, 9222.6046875, 9571.9671875, 9838.1125, 10033.3921875, 10116.3125, 10212.0609375, 10434.1734375, 10753.2921875, 11018.865625, 11214.1171875, 11356.428125, 11426.6140625, 11490.1828125, 11675.74375, 11839.625, 12007.4296875, 12134.6734375, 12248.86875, 12302.984375, 12359.115625, 12481.74375, 12583.1703125, 12680.4140625, 12759.3, 12845.121875, 12886.9375, 12936.371875, 13015.5578125, 13087.9875, 13152.625, 13237.80625, 13320.8703125, 13361.55, 13402.934375, 13485.61875, 13552.30625, 13612.6828125, 13676.6875, 13737.0625, 13770.375], [0.0, 0.5, 1.3125, 2.5625, 4.5625, 7.1875, 9.3125, 12.125, 18.8125, 26.25, 36.8125, 50.3125, 67.4375, 79.5, 93.1875, 127.0625, 164.25, 207.5, 260.375, 330.5, 378.125, 432.375, 511.8125, 599.8125, 696.5625, 805.0, 921.9375, 1015.5625, 1111.1875, 1253.5625, 1401.125, 1552.75, </t>
+  </si>
+  <si>
+    <t>1720.5625, 1900.9375, 2032.25, 2162.8125, 2357.875, 2552.0625, 2754.875, 2964.0625, 3180.3125, 3328.9375, 3475.6875, 3688.375, 3920.5625, 4168.5, 4386.1875, 4595.125, 4721.0625, 4851.0, 5064.0625, 5325.9375, 5584.625, 5809.0625, 5982.1875, 6080.9375, 6186.4375, 6413.5, 6694.25, 6952.4375, 7164.125, 7318.1875, 7403.5, 7493.6875, 7722.75, 7992.9375, 8244.3125, 8453.4375, 8604.6875, 8691.6875, 8789.375, 9162.5625, 9565.9375, 9909.1875, 10163.0625, 10343.0625, 10419.75, 10496.25, 10731.0625, 11021.25, 11265.6875, 11449.375, 11589.6875, 11648.125, 11711.8125, 11887.0, 12048.375, 12188.125, 12306.8125, 12413.1875, 12467.8125, 12522.75, 12633.375, 12726.0, 12811.5, 12893.4375, 12968.3125, 13009.5625, 13052.8125, 13128.5625, 13191.8125, 13257.375, 13332.4375, 13412.3125, 13449.25, 13485.875, 13562.3125, 13625.8125, 13683.625, 13739.0625, 13797.75, 13824.5625], [0.0, 1.0, 2.3125, 4.25, 6.4375, 10.0625, 12.75, 17.0, 25.5, 34.625, 48.1875, 66.25156249999998, 86.56406249999998, 102.0, 119.93906249999998, 162.31406249999998, 210.43906249999998, 262.75312499999995, 327.8765625, 411.6890625, 468.375, 535.5625, 638.378125, 740.4390625, 857.1937499999999, 975.5062499999999, 1117.5828124999998, 1235.5703125, 1340.3281249999998, 1504.1890625, 1673.9031249999996, 1832.9859374999992, 2023.1875, 2226.2640625, 2366.3140625, 2516.128125, 2723.8921874999996, 2936.2015625, 3166.0, 3372.8203125, 3603.7812499999995, 3760.0093749999996, 3893.9421875, 4108.63125, 4355.389062499999, 4607.807812499999, 4824.00625, 5029.640625, 5132.00625, 5249.206249999999, 5473.025, 5736.5125, 5990.81875, 6216.015625, 6361.81875, 6465.549999999999, 6558.7671875, 6783.0109375, 7080.912499999999, 7335.5078125, 7538.315625, 7683.201562499999, 7747.0640625, 7841.8234375, 8074.690625, 8329.321875, 8578.021875, 8788.640625, 8937.0390625, 9015.7578125, 9115.396875, 9468.6296875, 9870.1890625, 10192.5859375, 10433.0015625, 10605.071875, 10665.8171875, 10745.5703125, 10974.6390625, 11250.8765625, 11478.5640625, 11651.6875, 11781.753125, 11835.3828125, 11894.1890625, 12069.0640625, 12216.0125, 12339.690625, 12447.1359375, 12552.946875, 12603.578125, 12655.571875, 12761.5671875, 12847.7515625, 12923.7515625, 13003.7609375, 13075.0671875, 13113.125, 13151.9390625, 13222.2515625, 13284.878125, 13345.503125, 13415.4484375, 13491.6890625, 13525.690625, 13559.1265625, 13629.5640625, 13686.5625, 13742.440625, 13794.1890625, 13846.875, 13871.6890625]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.25, 0.25, 0.3125, 0.75, 1.125, 1.4375, 1.8125, 2.625, 3.125, 4.25, 5.9375, 7.998437500000007, 10.625, 14.3125, 18.9375, 21.81093750000001, 26.125, 34.125, 39.0, 46.1875, 52.93593750000001, 58.875, 59.5, 62.4375, 76.0625, 81.9375, 86.06093750000001, 91.62343750000001, 99.0, 92.74843750000001, 96.0, 107.8125, 110.5, 112.5, 115.3125, 117.0625, 109.4375, 106.875, 120.4375, 123.875, 124.625, 123.4375, 119.5625, 110.375, 105.875, 124.125, 127.0, 127.1875, 125.1875, 119.625, 110.0, 106.875, 126.5, 128.0, 127.625, 126.0, 122.4375, 112.9375, 111.1875, 129.4375, 130.0, 129.6875, 128.5, 125.625, 115.75, 109.4375, 127.9375, 129.0625, 128.4359375, 126.4375, 122.5625, 112.75, 105.1875, 125.6875, 123.9375, 121.0625, 117.875, 114.6875, 105.625, 97.75, 115.0, 110.125, 105.25, 106.6875, 102.9375, 95.0625, 88.25, 100.25, 97.0625, 95.8125, 98.81093750000001, 99.6875, 92.0625, 85.25, 97.43593750000001, 95.5625, 91.6875, 89.6875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.0625, 0.1875, 0.3125, 0.5, 0.5, 0.625, 1.0625, 1.5625, 2.0, 2.625, 3.6875, 4.625, 6.25, 8.6875, 11.75, 15.8125, 20.75, 27.0625, 30.3125, 35.0, 44.9375, 49.6875, 57.375, 64.625, 70.875, 69.3125, 72.25, 86.0, 90.875, 94.6875, 100.0625, 105.875, 99.0625, 101.0, 112.375, 114.9375, 116.9375, 118.3125, 118.75, 110.9375, 108.4375, 121.625, 125.0, 125.625, 124.1875, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">120.5625, 111.5625, 107.875, 125.0625, 127.4375, 127.5625, 125.5625, 120.5, 111.0, 108.5625, 126.875, 128.3125, 127.8125, 126.3125, 123.0, 113.5, 112.375, 129.6875, 130.0, 129.875, 128.8125, 126.375, 116.375, 111.0, 128.375, 129.375, 128.8125, 127.0625, 123.375, 113.625, 106.1875, 126.3125, 125.375, 122.8125, 119.75, 116.875, 107.6875, 99.6875, 116.6875, 112.25, 107.9375, 108.9375, 105.0625, 96.9375, 89.9375, 103.25, 99.8125, 97.8125, 101.3125, 102.5625, 94.6875, 87.5, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">101.25, 98.125, 94.875, 92.875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.1875, 0.375, 0.5625, 0.75, 0.75, 1.0, 1.375, 2.0, 2.625, 3.5625, 4.875, 6.25, 8.4375, 11.8125, 16.0625, 21.5625, 27.875, 35.4375, 39.25, 44.3125, 56.18906249999998, 60.375, 67.875, 75.8125, 81.75156249999998, 78.625, 81.3125, 95.0, 99.4375, 102.6875, 107.4375, 111.75, 104.625, 105.25, 116.125, 118.8125, 120.625, 120.875, 120.3125, 112.25, 110.0, 122.8125, 126.0625, 126.5625, 124.9375, 121.625, 112.75, 110.0625, 125.875, 127.8125, 127.9375, 125.9375, 121.4375, 112.125, 110.375, 127.1875, 128.56406249999998, 128.0, 126.625, 123.5625, 114.0625, 113.625, 129.875, 130.0, 130.0, 129.0, 127.0625, 117.0625, 112.6875, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">128.75, 129.6875, 129.1875, 127.625, 124.1875, 114.5625, 107.3125, 126.875, 126.5, 124.375, 121.56406249999998, 118.8125, 109.5625, 101.4375, 118.4375, 114.3125, 110.625, 111.125, 107.375, 99.0625, 91.6875, 106.125, 102.4375, 99.875, 103.6875, 105.0, 97.0, 89.5625, 104.75, 100.6875, 97.875, 96.0]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.1875, 0.3125, 0.5625, 1.0, 1.25, 1.875, 2.75, 3.8125, 4.8125, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1875, 8.310937500000007, 10.5, 12.873437500000007, 15.625, 18.87343750000001, 19.875, 21.4375, 25.875, 29.375, 32.625, 35.62343750000001, 39.81093750000001, 38.99843750000001, 39.8125, 44.875, 48.125, 50.3125, 52.1875, 53.5625, 50.9375, 48.8125, 53.75, 57.1875, 58.875, 58.875, 56.9375, 52.8125, 49.5, 55.0625, 58.625, 59.9375, 59.375, 56.25, 51.8125, 48.375, 54.875, 58.0625, 59.0, 58.4375, 56.4375, 52.0, 48.875, 55.875, 59.0, 59.4375, 58.8125, 57.25, 52.8125, 49.125, 54.4375, 56.8125, 57.125, 56.25, 54.0625, 50.0625, 46.25, 51.375, 52.4375, 51.3125, 49.5, 47.5, 43.875, 40.8125, 44.0625, 42.8125, 40.8125, 40.375, 38.8125, 36.125, 33.75, 35.125, 34.4375, 33.6875, 34.0, 34.875, 32.5625, 30.5625, 33.0625, 32.75, 31.375, 30.25], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.25, 0.4375, 0.6875, 1.0, 1.625, 2.0625, 3.0, 4.1875, 5.875, 7.3125, 9.0625, 12.125, 14.625, 17.375, 20.6875, 24.25, 25.0625, 26.375, 31.4375, 35.0625, 38.0, 41.125, 44.875, 43.25, 43.5, 48.375, 51.5625, 53.625, 55.0, 55.5, 52.5, 49.875, 54.625, 58.125, 59.8125, 59.5625, 57.5, 53.1875, 50.0, 55.5625, 59.0, 60.1875, 59.625, 56.6875, 52.3125, 48.9375, 55.125, 58.25, 59.0625, 58.6875, 56.6875, 52.25, 49.25, 56.125, 59.0, 59.6875, 58.9375, 57.6875, 53.1875, 49.625, 54.75, 57.125, 57.4375, 56.6875, 54.5625, 50.5, 46.6875, 51.8125, 53.25, 52.3125, 50.5625, 48.625, 44.9375, 41.75, 45.0, 44.0, 42.125, 41.5625, 39.9375, 37.1875, 34.625, 36.4375, 35.8125, 34.75, 35.3125, 36.25, 33.8125, 31.75, 34.625, 34.0625, 32.75, 31.625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.43906249999997726, 0.75, 1.0625, 1.5, 2.25, 3.0, 4.25, 5.8125, 8.1875, 10.1875, 12.375, 16.125, 19.126562499999977, 22.125, 26.0, 29.75, 30.25, 31.375, 36.6875, 40.4375, 43.31406249999998, 46.375, 49.5, 47.25, 46.75156249999998, 51.4375, 54.4375, 56.625, 57.375, 57.125, 53.75, 50.75, 55.4375, 59.0, 60.625, 60.1875, 58.0, 53.625, 50.5625, 56.0625, 59.3125, 60.4375, 59.875, 57.125, 52.8125, 49.5625, 55.375, 58.5, 59.1875, 58.875, 56.9375, 52.5, 49.6875, 56.375, 59.0, 59.875, 59.0, 58.125, 53.5625, 50.125, 55.0625, 57.4375, 57.75, 57.0625, 55.0625, 51.0, 47.125, 52.1875, 53.9375, 53.25, 51.625, 49.6875, 45.875, 42.625, 46.0, 45.1875, 43.375, 42.75, 41.125, 38.3125, 35.5625, 37.875, 37.125, 35.875, 36.5625, 37.5, 34.875, 32.8125, 36.125, 35.4375, 34.0625, 33.0625]), ([0.0, 0.0, 0.0625, 0.5625, 2.0625, 3.1875, 4.125, 5.8125, 9.0, 12.6875, 18.18593750000001, 24.6875, 35.0625, 41.87343750000001, 49.8125, 68.625, 90.12343750000001, 116.05937500000002, 150.1234375, 194.7484375, 225.17656250000005, 258.05468750000006, 307.3734375, 366.29843750000003, 430.8109375, 500.5, 586.0500000000001, 648.3703125000001, 728.5, 841.49375, 947.6171875, 1067.684375, 1211.5984375, </t>
+  </si>
+  <si>
+    <t>1362.3734375, 1486.7875000000001, 1595.75, 1769.109375, 1956.6859375, 2156.1859375, 2336.1625, 2559.309375, 2702.7828125, 2869.3343750000004, 3086.228125, 3306.3, 3538.0578125, 3762.8078125, 3997.53125, 4149.1375, 4286.053125, 4512.848437500001, 4763.8125, 5029.05625, 5268.11875, 5452.18125, 5580.3109375, 5693.0, 5913.8734375, 6180.109375, 6457.29375, 6673.68125, 6846.5578125, 6931.484375, 7037.121875, 7258.559375, 7541.609375, 7795.65625, 8014.470312500001, 8176.8, 8263.7484375, 8375.3734375, 8740.2296875, 9170.990625, 9537.8734375, 9805.125, 10008.11875, 10082.8703125, 10171.621875, 10412.1859375, 10728.1796875, 10998.0, 11196.6109375, 11332.740625, 11409.3046875, 11471.303125, 11652.93125, 11835.871875, 11984.8078125, 12110.309375, 12227.1234375, 12285.0578125, 12336.5625, 12455.559375, 12553.121875, 12638.9328125, 12734.6828125, 12818.05625, 12865.309375, 12904.8109375, 12988.3125, 13065.9328125, 13131.43125, 13211.559375, 13290.5609375, 13334.3109375, 13370.4359375, 13454.6234375, 13527.4984375, 13594.4359375, 13658.1859375, 13720.6859375, 13751.5578125], [0.0, 0.125, 0.375, 1.1875, 2.9375, 4.6875, 5.875, 8.0625, 12.625, 18.1875, 25.6875, 35.5, 48.3125, 57.1875, 67.8125, 92.375, 122.5, 155.3125, 197.25, 251.75, 288.625, 331.8125, 396.3125, 465.4375, 545.9375, 632.875, 733.75, 814.1875, 903.3125, 1036.75, 1161.125, 1302.25, 1458.5625, 1624.75, 1754.125, 1885.25, 2079.125, 2275.1875, 2470.5, 2678.3125, 2903.125, 3055.3125, 3216.125, 3435.5, 3666.375, 3902.4375, 4131.75, 4351.0625, 4494.3125, 4629.125, 4848.3125, 5108.75, 5372.6875, 5600.0, 5781.0, 5885.375, 5992.25, 6213.75, 6484.8125, 6758.375, 6973.375, 7129.3125, 7216.0, 7313.8125, 7544.0, 7819.25, 8076.5625, 8284.75, 8446.125, 8536.0, 8637.0625, 8999.0, 9414.3125, 9779.0625, 10041.125, 10226.625, 10304.875, 10386.5, 10620.3125, 10917.375, 11170.375, 11358.625, 11497.25, 11561.5625, 11625.6875, 11799.25, 11966.875, 12106.8125, 12228.5, 12337.375, 12393.0, 12446.125, 12557.4375, 12651.375, 12734.125, 12821.625, 12901.0, 12946.0625, 12989.625, 13067.4375, 13137.0, 13203.625, 13278.5, 13356.375, 13396.8125, 13433.5, 13511.6875, 13580.3125, 13643.8125, 13704.5, 13762.5, 13791.4375], [0.0, 0.3125, 0.75, 1.9375, 3.9375, 6.375, 7.8125, 10.5625, 17.0, 24.625, 34.1875, 47.125, 62.6875, 73.625, 87.5625, 118.75312499999995, 155.94218749999993, 195.625, 248.00312499999995, 313.9390625, 358.81562499999995, 410.3125, 492.00937499999986, 571.5124999999998, 670.1265625, 770.4437499999999, 894.75, 983.2515625, 1088.5781249999998, 1243.9468749999999, 1385.3359374999995, 1542.2078124999998, 1714.3968749999997, 1900.0015625, 2034.8765625, 2173.3765625, 2385.4624999999996, 2597.6984374999997, 2802.6390625, 3025.6984374999997, 3254.628125, 3419.215625, 3567.5812499999997, 3779.1359374999997, 4013.325, 4268.196875, 4484.8875, 4692.299999999999, 4831.189062499999, 4960.8234375, 5159.690625, 5438.6375, 5689.3796875, 5921.003125, 6090.226562499999, 6179.625, 6279.94375, 6509.190625, 6778.459374999999, 7061.1921875, 7276.6296875, 7420.9546875, 7500.8125, 7591.639062499999, 7817.4390625, 8089.4390625, 8341.284375, 8562.56875, 8711.3296875, 8795.25, 8895.1265625, 9257.4484375, 9662.625, 10014.128125, 10267.003125, 10436.4375, 10526.1890625, 10601.3765625, 10823.0078125, 11097.690625, 11331.946875, 11513.7640625, 11651.9390625, 11715.5015625, 11775.959375, 11943.6265625, 12098.19375, 12227.3234375, 12337.25, 12445.3125, 12500.8140625, 12551.6296875, 12656.81875, 12747.0, 12823.128125, 12909.378125, 12981.565625, 13026.0015625, 13070.1890625, 13145.190625, 13210.565625, 13270.3765625, 13345.6890625, 13418.3125, 13457.8125, 13491.9390625, 13566.1921875, 13632.1890625, 13691.6265625, 13747.2515625, 13801.4421875, 13831.0625]))</t>
+  </si>
+  <si>
+    <t>Add_Infected 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.25, 0.3125, 0.375, 0.9375, 0.9375, 1.0625, 1.875, 2.375, 3.3125, 4.5, 6.125, 7.75, 10.375, 14.435937500000007, 19.5625, 25.5625, 32.0625, 39.06093750000001, 41.3125, 47.0625, 58.5625, 65.5, 70.25, 78.0625, 84.62343750000001, 80.75, 82.4375, 98.06093750000001, 100.1875, 105.74843750000001, 108.4375, 113.0, 104.75, 104.8125, 117.4375, 119.5, 121.1875, 120.625, 118.8125, 109.5625, 106.3125, 121.75, 125.75, 126.8125, 124.375, 118.5, 109.125, 104.0, 125.5625, 127.625, 127.5625, 125.0625, 119.6875, 110.0625, 106.625, 126.5625, 127.8125, 127.75, 125.625, 120.3125, 111.0625, 110.0625, 129.25, 129.8125, 129.375, 127.875, 124.6875, 114.6875, 107.6875, 128.0625, 128.4375, 127.0, 125.0625, 120.25, 110.4375, 103.75, 124.125, 122.4375, 118.4375, 115.0, 112.3125, 103.9375, 96.1875, 110.4375, 105.25, 100.4375, 99.3125, 98.375, 90.8125, 84.125, 95.8125, 92.56093750000001, 89.5625, 94.125, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">95.6875, 88.4375, 81.9375, 93.5625, 92.0625, 87.25, 84.625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.4375, 0.5, 0.5625, 0.625, 1.25, 1.25, 1.5, 2.3125, 3.0625, 4.25, 5.875, 8.0, 10.3125, 14.0625, 19.4375, 26.375, 33.1875, 40.4375, 48.4375, 50.6875, 56.0, 68.375, 74.9375, 79.5, 87.0625, 92.4375, 88.0, 88.75, 103.8125, 105.8125, 110.1875, 112.1875, 115.6875, 107.125, 106.875, 118.6875, 121.5, 122.875, 121.625, 119.875, 110.5625, 108.0625, 123.0, 126.3125, 127.3125, 125.0, 119.8125, 110.1875, 105.75, 126.0, 128.0, 127.875, 125.625, 120.6875, 111.0, 108.3125, 127.0, 128.0, 127.9375, 126.1875, 121.3125, 111.8125, 111.4375, 129.5, 129.9375, 129.625, 128.25, 125.3125, 115.3125, 109.125, 128.25, 128.8125, 127.625, 125.75, 121.5625, 111.6875, 104.875, 125.0625, 123.625, 120.125, 117.0, 114.3125, 105.4375, 97.625, 112.5, 107.8125, 103.375, 101.875, 100.5625, 92.8125, 85.875, 98.6875, 94.6875, 92.625, 96.5, 98.75, 91.125, 84.375, 96.4375, 94.375, 89.5, 87.25], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.6875, 0.75, 0.8125, 0.875, 1.5625, 1.5625, 1.9375, 2.75, 3.75, 5.25, 7.3125, 9.9375, 12.814062499999977, 17.8125, 24.4375, 33.125, 40.5, 49.0625, 57.8125, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.8125, 65.0625, 78.00156249999998, 84.25, 88.50156249999998, 95.0625, 99.9375, 94.81406249999998, 94.875, 109.00156249999998, 111.4375, 114.4375, 115.75, 118.06406249999998, 109.1875, 109.0, 119.875, 123.4375, 124.4375, 122.625, 121.0, 111.5625, 109.75, 124.25, 126.875, 127.75, 125.625, 121.0625, 111.25, 107.6875, 126.4375, 128.3125, 128.1875, 126.1875, 121.625, 111.8125, 109.9375, 127.4375, 128.1875, 128.125, 126.6875, 122.375, 112.5625, 112.875, 129.75, 130.0, 129.875, 128.625, 125.9375, 115.9375, 110.6875, 128.5, 129.1875, 128.1875, 126.375, 122.875, 112.875, 106.0625, 125.9375, 124.75, 121.75156249999998, 118.9375, 116.12656249999998, 107.0625, 99.125, 114.4375, 110.0, 106.375, 104.5, 102.625, 94.625, 87.5625, 101.5625, 96.6875, 95.625, 98.8125, 101.5625, 93.5625, 86.6875, 99.375, 96.9375, 91.8125, 89.9375]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.25, 0.6875, 0.875, 1.25, 2.0625, 2.875, 3.875, 5.5625, 7.125, 9.8125, 11.4375, 13.375, 16.9375, 20.9375, 23.5, 27.3125, 31.37343750000001, 31.5625, 32.125, 37.9375, 41.4375, 44.5625, 47.0, 50.375, 48.0625, 47.125, 52.4375, 55.4375, 57.375, 57.5625, 56.9375, 52.875, 49.6875, 54.9375, 58.875, 60.75, 60.0, 57.0625, 52.5625, 49.0625, 55.5625, 59.0, 60.375, 59.25, 56.4375, 51.75, 48.6875, 55.125, 58.0, 59.0, 58.5, 55.4375, 51.1875, 48.375, 55.5, 58.625, 59.125, 58.625, 56.75, 52.0625, 48.3125, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">54.125, 56.4375, 56.5, 55.25, 52.75, 48.75, 45.1875, 50.1875, 51.375, 49.75, 47.5625, 45.875, 42.4375, 39.3125, 41.625, 40.0, 38.0, 36.5625, 35.625, 33.4375, 31.25, 32.75, 31.8125, 30.875, 31.6875, 32.375, 30.625, 28.875, 30.8125, 30.75, 29.25, 28.1875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.5, 1.0625, 1.3125, 1.8125, 2.8125, 3.9375, 5.3125, 7.4375, 9.6875, 12.9375, 15.1875, 17.375, 21.6875, 25.8125, 28.6875, 32.4375, 36.5, 36.1875, 36.3125, 42.0625, 45.625, 48.4375, 50.5625, 52.9375, 50.0625, 48.8125, 53.5625, 56.875, 58.8125, 58.6875, 57.5625, 53.4375, 50.3125, 55.5, 59.375, 61.125, 60.4375, 57.5625, 53.0, 49.5, 55.875, 59.25, 60.625, 59.5625, 56.875, 52.1875, 49.0, 55.3125, 58.125, 59.0625, 58.875, 55.9375, 51.5625, 48.8125, 55.8125, 58.8125, 59.3125, 58.8125, 57.125, 52.5, 48.75, 54.375, 56.6875, 56.9375, 55.6875, 53.4375, 49.375, 45.75, 50.75, 52.125, 50.75, 48.6875, </t>
+  </si>
+  <si>
+    <t>47.0, 43.4375, 40.1875, 42.75, 41.3125, 39.4375, 37.9375, 36.75, 34.5, 32.25, 33.9375, 32.9375, 32.125, 32.8125, 33.8125, 31.875, 29.9375, 32.0625, 31.875, 30.375, 29.1875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.5625, 0.75, 1.4375, 1.75, 2.3125, 3.625, 5.0625, 6.8125, 9.4375, 12.3125, 16.3125, 19.0, 21.4375, 26.4375, 30.625, 34.0, 37.625, 41.375, 40.875, 40.375, 46.0625, 49.75, 52.375, 53.75, 55.375, 51.9375, 50.25, 54.5625, 58.25, 60.1875, 59.75, 58.1875, 54.0, 50.875, 56.0625, 59.875, 61.5, 60.875, 58.0625, 53.5, 49.9375, 56.1875, 59.5, 60.875, 59.8125, 57.25, 52.625, 49.375, 55.5625, 58.3125, 59.1875, 59.1875, 56.4375, 52.0, 49.3125, 56.125, 59.0, 59.5625, 59.0, 57.5, 52.9375, 49.1875, 54.625, 56.875, 57.3125, 56.1875, 54.125, 50.0625, 46.375, 51.3125, 52.8125, 51.6875, 49.8125, 48.0, 44.375, 41.0625, 43.875, 42.4375, 40.81406249999998, 39.3125, 37.8125, 35.5625, 33.1875, 35.1875, 34.0, 33.375, 34.0, 35.1875, 33.125, 31.0, 33.375, 33.0, 31.5, 30.1875]), ([0.0, 0.3125, 0.875, 1.9375, 3.875, 7.498437500000007, 9.875, 12.375, 20.25, 29.75, 39.49843750000001, 51.93437500000002, 71.24843750000001, 83.8125, 97.8125, 131.0609375, 169.8734375, 213.74687500000002, 272.684375, 337.93125000000003, 385.5625, 445.92656250000005, 523.11875, 613.30625, 713.6171875, 819.4328125000001, 937.740625, 1043.5, 1143.934375, 1294.1875, 1454.9906250000001, 1606.6671875000002, 1787.6640625, 1974.4984375, 2115.665625, 2258.5546875, 2478.996875, 2668.5578125, 2889.4890625000003, 3106.7625000000003, 3341.7156250000003, 3482.5, 3640.9359375, 3885.359375, 4116.996875, 4362.4296875, 4596.559375, 4784.4171875, 4923.8640625, 5043.9953125, 5251.246875, 5507.4953125, 5789.6734375, 6016.782812500001, 6180.61875, 6262.9296875, 6363.6234375, 6591.8, 6865.36875, 7131.1765625, 7351.1828125, 7499.7375, 7582.371875, 7677.121875, 7907.4859375, 8173.8078125, 8429.3953125, 8647.9125, 8792.5609375, 8866.3671875, 8970.0625, 9330.5609375, 9731.2953125, 10049.0609375, 10307.1875, 10478.0578125, 10546.7484375, 10633.0625, 10861.68125, 11137.9953125, 11366.1796875, 11544.3640625, 11679.928125, 11742.7484375, 11801.68125, 11968.4046875, 12117.5609375, 12255.61875, 12371.9359375, 12476.36875, 12526.121875, 12583.11875, 12682.4375, 12767.8109375, 12845.059375, 12924.3703125, 12997.9171875, 13041.1171875, 13080.5, 13150.1859375, 13213.3109375, 13274.621875, 13345.309375, 13417.934375, 13457.6171875, 13490.684375, 13559.809375, 13624.9359375, 13679.4375, 13733.3078125, 13787.5625, 13813.434375], [0.0, 0.6875, 1.5625, 2.9375, 5.625, 9.9375, 13.125, 16.875, 27.0, 37.9375, 51.0625, 68.5, 91.25, 106.0, 124.75, 165.75, 213.1875, 267.0625, 335.3125, 415.875, 471.0, 541.0625, 637.1875, 747.875, 860.25, 985.1875, 1126.4375, 1236.6875, 1352.0625, 1520.5625, 1693.75, 1864.9375, 2056.375, 2257.1875, 2407.625, 2552.3125, 2768.75, 2981.375, 3203.5625, 3422.0625, 3653.5, 3800.75, 3950.375, 4171.6875, 4417.875, 4667.625, 4888.1875, 5082.8125, 5193.75, 5311.5, 5523.8125, 5787.375, 6064.0625, 6286.875, 6445.8125, 6528.1875, 6620.125, 6846.25, 7125.375, 7395.6875, 7604.125, 7754.9375, 7831.4375, 7924.75, 8154.5, 8413.6875, 8665.75, 8870.5625, 9016.3125, 9094.375, 9190.5625, 9547.5625, 9926.1875, 10249.4375, 10486.875, 10655.6875, 10725.6875, 10800.8125, 11028.5625, 11289.75, 11505.0, 11674.6875, 11803.6875, 11859.75, 11921.9375, 12081.1875, 12229.0625, 12353.5625, 12463.4375, 12564.3125, 12619.5, 12669.5625, 12767.0, 12849.5625, 12923.625, 12995.875, 13066.3125, 13107.0, 13145.875, 13215.1875, 13275.3125, 13333.625, 13399.75, 13471.1875, 13507.25, 13538.3125, 13606.3125, 13668.25, 13720.625, 13772.75, 13824.875, 13848.75], [0.0, 1.125, 2.3125, 4.0, 7.5625, 12.5625, 16.6875, 21.6875, 34.1875, 46.87656249999998, 63.6875, 86.4375, 112.75, 129.68906249999998, 151.69062499999995, 200.94062499999995, 258.0640625, 320.0749999999998, 402.31562499999995, 496.44062499999995, 561.128125, 643.4375, 754.8249999999998, 883.628125, 1007.3843749999999, 1151.3937499999997, 1321.5187499999997, 1438.25, 1566.0, 1741.3171874999998, 1943.4515625, 2126.8828125, 2332.440625, 2539.45, 2709.8796875, 2856.375, 3075.253125, 3287.6562499999995, 3514.2609374999997, 3738.546874999999, 3962.8328125, 4112.393749999999, 4244.928124999999, 4458.003125, 4721.628125, 4967.2078125, 5194.2515625, 5365.5671875, 5467.3984375, 5575.7578125, 5804.9390625, 6056.0625, 6336.1890625, 6555.1296875, 6714.69375, 6793.328125, 6873.128125, 7105.1953125, 7381.7109375, 7652.0640625, 7864.9375, 8011.259375, 8082.384375, 8177.0078125, 8396.8234375, 8661.0015625, 8909.65625, 9104.1328125, 9244.00625, 9318.6328125, 9414.628125, 9763.4390625, 10125.0671875, 10438.5671875, 10672.1328125, 10833.6921875, 10902.1875, 10969.0671875, 11189.3125, 11438.1265625, 11641.5015625, 11803.8203125, 11929.19375, 11979.5640625, 12043.00625, 12197.2515625, 12337.9421875, 12454.0046875, 12556.946875, 12656.628125, 12709.0, 12757.128125, 12852.1953125, 12926.31875, 12998.003125, 13065.3828125, 13132.503125, 13172.9515625, 13209.9390625, 13276.0015625, 13334.0, 13388.875, 13453.3765625, 13522.63125, 13555.4390625, 13586.0015625, 13650.253125, 13707.8140625, 13760.5015625, 13809.6890625, 13859.0015625, 13881.5640625]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.875, 0.875, 1.1875, 1.75, 2.125, 2.75, 3.6875, 5.125, 7.0, 9.8125, 13.75, 18.24843750000001, 24.3125, 33.25, 41.8125, 50.3125, 58.4375, 67.875, 69.06093750000001, 73.75, 88.37343750000001, 91.56093750000001, 96.125, 100.74843750000001, 105.1875, 98.25, 97.5, 110.125, 113.75, 116.0625, 117.375, 115.6875, 107.25, 103.0625, 119.5625, 123.3125, 123.5625, 122.375, 116.875, 107.875, 101.6875, 123.5, 126.8125, 127.25, 124.3125, 117.0625, 107.875, 103.75, 125.875, 127.6875, 128.0, 125.1875, 119.0, 109.3125, 104.625, 126.25, 127.5, 127.3125, 124.625, 119.3125, 109.5, 109.75, 129.0, 129.3125, 128.8125, 127.125, 123.0625, 113.125, 104.8125, 127.0625, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.0625, 125.625, 122.875, 118.1875, 108.9375, 101.1875, 121.62343750000001, 118.3125, 113.3125, 111.875, 109.0625, 100.5625, 93.25, 105.0, 100.375, 96.5625, 93.5, 91.9375, 85.0625, 79.0625, 91.25, 86.56093750000001, 85.25, 87.625, 89.8125, 83.24843750000001, 77.5625, 88.5, 84.625, 82.0, 78.125], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.1875, 0.1875, 0.1875, 0.5625, 1.0625, 1.125, 1.5625, 2.1875, 2.6875, 3.5, 4.75, 6.6875, 9.125, 12.75, 17.8125, 23.5625, 31.5625, 41.875, 51.375, 60.125, 68.75, 78.4375, 78.5, 83.5625, 97.5625, 100.5, 102.8125, 107.0625, 110.9375, 103.375, 102.0, 113.625, 117.875, 119.9375, 119.6875, 117.5625, 108.75, 105.125, 120.8125, 124.6875, 125.125, 123.375, 117.9375, 109.0, 103.4375, 124.5, 127.3125, 127.5625, 124.875, 118.3125, 108.9375, 105.125, 126.5, 128.0, 128.0625, 125.8125, 120.0, 110.3125, 106.1875, 126.75, 127.75, 127.625, 125.3125, 120.4375, 110.5625, 110.6875, 129.1875, 129.5625, 129.0625, 127.5625, 124.125, 114.0, 105.8125, 127.5, 127.625, 126.25, 123.9375, 119.625, 110.25, 102.1875, 122.6875, 119.8125, 115.5, 113.5625, 110.9375, 102.125, 94.75, 107.6875, 103.1875, 99.0, 96.0, 94.75, 87.5625, 81.375, 94.8125, 89.8125, 88.0625, 89.5, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">93.3125, 86.3125, 80.25, 91.1875, 87.125, 84.375, 80.6875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.375, 0.375, 0.375, 0.8125, 1.25, 1.375, 1.9375, 2.625, 3.3125, 4.3125, 5.9375, 8.25, 11.375, 15.876562499999977, 22.125, 29.3125, 39.12656249999998, 50.8125, 61.06406249999998, 69.68906249999998, 79.0, 88.625, 86.93906249999998, 92.375, 105.75, 108.12656249999998, 108.9375, 112.6875, 115.31406249999998, 107.375, 105.375, 116.375, 121.12656249999998, 122.625, 121.625, 119.125, 110.125, 107.25, 122.125, 125.8125, 126.3125, 124.25, 118.9375, 110.25, 105.4375, 125.375, 127.8125, 127.8125, 125.4375, 119.6875, 110.125, 106.5, 127.0, 128.3125, 128.1875, 126.375, 121.125, 111.3125, 107.8125, 127.1875, 127.9375, 127.875, 125.9375, 121.5625, 111.625, 111.8125, 129.375, 129.8125, 129.3125, 128.0, 125.125, 114.875, 106.75, 127.875, 128.1875, 126.875, 124.9375, 121.0, 111.4375, 103.18906249999998, 123.8125, 121.25, 117.8125, 115.1875, 112.8125, 103.6875, 96.3125, 110.3125, 105.875, 101.5625, 98.68906249999998, 97.625, 90.1875, 83.6875, 98.25, 93.0625, 90.875, 91.3125, 96.8125, 89.375, 83.0, 94.0625, 89.8125, 87.0625, 83.625]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.4375, 0.6875, 1.25, 1.75, 2.8125, 3.5625, 4.875, 7.125, 9.5625, 12.6875, 16.5625, 20.75, 23.5, 26.4375, 32.1875, 36.5, 39.25, 42.1875, 45.75, 44.25, 43.375, 47.875, 51.75, 54.12343750000001, 55.4375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.1875, 51.75, 49.5, 54.5, 58.375, 59.6875, 59.5625, 56.9375, 52.75, 49.1875, 55.3125, 59.5625, 61.1875, 60.25, 56.5, 52.125, 48.4375, 55.5, 59.125, 60.375, 59.4375, 56.0, 51.6875, 48.0625, 54.625, 57.8125, 58.5, 57.5625, 54.625, 50.4375, 47.6875, 55.25, 58.125, 58.8125, 58.0, 55.75, 51.375, 47.5625, 53.3125, 55.3125, 55.4375, 53.75, 51.3125, 47.375, 44.0, 48.6875, 48.875, 46.625, 45.12343750000001, 43.3125, 40.25, 37.375, 38.5625, 37.375, 35.625, 33.6875, 32.6875, 30.68593750000001, 28.875, 30.25, 29.0625, 28.375, 28.5625, 29.5, 28.0625, 26.4375, 28.25, 27.5, 26.5, 25.1875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.125, 0.375, 0.75, 1.0625, 1.6875, 2.375, 3.625, 4.75, 6.5, 9.375, 12.75, 16.5, 20.8125, 25.75, 28.5625, 31.6875, 37.9375, 42.25, 44.5625, 47.4375, 50.3125, 48.25, 46.75, 50.9375, 54.875, 57.375, 57.875, 57.0625, 53.1875, 50.1875, 55.25, 59.375, 60.875, 60.375, 57.5, 53.3125, 49.5625, 55.8125, 59.9375, 61.5, 60.5625, 57.0625, 52.5625, 48.8125, 55.75, 59.3125, 60.625, 59.75, 56.5, 52.0625, 48.5, 54.875, 57.9375, 58.75, 58.0, 55.1875, 50.9375, 48.125, 55.5, 58.375, 59.0, 58.3125, 56.3125, 51.875, 48.0, 53.6875, 55.75, 55.8125, 54.4375, 52.0, 48.0, 44.5625, 49.3125, 49.6875, 47.8125, 46.0625, 44.3125, 41.1875, 38.1875, 39.8125, 38.8125, 36.875, 34.875, 33.9375, 31.8125, 29.9375, 31.8125, 30.625, 29.75, 29.5625, 31.0, 29.375, 27.625, 29.5, 28.6875, 27.625, 26.25], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.3125, 0.625, 1.0625, 1.5, 2.125, 3.0625, 4.5625, 6.125, 8.3125, 11.9375, 16.0625, 20.3125, 25.3125, 30.9375, 33.31406249999998, 36.8125, 43.4375, 47.5625, 49.375, 52.0, 54.125, 51.50156249999998, 49.3125, 53.25, 57.375, 59.8125, 59.75, 58.375, 54.25, 50.8125, 55.875, 60.1875, 61.8125, 61.0625, 58.0, 53.875, 49.9375, 56.25, 60.3125, 61.75, 60.8125, 57.6875, 53.0625, 49.25, 55.9375, 59.5625, 60.875, 60.0625, 57.0, 52.5, 48.9375, 55.125, 58.0, 58.9375, 58.4375, 55.75, 51.375, 48.6875, 55.8125, 58.625, 59.1875, 58.625, 56.875, 52.375, 48.4375, 54.0, 56.1875, 56.1875, 55.125, 52.6875, 48.6875, 45.125, 49.9375, 50.5, 49.0625, 47.0625, 45.3125, 42.125, 39.0625, 41.0625, 40.3125, 38.25, 36.1875, 35.25, 33.0625, 31.0, 33.375, 32.125, 31.0625, 30.5, 32.4375, 30.6875, 28.8125, 30.814062499999977, 30.0625, 28.9375, 27.4375]), ([0.0, 0.8125, 1.8125, 4.810937500000007, 10.5, 17.0, 21.3125, 26.5625, 39.56093750000001, 57.75, 78.0625, 102.12343750000001, 134.5, 158.5609375, 185.4359375, 240.9375, 311.246875, 387.86406250000005, 482.6859375, 598.1875, 679.8734375, 768.0578125000001, 902.246875, 1037.80625, 1210.425, 1360.4875, 1550.6109375, 1685.5578125, 1831.1625000000001, 2043.0578125, 2237.471875, 2448.30625, 2640.625, 2863.1859375, 3017.4187500000003, 3164.540625, 3367.0281250000003, 3583.6828125, 3824.8625, 4034.746875, 4241.246875, 4388.3046875, 4510.1796875, 4710.3359375, 4950.6640625, 5188.9859375, 5402.778125, 5588.400000000001, 5688.375, 5764.564062500001, 5987.684375, 6260.234375, 6522.9359375, 6734.840625, 6890.0578125, 6970.1734375, 7062.7484375, 7282.4359375, 7559.9359375, 7823.4984375, 8025.2765625, 8187.734375, 8252.4296875, 8342.5578125, 8562.6828125, 8810.48125, 9047.85625, 9245.6609375, 9375.7359375, 9437.575, 9551.3, 9902.010937500001, 10252.6828125, 10551.984375, 10776.621875, 10945.425, 11017.5578125, 11081.9921875, 11294.4359375, 11524.8078125, 11719.6203125, 11881.8109375, 12002.228125, 12061.1765625, 12114.93125, 12263.1859375, 12390.8078125, 12506.553125, 12607.0609375, 12698.9359375, 12747.6171875, 12799.0609375, 12891.0625, 12965.9375, 13034.4328125, 13101.990625, 13165.6140625, 13202.5609375, 13234.9953125, 13306.859375, 13359.2421875, 13414.05625, 13470.0625, 13533.3703125, 13567.184375, 13602.1859375, 13662.6859375, 13721.4984375, 13771.1875, 13815.6875, 13865.0609375, 13887.7484375], [0.0, 1.4375, 3.0625, 6.9375, 14.625, 22.375, 27.5, 34.5, 51.6875, 72.5625, 97.5625, 127.8125, 166.375, 195.4375, 227.75, 297.125, 375.125, 467.0, 582.5, 718.0625, 809.375, </t>
+  </si>
+  <si>
+    <t>917.375, 1072.4375, 1235.3125, 1407.375, 1587.8125, 1790.5, 1942.0, 2099.1875, 2328.75, 2546.375, 2752.75, 2967.5625, 3191.5625, 3339.625, 3483.625, 3685.6875, 3918.5, 4160.3125, 4380.6875, 4573.6875, 4685.8125, 4800.1875, 5001.8125, 5252.8125, 5504.375, 5721.0, 5879.75, 5964.6875, 6053.625, 6273.9375, 6545.0625, 6814.875, 7022.625, 7163.6875, 7241.1875, 7327.9375, 7557.0, 7827.9375, 8094.5625, 8298.75, 8437.9375, 8512.0, 8595.0625, 8810.9375, 9056.125, 9288.8125, 9473.8125, 9610.8125, 9679.9375, 9773.75, 10113.6875, 10449.5625, 10744.5625, 10959.625, 11115.0, 11180.375, 11243.375, 11449.25, 11667.375, 11848.6875, 12002.1875, 12122.6875, 12179.75, 12234.625, 12375.125, 12497.875, 12603.25, 12700.625, 12790.9375, 12838.1875, 12889.25, 12974.4375, 13048.125, 13112.8125, 13174.8125, 13236.125, 13271.0, 13305.9375, 13369.5, 13419.875, 13471.6875, 13526.375, 13588.75, 13620.625, 13652.0625, 13711.3125, 13762.8125, 13811.1875, 13852.0, 13897.625, 13919.6875], [0.0, 2.0625, 4.5, 9.3125, 19.125, 28.0, 33.93906249999998, 43.375, 64.6875, 87.6875, 117.81718749999993, 155.06562499999995, 198.9375, 233.06406249999998, 272.69062499999995, 353.8140625, 443.9390625, 549.3796874999999, 683.628125, 846.2015624999998, 949.2546874999999, 1066.56875, 1236.8265625, 1425.3218749999999, 1614.4499999999998, 1811.8859374999997, 2031.5749999999998, 2192.003125, 2375.2, 2604.1953125, 2835.203125, 3047.06875, 3272.2515625, 3497.3765625, 3638.5125, 3776.6265625, 3978.6875, 4220.826562499999, 4464.3859375, 4682.375, 4860.6921875, 4958.696875, 5067.331249999999, 5259.9421875, 5530.2703125, 5790.128125, 5992.5734375, 6143.576562499999, 6220.8234375, 6310.576562499999, 6520.9421875, 6802.2546875, 7081.878125, 7281.5640625, 7410.3328125, 7482.0109375, 7566.06875, 7799.440625, 8068.7515625, 8337.1921875, 8531.6921875, 8664.6890625, 8743.1265625, 8824.753125, 9033.64375, 9279.2, 9509.9515625, 9677.196875, 9815.08125, 9886.33125, 9981.5765625, 10307.6875, 10633.0671875, 10912.1328125, 11116.628125, 11262.0125, 11326.075, 11389.56875, 11590.8265625, 11794.259375, 11970.8171875, 12112.6328125, 12231.4421875, 12285.75625, 12344.753125, 12479.628125, 12596.75625, 12695.0109375, 12788.6875, 12872.75, 12921.1890625, 12970.690625, 13054.0625, 13121.5, 13181.6328125, 13242.38125, 13298.3140625, 13333.065625, 13366.065625, 13425.5640625, 13473.75, 13522.63125, 13576.3140625, 13637.3765625, 13667.125, 13697.1890625, 13753.1265625, 13801.6265625, 13847.196875, 13886.1265625, 13927.6890625, 13949.1265625]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.4375, 0.4375, 0.5625, 1.0, 1.1875, 1.8125, 2.375, 3.3125, 4.0, 5.3125, 7.3125, 10.5625, 14.5, 20.0, 27.625, 34.49843750000001, 44.625, 57.1875, 66.4375, 75.8125, 85.1875, 93.375, 91.125, 93.4375, 107.4375, 108.6875, 111.875, 114.0, 115.5625, 107.4375, 103.875, 116.0, 121.4375, 122.8125, 120.875, 116.625, 107.4375, 101.625, 120.5625, 126.0, 126.4375, 123.25, 115.3125, 106.125, 100.4375, 124.9375, 127.6875, 127.5, 124.5, 115.8125, 106.4375, 102.1875, 125.9375, 128.0, 127.4375, 125.0625, 117.4375, 108.0, 102.5, 126.0, 127.375, 126.9375, 124.4375, 117.875, 108.5625, 106.3125, 128.75, 129.0, 128.4375, 126.4375, 121.75, 111.75, 103.6875, 126.5625, 126.37343750000001, 123.875, 121.625, 117.0625, 107.8125, 99.9375, 119.25, 113.5, 111.8125, 107.3125, 104.5, 96.4375, 89.625, 102.4375, 97.3125, 94.5625, 90.875, 89.0, 82.4375, 76.875, 84.4375, 81.625, 83.3125, 84.625, 87.125, 80.8125, 75.1875, 86.0625, 81.9375, 77.43593750000001, 73.75], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.375, 0.6875, 0.6875, 0.8125, 1.1875, 1.4375, 2.125, 2.8125, 3.875, 4.875, 6.375, 8.875, 12.625, 17.25, 23.375, 31.4375, 38.8125, 49.9375, 63.25, 72.75, 81.875, 90.5, 98.5, 95.5, 96.75, 110.125, 111.375, 114.4375, 115.625, 116.75, 108.5, 105.25, 117.0625, 122.25, 123.875, 122.0625, 118.125, 108.75, 103.1875, 122.0625, 126.4375, 126.9375, 124.0, 116.3125, 107.0, 102.0625, 125.875, 127.9375, 127.75, 125.0625, 116.9375, 107.4375, 104.0625, 126.5625, 128.1875, 127.6875, 125.625, 118.0, 108.5, 103.8125, 126.375, 127.625, 127.25, 125.0625, 118.8125, 109.375, 108.125, 128.9375, 129.125, 128.6875, 127.0, 122.625, 112.6875, 104.625, 126.9375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">126.875, 124.8125, 122.5625, 118.25, 108.875, 100.8125, 120.5625, 115.4375, 113.0625, 109.0625, 106.375, 98.0625, 91.25, 104.6875, 99.1875, 96.5, 93.1875, 91.0625, 84.375, 78.375, 87.5625, 83.9375, 85.75, 87.75, 89.125, 82.625, 76.75, 88.3125, 84.1875, 78.9375, 75.625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.625, 0.875, 0.875, 1.0625, 1.375, 1.75, 2.5, 3.3125, 4.5625, 6.0, 7.6875, 10.8125, 15.189062499999977, 20.625, 27.25, 35.875, 43.37656249999998, 55.75, 69.75156249999998, 79.125, 87.93906249999998, 95.8125, 103.75, 99.8125, 100.0625, 112.75, 114.1875, 116.9375, 117.25, 117.9375, 109.5625, 106.625, 118.125, 123.0625, 124.875, 123.125, 119.5625, 110.0625, 104.875, 123.4375, 126.875, 127.375, 124.75, 117.3125, 107.875, 104.0, 126.5, 128.1875, 127.9375, 125.625, 118.1875, 108.5625, 106.25, 127.0625, 128.375, 127.875, 126.1875, 118.5625, 108.9375, 105.3125, 126.75, 127.875, 127.5625, 125.625, 119.75, 110.1875, 109.9375, 129.125, 129.3125, 128.875, 127.5, 123.5, 113.5625, 105.5, 127.25, 127.375, 125.625, 123.4375, 119.5, 109.9375, 101.75, 121.875, 117.25, 114.1875, 110.75, 108.125, 99.5625, 92.75, 106.875, 101.125, 98.43906249999998, 95.50156249999998, 92.9375, 86.1875, 79.8125, 90.375, 86.0625, 88.3125, 90.625, 91.1875, 84.43906249999998, 78.375, 90.625, 86.1875, 80.5, 77.5625]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.25, 0.5, 1.0, 1.25, 1.8125, 2.6875, 3.875, 5.6875, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.4375, 10.25, 14.1875, 18.8125, 23.0625, 28.125, 33.625, 36.1875, 38.3125, 44.75, 48.3125, 51.1875, 53.4375, 55.18593750000001, 51.9375, 49.375, 53.375, 57.625, 59.9375, 59.8125, 57.625, 53.375, 49.4375, 55.25, 59.9375, 61.9375, 60.8125, 56.75, 52.4375, 48.8125, 55.875, 60.1875, 61.625, 60.5, 56.1875, 51.75, 48.25, 55.4375, 59.125, 60.3125, 59.375, 55.4375, 51.1875, 47.3125, 54.1875, 57.625, 58.625, 57.375, 54.25, 50.125, 47.0, 54.75, 57.8125, 58.625, 57.4375, 54.8125, 50.625, 46.875, 52.75, 55.0, 54.375, 52.75, 50.5, 46.6875, 43.25, 47.375, 46.25, 45.0625, 42.625, 40.9375, 38.125, 35.375, 36.875, 35.5, 34.25, 32.625, 31.375, 29.5, 27.875, 28.4375, 27.3125, 27.1875, 27.25, 28.5625, 27.0, 25.375, 27.125, 26.5625, 24.875, 23.6875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.5, 0.75, 1.125, 1.625, 2.25, 3.25, 4.6875, 6.75, 8.8125, 11.9375, 16.25, 21.3125, 26.125, 31.4375, 37.25, 39.5625, 41.0, 47.1875, 50.6875, 53.5, 55.1875, 56.375, 52.875, 50.0625, 54.0, 58.25, 60.6875, 60.625, 58.375, 54.125, 50.125, 55.875, 60.3125, 62.1875, 61.25, 57.1875, 52.875, 49.125, 56.3125, 60.5, 61.8125, 60.8125, 56.6875, 52.1875, 48.6875, 55.8125, 59.375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">60.5625, 59.6875, 55.75, 51.5, 47.6875, 54.4375, 57.8125, 58.8125, 57.8125, 54.625, 50.5, 47.375, 55.0, 57.9375, 58.8125, 57.75, 55.375, 51.0625, 47.3125, 53.0, 55.375, 54.875, 53.3125, 51.125, 47.1875, 43.6875, 48.1875, 47.3125, 45.8125, 43.4375, 41.75, 38.875, 36.0625, 37.9375, 36.4375, 35.0625, 33.5, 32.1875, 30.25, 28.5, 29.25, 28.0625, 28.0625, 28.5, 29.4375, 27.8125, 26.0625, 28.0, 27.375, 25.625, 24.4375], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0,0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.0, 0.0, 0.1875, 0.75, 1.0, 1.375, 2.0625, 2.75, 4.0625, 5.75, 8.0625, 10.4375, 13.8125, 18.5, 23.9375, 29.5, 35.0, 40.87656249999998, 42.93906249999998, 43.75, 49.5625, 53.0625, 55.75, 56.9375, 57.5625, 53.8125, 50.75, 54.625, 58.875, 61.4375, 61.375, 59.125, 54.9375, 50.75, 56.4375, 60.6875, 62.4375, 61.75, 57.625, 53.3125, 49.5, 56.6875, 60.75, 62.0, 61.125, 57.1875, 52.625, 49.1875, 56.125, 59.625, 60.8125, 59.9375, 56.0, 51.75, 48.0, 54.6875, 58.0, 59.0, 58.25, 55.0, 50.875, 47.75, 55.25, 58.0, 59.0, 58.0625, 55.875, 51.5, 47.75, 53.25, 55.6875, 55.3125, 53.875, 51.75, 47.6875, 44.1875, 48.9375, 48.3125, 46.5625, 44.1875, 42.5, 39.5625, 36.6875, 38.875, 37.3125, 35.8125, 34.375, 32.9375, 30.9375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.0625, 30.0625, 28.8125, 28.9375, 29.6875, 30.375, 28.6875, 26.75, 28.8125, 28.1875, 26.375, 25.1875]), ([0.0, 2.0, 4.8125, 11.0625, 21.1875, 33.81093750000001, 42.9375, 53.75, 77.5625, 102.6875, 135.75, 175.6875, 228.0, 259.4359375, 301.1875, 393.8125, 486.9375, 600.3125, 734.746875, 902.121875, 1017.496875, 1145.434375, 1328.1234375, 1522.18125, 1717.8015625, 1933.99375, 2156.4171875, 2325.434375, 2484.6171875, 2715.684375, 2942.1109375, 3167.4984375, 3393.309375, 3614.6828125, 3754.4328125, 3896.246875, 4085.55, 4323.1078125, 4570.2484375, 4785.3671875, 4963.30625, 5060.6875, 5160.434375, 5363.61875, 5622.984375, 5892.6171875, 6105.61875, 6248.1875, 6320.1078125, 6405.8078125, 6640.8671875, 6928.9296875, 7197.8703125, 7402.1875, 7534.434375, 7603.0, 7681.8046875, 7906.809375, 8177.4875, 8433.625, 8633.371875, 8757.053125, 8828.25, 8904.1234375, 9118.125, 9353.1234375, 9578.5, 9767.309375, 9892.9375, 9962.875, 10050.74375, 10375.8078125, 10688.5609375, 10954.25, 11161.184375, 11308.5578125, 11369.0, 11431.61875, 11626.559375, 11829.7484375, 11999.8703125, 12146.1875, 12261.2453125, 12317.7484375, 12367.2484375, 12502.8125, 12609.8125, 12707.75, 12792.746875, 12875.3078125, 12923.9359375, 12970.8734375, 13050.5578125, 13115.3125, 13176.4921875, 13232.2453125, 13289.371875, 13320.25, 13353.371875, 13405.3109375, 13451.9984375, 13503.4984375, 13557.9984375, 13611.9359375, 13641.5, 13670.6171875, 13725.9984375, 13775.9359375, 13814.3109375, 13852.375, 13892.7484375, 13916.6875], [0.0, 2.8125, 6.0, 13.375, 24.3125, 38.0625, 48.875, 61.1875, 87.75, 115.5, 152.1875, 196.5, 252.875, 290.375, 334.8125, 434.0, 537.9375, 659.9375, 809.625, 991.375, 1110.625, 1246.4375, 1449.875, 1652.3125, 1862.3125, 2081.5625, 2315.0625, 2489.3125, 2654.375, 2889.6875, 3112.9375, 3343.125, 3564.125, 3779.875, 3917.75, 4047.0625, 4237.0625, 4472.3125, 4722.3125, 4938.5625, 5112.5, 5201.1875, 5293.5, 5496.9375, 5754.4375, 6024.375, 6236.25, 6373.75, 6444.3125, 6527.5625, 6765.0625, 7050.9375, 7321.9375, 7525.3125, 7648.9375, 7717.5625, 7798.9375, 8026.4375, 8298.3125, 8551.25, 8747.125, 8870.1875, 8940.5, 9018.0, 9227.4375, 9463.4375, 9687.25, 9869.4375, 9994.625, 10065.5625, 10152.125, 10476.6875, 10782.625, 11047.0625, 11248.6875, 11391.75, 11451.0, 11512.6875, 11708.375, 11905.25, 12068.3125, 12209.125, 12323.625, 12382.25, 12432.4375, 12561.875, 12664.625, 12760.0, 12845.0625, 12924.875, 12971.8125, 13015.6875, 13093.875, 13156.3125, 13218.625, 13276.25, 13330.75, 13362.5625, 13393.8125, 13446.3125, 13491.3125, 13541.3125, 13594.3125, 13648.875, 13677.9375, 13705.625, 13760.5625, 13806.5625, 13845.0, 13881.9375, 13921.625, 13943.8125], [0.0, 3.625, 7.126562499999977, 16.0625, 27.5, 42.5625, 55.00156249999998, 69.43906249999998, 98.68906249999998, 130.0, 170.12656249999998, 219.125, 281.125, 324.0640625, 371.1875, </t>
+  </si>
+  <si>
+    <t>479.6875, 592.628125, 727.6359374999998, 895.878125, 1088.4421874999998, 1213.440625, 1363.065625, 1574.5640625, 1792.63125, 2010.1890625, 2242.4453125, 2483.753125, 2668.878125, 2827.1296875, 3070.7703125, 3299.6921875, 3528.4593749999995, 3753.5, 3957.1921875, 4085.753125, 4204.389062499999, 4392.565625, 4618.8796875, 4877.06875, 5091.7515625, 5256.3140625, 5336.6265625, 5430.706249999999, 5635.9484375, 5893.671874999999, 6160.571875, 6373.196875, 6502.440625, 6573.5625, 6655.1265625, 6897.075, 7177.4390625, 7443.5171875, 7647.8796875, 7770.7515625, 7837.003125, 7914.8234375, 8153.515625, 8419.503125, 8671.3140625, 8867.6359375, 8985.8828125, 9056.0015625, 9135.0765625, 9342.5046875, 9572.7640625, 9797.003125, 9974.6265625, 10096.7546875, 10170.3765625, 10262.190625, 10582.56875, 10888.8265625, 11140.628125, 11342.190625, 11477.5640625, 11536.0625, 11597.128125, 11793.4390625, 11979.3125, 12139.9390625, 12274.815625, 12391.628125, 12446.7515625, 12496.7515625, 12621.2546875, 12719.3125, 12814.7578125, 12896.3203125, 12974.3765625, 13018.6890625, 13060.0625, 13136.815625, 13198.1375, 13260.9390625, 13319.3171875, 13375.6890625, 13405.9375, 13436.5015625, 13489.19375, 13531.753125, 13580.0015625, 13631.8125, 13685.1265625, 13714.1921875, 13742.625, 13794.5015625, 13840.6875, 13878.253125, 13913.1265625, 13952.0015625, 13973.8140625]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.8125, 1.0, 1.0, 1.125, 1.8125, 2.3125, 3.3125, 4.625, 6.125, 7.9375, 11.125, 15.5, 21.5, 29.5625, 39.5625, 51.625, 59.5, 70.875, 85.5625, 94.25, 100.6875, 107.375, 113.3125, 108.0, 106.5, 114.5625, 116.875, 119.1875, 118.74843750000001, 117.4375, 108.125, 103.12343750000001, 115.4375, 124.1875, 125.4375, 121.625, 114.375, 105.3125, 99.5625, 122.1875, 126.4375, 126.5625, 122.1875, 113.6875, 104.75, 101.0, 125.3125, 127.625, 127.375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">124.4375, 115.6875, 106.625, 101.375, 126.375, 127.9375, 127.4375, 124.3125, 116.3125, 107.0, 100.5, 125.5, 126.9375, 126.1875, 122.875, 117.3125, 108.0625, 105.3125, 128.25, 128.625, 127.75, 125.375, 121.125, 111.3125, 103.0625, 125.875, 124.9375, 122.75, 119.0, 115.1875, 106.3125, 99.0625, 115.75, 109.9375, 106.125, 101.25, 99.875, 92.3125, 86.1875, 95.4375, 92.0625, 87.8125, 87.375, 83.625, 78.0, 73.4375, 82.75, 79.8125, 81.0, 81.25, 82.625, 76.5625, 71.1875, 79.8125, 77.125, 72.6875, 71.5625], [0.0, 0.0, 0.125, 0.125, 0.125, 0.4375, 1.0, 1.0625, 1.1875, 1.375, 2.125, 2.6875, 3.75, 5.25, 7.0, 9.125, 12.625, 17.625, 24.5, 33.3125, 43.75, 56.0, 63.8125, 75.9375, 90.6875, 98.8125, 105.0625, 110.625, 115.5625, 109.9375, 108.5, 115.9375, 117.75, 120.6875, 120.0, 118.8125, 109.375, 105.0, 118.3125, 124.625, 125.9375, 122.8125, 115.8125, 106.625, 101.0625, 123.5, 127.0, 126.9375, 123.3125, 115.1875, 106.0625, 103.0, 126.0625, 127.8125, 127.625, 125.0625, 116.5, 107.3125, 102.6875, 126.75, 128.1875, 127.6875, 125.0, 116.8125, 107.5, 101.5625, 125.9375, 127.1875, 126.625, 123.75, 118.0625, 108.8125, 107.4375, 128.5625, 128.8125, 128.0, 125.875, 121.8125, 111.9375, 103.8125, 126.3125, 125.5, 123.6875, 120.125, 116.5625, 107.5625, 100.0, 117.0625, 111.6875, 108.3125, 103.5, 102.0625, 94.1875, 87.8125, 98.0, 95.3125, 89.8125, 89.4375, 85.1875, 79.3125, 75.6875, 85.375, 82.625, 83.75, 83.1875, 85.1875, 78.9375, 73.25, 83.125, 79.5625, 74.75, 74.1875], [0.0, 0.0, 0.3125, 0.3125, 0.3125, 0.6875, 1.1875, 1.1875, 1.375, 1.625, 2.4375, 3.0625, 4.1875, 5.9375, 7.875, 10.375, 14.3125, 19.9375, 27.5625, 37.5, 48.375, 61.125, 68.6875, 81.0, 95.75, 103.25, 109.1875, 113.5625, 117.5, 111.6875, 110.3125, 117.125, 118.6875, 122.125, 121.3125, 120.12656249999998, 110.5625, 106.875, 120.625, 125.0625, 126.375, 124.0625, 117.25, 107.9375, 102.875, 124.75, 127.5, 127.3125, 124.25, 116.625, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">107.4375, 105.1875, 126.68906249999998, 128.0, 127.875, 125.625, 117.375, 108.0625, 104.0625, 127.0625, 128.4375, 127.875, 125.5, 117.375, 108.0, 102.8125, 126.3125, 127.4375, 127.0, 124.625, 118.8125, 109.5625, 109.5625, 128.8125, 129.0, 128.25, 126.4375, 122.5, 112.5625, 104.50156249999998, 126.6875, 126.0625, 124.5625, 121.3125, 117.75, 108.6875, 100.875, 118.375, 113.3125, 110.5625, 105.8125, 104.31406249999998, 96.25, 89.5, 100.4375, 98.3125, 91.8125, 91.375, 86.6875, 80.625, 78.31406249999998, 88.1875, 85.625, 86.5, 84.9375, 87.75, 81.25, 75.3125, 86.0625, 81.9375, 76.75, 76.75]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.6875, 1.125, 1.5, 2.0625, 3.0625, 4.25, 5.875, 8.5625, 11.875, 15.625, 20.375, 26.375, 32.5, 37.875, 43.625, 49.625, 50.25, 50.1875, 53.75, 56.5625, 58.375, 58.8125, 58.4375, 54.0, 50.9375, 54.0625, 59.3125, 62.3125, 61.0625, 57.25, 52.8125, 49.1875, 55.75, 60.3125, 62.25, 60.5625, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">56.3125, 51.8125, 48.5625, 56.1875, 60.125, 61.6875, 60.4375, 56.1875, 51.625, 48.0625, 55.5, 59.25, 60.125, 58.8125, 54.9375, 50.5625, 46.875, 53.625, 56.875, 57.8125, 56.375, 53.5, 49.4375, 46.5, 54.25, 57.4375, 58.0625, 56.8125, 54.3125, 50.1875, 46.3125, 52.1875, 54.0625, 53.3125, 51.125, 49.25, 45.625, 42.1875, 45.3125, 43.875, 42.0, 39.5, 37.875, 35.3125, 33.0, 33.875, 33.0625, 31.125, 30.25, 28.8125, 27.125, 26.0625, 26.6875, 26.25, 26.3125, 26.0, 26.8125, 25.3125, 23.8125, 25.3125, 24.625, 23.125, 22.375], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.375, 0.875, 1.3125, 1.75, 2.375, 3.5, 4.9375, 6.75, 9.75, 13.4375, 17.4375, 22.3125, 28.75, 35.25, 40.875, 46.5, 52.0625, 52.25, 51.8125, 54.875, 57.1875, 59.3125, 59.75, 59.3125, 54.8125, 51.625, 55.25, 60.0625, 62.6875, 61.75, 58.0, 53.4375, 49.6875, 56.3125, 60.8125, 62.5, 61.125, 57.0, 52.4375, 49.0625, 56.5, 60.3125, 61.875, 60.8125, 56.625, 52.0, 48.25, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.75, 59.5, 60.375, 59.1875, 55.1875, 50.9375, 47.0625, 53.8125, 57.125, 58.0625, 56.875, 53.8125, 49.75, 46.9375, 54.625, 57.6875, 58.25, 57.125, 54.625, 50.5, 46.625, 52.5, 54.4375, 53.875, 51.8125, 49.75, 46.125, 42.625, 46.0, 44.875, 43.0, 40.625, 39.0, 36.375, 33.9375, 34.75, 34.3125, 32.1875, 31.125, 29.625, 27.8125, 26.6875, 27.5625, 27.1875, 27.25, 26.75, 27.5, 26.125, 24.5, 26.1875, 25.5, 23.9375, 23.1875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.625, 1.0, 1.5625, 2.0, 2.75, 4.0, 5.625, 7.626562499999977, 11.0, 15.1875, 19.5625, 24.625, 31.375, 38.4375, 44.25156249999998, 49.4375, 54.4375, 54.0, 53.1875, 55.75, 57.8125, 60.25, 60.75, 60.25, 55.6875, 52.3125, 56.125, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">60.6875, 63.0, 62.4375, 58.8125, 54.125, 50.25, 56.875, 61.25, 62.75, 61.6875, 57.62656249999998, 53.0625, 49.5625, 56.8125, 60.5625, 62.0, 61.1875, 57.0625, 52.3125, 48.4375, 55.9375, 59.75, 60.625, 59.5, 55.4375, 51.25, 47.25, 54.0, 57.375, 58.3125, 57.375, 54.125, 50.0, 47.4375, 54.9375, 57.875, 58.5, 57.4375, 55.0625, 50.8125, 46.9375, 52.8125, 54.8125, 54.375, 52.4375, 50.25, 46.625, 43.0625, 46.625, 45.75, 44.0, 41.8125, 40.125, 37.375, 34.875, 35.6875, 35.625, 33.3125, 31.9375, 30.375, 28.5, 27.3125, 28.5, 28.25, 28.25, 27.4375, 28.25, 26.875, 25.1875, 27.0625, 26.375, 24.75, 24.0]), ([0.0, 3.0625, 7.375, 18.6875, 35.375, 54.6875, 71.9375, 92.625, 130.75, 173.4375, 219.5625, 280.9984375, 355.80468750000006, 407.0609375, 470.8734375, 607.1875, 753.8734375, 920.29375, 1121.121875, 1363.6734375, 1513.6234375, 1694.1203125, 1934.559375, 2179.0, 2418.0, 2668.0609375, 2932.309375, 3120.3, 3291.4328125, 3502.05625, 3716.309375, 3945.175, 4151.125, 4341.496875, 4451.05625, 4561.4359375, 4741.6859375, 4981.9921875, 5232.809375, 5436.625, 5583.55, 5653.30625, 5731.1765625, 5950.43125, 6213.2359375, 6471.6859375, 6669.3125, 6792.309375, 6855.9375, 6935.871875, 7172.4984375, 7447.2484375, 7705.8109375, 7908.6109375, 8021.99375, 8086.6234375, 8166.55625, 8396.7421875, 8664.125, 8899.3109375, 9088.2390625, 9201.8078125, 9268.496875, 9334.9296875, 9539.6203125, 9759.3125, 9972.3109375, 10143.559375, 10267.8125, 10335.1875, 10422.2484375, 10735.1859375, 11032.3734375, 11275.7484375, 11459.9359375, 11599.1859375, 11652.1875, 11713.25, 11900.80625, 12080.3109375, 12234.6859375, 12363.4984375, 12470.99375, 12522.61875, 12575.3109375, 12692.6875, 12786.5609375, 12872.1875, 12945.375, 13018.3125, 13060.2484375, 13100.9375, 13168.125, 13228.8109375, 13278.309375, 13331.8125, 13378.375, 13413.1875, 13447.0625, 13496.75, 13540.559375, 13586.5, 13631.625, 13682.0625, 13709.1234375, 13733.3734375, 13781.625, 13821.6234375, 13856.4359375, 13894.125, 13930.0609375, 13952.4359375], [0.0, 4.0625, 9.25, 21.4375, 39.4375, 59.8125, 77.6875, 100.625, 142.0, 187.375, 238.0625, 305.0, 386.375, 440.5625, 509.6875, 656.625, 813.0625, 991.125, 1205.625, 1468.9375, 1628.125, 1811.5625, 2065.1875, 2320.75, 2572.6875, 2825.5, 3090.625, 3275.5625, 3442.6875, 3647.625, 3856.625, 4081.375, 4288.125, 4476.75, 4578.5, 4681.8125, 4859.625, 5094.75, 5346.9375, 5556.625, 5700.9375, 5766.25, 5844.4375, 6057.5, 6321.5, 6583.0625, 6780.4375, 6900.1875, 6962.3125, 7044.5, 7282.625, 7553.8125, 7815.8125, 8012.6875, 8131.5625, 8193.0, 8268.875, 8496.4375, 8762.4375, 9002.1875, 9184.9375, 9299.6875, 9364.25, 9433.75, 9633.125, 9849.375, 10057.5, 10223.9375, 10345.875, 10414.3125, 10499.9375, 10813.5, 11100.3125, 11339.8125, 11521.5625, 11658.875, 11715.8125, 11775.4375, 11961.125, 12134.125, 12285.1875, 12410.25, 12518.375, 12570.25, 12623.5625, 12734.75, 12825.9375, 12908.1875, 12980.5625, 13051.4375, 13092.75, 13133.375, 13198.9375, 13257.1875, 13305.9375, 13357.1875, 13402.875, 13437.25, 13469.6875, 13519.3125, 13561.25, 13607.25, 13652.75, 13701.3125, 13728.4375, 13753.0625, 13801.0, 13840.8125, 13875.75, 13912.625, 13948.375, 13969.8125], [0.0, 5.1875, 11.5, 24.9375, 43.875, 65.5, 84.625, 110.18906249999998, 154.9375, 203.93906249999998, 258.7515625, 331.6875, 420.5625, 477.5, 551.8140625, 713.378125, </t>
+  </si>
+  <si>
+    <t>879.9375, 1065.9421874999998, 1299.6890625, 1580.63125, 1745.69375, 1936.125, 2206.0015625, 2470.5015625, 2735.75, 2990.1328125, 3256.75625, 3439.0109374999997, 3591.9390625, 3785.0046875, 3990.190625, 4215.95, 4427.1421875, 4612.7625, 4708.7, 4800.63125, 4971.8140625, 5211.8234375, 5462.509375, 5673.571875, 5819.190625, 5878.6296875, 5954.3125, 6166.25, 6433.634375, 6693.4421875, 6894.25625, 7014.0640625, 7080.0015625, 7154.628125, 7392.503125, 7659.3828125, 7922.6265625, 8117.3859375, 8232.1984375, 8296.1296875, 8368.8125, 8597.196875, 8858.378125, 9100.315625, 9274.4390625, 9392.565625, 9453.5015625, 9524.628125, 9722.5640625, 9935.4421875, 10145.00625, 10299.5640625, 10424.44375, 10494.1921875, 10575.5, 10888.1296875, 11164.8796875, 11400.1921875, 11581.753125, 11715.88125, 11777.3125, 11837.003125, 12019.1890625, 12184.125, 12334.0046875, 12456.3140625, 12562.25, 12616.0640625, 12668.3125, 12776.7515625, 12865.0046875, 12943.2515625, 13014.5640625, 13085.0640625, 13124.1265625, 13165.0015625, 13228.875, 13284.0640625, 13333.1875, 13383.2515625, 13427.4421875, 13461.1875, 13493.5015625, 13542.9390625, 13583.8765625, 13628.9390625, 13674.5015625, 13721.5, 13749.4375, 13774.0625, 13821.4390625, 13861.125, 13895.1875, 13930.6875, 13966.1875, 13987.5]))</t>
+  </si>
+  <si>
+    <t>58.8125, 59.5625, 58.125, 54.0625, 49.875, 46.25, 52.5625, 55.5625, 55.9375, 55.375, 52.8125, 48.75, 45.5625, 53.5, 56.5, 56.8125, 55.75, 53.5, 49.4375, 45.5625, 50.6875, 51.3125, 50.0, 47.9375, 45.875, 42.5625, 39.5, 41.4375, 39.9375, 38.25, 36.8125, 35.1875, 33.0, 31.0, 31.0625, 29.4375, 27.875, 26.5, 25.75, 24.5, 23.1875, 23.6875, 23.0625, 22.5625, 22.75, 23.3125, 22.375, 21.25, 22.125, 21.625, 20.875, 19.9375], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.875, 1.0, 1.0, 2.0, 2.1875, 3.1875, 4.875, 6.875, 9.9375, 14.0625, 19.875, 27.8125, 37.1875, 44.4375, 51.8125, 59.1875, 63.0, 63.75, 61.6875, 58.4375, 54.3125, 52.6875, 60.125, 64.1875, 65.6875, 62.68906249999998, 58.125, 53.5625, 50.3125, 58.18906249999998, 62.625, 64.0, 61.9375, 57.1875, 52.9375, 49.125, 56.9375, 61.5, 63.0, 61.9375, 57.1875, 53.0, 49.25, 56.6875, 60.875, 62.1875, 61.0625, 56.5, 51.9375, 48.0, 55.25, 59.0, 59.8125, 58.4375, 54.4375, 50.1875, 46.5625, 52.8125, 55.8125, 56.3125, 55.6875, 53.1875, 49.125, 45.8125, 53.75, 56.75, 57.0625, 56.0, 53.9375, 49.875, 46.0, 51.0625, 51.8125, 50.75, 48.625, 46.5, 43.125, 40.0, 42.3125, 40.6875, 39.0, 37.6875, 36.25, 33.9375, 31.75, 32.0, 30.1875, 28.6875, 27.125, 26.4375, 25.125, 23.75, 24.25, 23.625, 23.1875, 23.4375, 24.125, 23.1875, 21.8125, 22.5625, 22.001562499999977, 21.3125, 20.25]), ([0.0, 8.0625, 17.5625, 44.6875, 87.87343750000001, 133.6875, 170.5625, 213.875, 298.1859375, 390.1875, 488.6875, 619.9375, 773.0609375, 874.1859375, 1002.3125, 1264.3640625, 1541.1234375, 1841.3734375, 2196.8671875, 2609.9359375, 2846.0625, 3098.6140625000003, 3448.0625, 3750.18125, 3996.0578125, 4186.6234375, 4331.6875, 4424.80625, 4533.5578125, 4752.4328125, 4992.5609375, 5247.9984375, 5410.43125, 5511.4359375, 5558.0609375, 5644.8046875, 5873.1171875, 6135.371875, 6387.7453125, 6573.3734375, 6675.4359375, 6731.2453125, 6808.246875, 7034.2484375, 7297.559375, 7548.934375, 7742.2484375, 7848.4359375, 7909.625, 7982.678125, 8198.8109375, 8475.7484375, 8732.5546875, 8915.75, 9021.8109375, 9077.4359375, 9148.0609375, 9357.371875, 9588.1234375, 9801.2453125, 9964.875, 10071.996875, 10128.934375, 10198.2484375, 10367.121875, 10548.7359375, 10715.6859375, 10865.9984375, 10989.7484375, 11058.1859375, 11135.496875, 11395.309375, 11622.496875, 11826.6859375, 11989.8109375, 12122.375, 12174.8109375, 12225.684375, 12381.8125, 12517.4921875, 12639.1875, 12740.0, 12835.4375, 12882.8109375, 12927.1859375, 13015.9359375, 13089.375, 13156.75, 13221.7484375, 13282.0, 13313.8734375, 13347.8109375, 13403.996875, 13448.5625, 13490.6875, 13529.9984375, 13568.0578125, 13593.4359375, 13616.1234375, 13656.625, 13689.3125, 13723.0609375, 13761.0609375, 13798.625, 13822.3734375, 13843.625, 13878.934375, 13913.246875, 13944.0, 13970.371875, 13998.625, 14018.1875], [0.0, 9.25, 19.3125, 47.875, 94.0625, 140.6875, 179.125, 224.5, 312.0625, 406.875, 507.3125, 643.75, 802.5, 908.6875, 1039.8125, 1313.125, 1601.5, 1910.875, 2279.3125, 2699.5625, 2939.125, 3198.625, 3552.125, 3852.625, 4097.3125, 4275.8125, 4414.3125, 4503.5, 4615.8125, 4837.5, 5082.4375, 5332.375, 5488.1875, 5585.9375, 5630.3125, 5714.3125, 5950.125, 6213.25, 6468.8125, 6648.625, 6747.375, 6801.125, 6880.9375, 7110.8125, 7377.625, 7627.0, 7817.125, 7923.5, 7980.875, 8053.8125, 8277.0, 8549.3125, 8810.0, 8993.0625, 9099.1875, 9151.4375, 9219.8125, 9427.8125, 9655.875, 9868.5, 10029.4375, 10137.75, 10194.5, 10264.875, 10433.125, 10610.0625, 10775.375, 10926.9375, 11049.6875, 11115.9375, 11192.375, 11449.8125, 11673.0625, 11871.25, 12035.0, 12167.4375, 12218.8125, 12270.3125, 12422.0625, 12554.125, 12671.75, 12773.375, 12866.125, 12913.6875, 12956.75, 13043.4375, 13115.8125, 13180.0, 13244.875, 13304.3125, 13337.375, 13371.125, 13425.9375, 13471.4375, 13512.1875, 13551.6875, 13590.6875, 13616.0625, 13638.75, 13677.25, 13710.125, 13744.125, 13781.1875, 13818.4375, 13842.125, 13863.6875, 13900.375, 13933.4375, 13962.5625, 13988.5625, 14016.0625, 14034.875], [0.0, 10.5625, 21.125, 51.1875, 100.4375, 147.3125, 186.8125, 234.1875, 325.3140625, 422.5640625, 525.5640625, 666.8765625, 832.4375, 942.6296874999999, 1079.3765625, 1362.5640625, 1660.9375, 1979.6890625, 2360.440625, 2788.940625, 3030.88125, 3293.5, 3652.9390625, 3957.44375, 4193.1265625, 4367.890625, 4497.0078125, 4582.0640625, 4698.4390625, 4924.3140625, 5168.4421875, 5413.45, 5564.31875, 5659.75625, 5704.2515625, 5786.5, 6026.0, 6290.38125, 6545.6953125, 6726.63125, 6822.3171875, 6875.076562499999, 6955.8140625, 7190.5015625, 7459.25, 7709.00625, 7893.128125, 8000.4453125, 8060.071875, 8129.1265625, 8355.4375, 8626.7625, 8891.0015625, 9070.1265625, 9175.8765625, 9227.440625, 9294.7546875, 9501.565625, 9724.128125, 9938.1984375, 10099.3765625, 10206.6265625, 10263.8140625, 10331.759375, 10497.8140625, 10675.5046875, 10838.25, 10991.3125, 11110.190625, 11177.003125, 11252.5640625, 11509.0625, 11725.44375, 11920.628125, 12084.0, 12214.440625, 12263.940625, 12317.625, 12462.2515625, 12593.6265625, 12706.6890625, 12807.625, 12896.7515625, 12945.25, 12987.3125, 13072.0, 13142.6875, 13206.0, 13269.1875, 13326.9390625, 13360.8125, 13395.440625, 13448.7515625, 13494.0640625, 13533.1265625, 13573.1875, 13612.5625, 13638.1875, 13660.8765625, 13697.6890625, 13730.3140625, 13764.8125, 13800.9375, 13838.0, 13861.4390625, 13883.8125, 13920.5, 13953.4390625, 13980.9390625, 14006.1890625, 14032.8125, 14051.4375]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.0, 0.0, 1.0, 1.0, 1.0, 1.0, 1.625, 2.0, 2.625, 3.0, 4.625, 6.1875, 8.5, 11.873437500000007, 16.5625, 22.5625, 31.0625, 43.75, 60.8125, 79.0, 93.875, 107.25, 107.6875, 114.1875, 122.625, 122.5, 121.5625, 116.0625, 110.5, 103.125, 105.9375, 122.0, 125.375, 126.0625, 117.8125, 109.1875, 100.3125, 98.6875, 123.5625, 126.5, 126.0, 120.3125, 110.875, 102.0625, 98.6875, 124.5625, 127.0, 126.875, 123.3125, 113.8125, 104.8125, 99.4375, 125.375, 128.0, 127.875, 124.0625, 114.875, 105.75, 99.75, 125.875, 126.9375, 126.25, 122.625, 114.375, 105.25, 100.5625, 123.5625, 124.4375, 123.0, 121.75, 116.75, 107.625, 102.875, 127.1875, 126.875, 125.75, 123.6875, 119.375, 109.8125, 101.25, 122.0, 119.75, 116.375, 112.9375, 109.875, 101.4375, 93.4375, 107.1875, 102.875, 97.9375, 96.375, 92.75, 85.6875, 79.9375, 87.5, 83.74843750000001, 79.625, 77.3125, 75.625, 70.5625, 65.9375, 72.74843750000001, 70.875, 70.125, 72.125, 72.9375, 67.8125, 63.875, 72.0625, 69.8125, 66.6875, 63.5625], [0.0, 0.125, 1.0, 1.0, 1.0, 1.0, 1.8125, 2.0, 2.8125, 3.1875, 4.8125, 6.5, 8.875, 12.375, 17.25, 23.5, 32.375, 45.5, 63.125, 81.875, 96.6875, 109.9375, 109.4375, 115.625, 123.5625, 123.375, 122.125, 117.1875, 112.0625, 104.25, 108.0625, 123.75, 126.0, 126.5, 119.125, 110.5625, 101.5625, 101.25, 124.5, 126.9375, 126.3125, 121.375, 111.75, 102.875, 100.375, 125.1875, 127.25, 127.125, 124.0625, 114.4375, 105.375, 101.4375, 125.875, 128.25, 128.0625, 124.6875, 115.5625, 106.3125, 100.75, 126.25, 127.25, 126.5625, 123.1875, 115.375, 106.0625, 101.8125, 123.9375, 124.8125, 123.6875, 122.3125, 117.5625, 108.4375, 104.0625, 127.4375, 127.1875, 126.25, 124.1875, 120.3125, 110.625, 102.0, 123.0625, 120.625, 117.8125, 114.1875, 111.5, 102.8125, 94.8125, 109.0, 104.3125, 99.75, 98.6875, 95.125, 87.875, 81.6875, 90.25, 85.4375, 81.4375, 79.0, 78.0, 72.6875, 67.8125, 75.25, 72.8125, 72.25, 74.625, 75.5, 70.125, 66.0, 73.375, 71.125, 68.3125, 65.4375], [0.0, 0.3125, 1.0, 1.0, 1.0, 1.0, 2.0, 2.0, 3.0, 3.375, 5.0, 6.75, 9.1875, 12.8125, 17.8125, 24.3125, 33.5625, 47.0625, 65.1875, 84.5625, 99.25, 112.25, 111.1875, 117.125, 124.5, 124.25, 122.625, 118.625, 113.75, 105.31406249999998, 110.125, 125.125, 126.5625, 126.9375, 120.5625, 112.0, 102.75, 103.875, 125.4375, 127.375, 126.5625, 122.4375, 112.6875, 103.625, 102.1875, 125.8125, 127.5, 127.375, 124.875, 115.0625, 106.0, 103.75, 126.375, 128.5, 128.25, 125.25, 116.1875, 106.875, 101.9375, 126.5625, 127.5625, 126.875, 123.75, 116.4375, 106.9375, 103.0, 124.3125, 125.1875, 124.3125, 122.9375, 118.3125, 109.1875, 105.25, 127.6875, 127.5, 126.6875, 124.625, 121.25, 111.5, 102.8125, 124.0625, 121.375, 119.25156249999998, 115.5, 112.9375, 104.0625, 96.0, 110.75, 105.8125, 101.56406249999998, 101.0625, 97.625, 90.1875, 83.625, 92.6875, 87.0625, 83.3125, 80.6875, 80.3125, 74.75, 69.5625, 77.8125, 74.6875, 74.4375, 77.1875, 78.125, 72.5, 68.125, 74.6875, 72.4375, 70.0, 67.25]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.4375, 1.0, 1.0, 1.625, 2.0, 3.0, 4.4375, 6.3125, 9.1875, 13.0, 18.4375, 25.75, 34.5, 41.625, 48.875, 56.5, 60.875, 62.625, 60.375, 57.0625, 53.0, 51.4375, 58.375, 63.0, 65.0625, 61.1875, 56.625, 52.1875, 49.5, 57.31093750000001, 62.0625, 63.5, 60.9375, 56.1875, 52.0, 48.375, 56.25, 61.0625, 62.625, 61.0625, 56.49843750000001, 52.125, 48.4375, 55.9375, 60.4375, 62.0, 60.3125, 55.875, 51.375, 47.6875, 54.875, 58.625, 59.3125, 57.8125, 53.6875, 49.5, 45.9375, 52.25, 55.3125, 55.5, 55.0625, 52.4375, 48.375, 45.25, 53.25, 56.25, 56.5625, 55.5, 53.0625, 49.0625, 45.1875, 50.25, 50.8125, 49.25, 47.1875, 45.1875, 42.0, 38.9375, 40.625, 39.25, 37.5, 35.9375, 34.125, 32.125, 30.25, 30.0625, 28.6875, 27.0625, 25.8125, 25.0625, 23.8125, 22.625, 23.125, 22.4375, 22.0, 22.0625, 22.5, 21.5625, 20.625, 21.6875, 21.1875, 20.4375, 19.5625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.6875, 1.0, 1.0, 1.8125, 2.0625, 3.0625, 4.6875, 6.625, 9.5625, 13.5625, 19.1875, 26.8125, 35.9375, 43.125, 50.375, 57.875, 61.9375, 63.1875, 61.0, 57.6875, 53.5625, 52.0625, 59.3125, 63.625, 65.375, 61.9375, 57.375, 52.875, 49.875, 57.75, 62.375, 63.8125, 61.4375, 56.6875, 52.4375, 48.75, 56.625, 61.25, 62.8125, 61.5, 56.8125, 52.5625, 48.8125, 56.3125, 60.6875, 62.0625, 60.6875, 56.1875, 51.6875, 47.875, 55.0625, </t>
+  </si>
+  <si>
+    <t>Infection Riks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.125, 0.375, 0.375, 0.4375, 0.875, 1.125, 1.5, 2.0625, 2.75, 3.4375, 4.4375, 6.3125, 8.6875, 11.25, 14.4375, 18.8125, 21.0625, 23.75, 30.125, 34.4375, 39.875, 44.43593750000001, 49.625, 48.0, 50.75, 61.0625, 64.8125, 68.9375, 73.81093750000001, 79.6875, 75.5, 77.0, 89.875, 93.25, 95.6875, 100.3125, 103.625, 97.3125, 96.6875, 109.0, 113.1875, 113.875, 116.3125, 116.0, 107.625, 105.5625, 120.4375, 122.375, 122.62343750000001, 122.375, 119.9375, 111.1875, 108.0, 124.0625, 126.4375, 126.3125, 125.1875, 121.9375, 112.5625, 110.0625, 129.1875, 129.8125, 130.0, 128.5625, 125.5, 115.5, 109.5, 128.5625, 129.5625, 128.75, 127.4375, 123.9375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">114.0625, 106.375, 126.6875, 126.375, 124.125, 122.0, 117.9375, 108.43593750000001, 100.81093750000001, 118.9375, 115.25, 110.1875, 108.9375, 106.4375, 98.0625, 90.8125, 104.99843750000001, 99.375, 98.9375, 100.125, 103.8125, 95.875, 88.5, 103.3125, 96.6875, 95.0, 93.5], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.125, 0.3125, 0.375, 0.6875, 0.75, 0.8125, 1.375, 1.8125, 2.375, 3.3125, 4.5, 5.75, 7.5625, 10.375, 14.0, 17.8125, 22.25, 27.75, 29.8125, 32.8125, 41.3125, 45.9375, 51.625, 57.0, 62.8125, 60.0, 62.6875, 74.75, 79.25, 82.8125, 87.1875, 93.125, 87.1875, 88.125, 101.8125, 104.0625, 105.3125, 108.9375, 111.875, 104.25, 102.6875, 115.125, 118.5, 119.625, 120.0625, 118.875, 109.9375, 107.125, 122.1875, 124.625, 124.8125, 123.6875, 121.0625, 112.0, 109.5, 124.9375, 127.125, 126.8125, 125.8125, 122.8125, 113.375, 112.125, 129.4375, 129.9375, 130.0, 128.8125, 126.1875, 116.3125, 111.5, 128.875, 129.75, 129.0, 127.8125, 124.8125, 115.0, 108.125, 127.4375, 127.3125, 125.75, 123.375, 119.5, 109.875, 102.6875, 121.0625, 117.75, 113.25, 111.3125, 109.6875, 100.9375, 93.4375, 108.0625, 102.75, 101.5625, 103.375, 106.3125, 98.125, 90.5, 106.25, 99.4375, 97.5625, 96.6875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.3125, 0.5625, 0.625, 1.0, 1.125, 1.25, 1.9375, 2.5625, 3.4375, 4.6875, 6.5625, 8.4375, 11.0625, 15.125, 20.5625, 25.4375, 30.8125, 37.25, 38.75156249999998, 42.3125, 52.4375, 57.12656249999998, 62.8125, 68.62656249999998, 74.9375, 70.8125, 73.3125, 86.875, 90.75, 94.0, 98.0, 103.5, 96.3125, 97.625, 111.1875, 112.6875, 113.375, 115.625, 117.6875, 109.625, 107.375, 119.6875, 122.5, 123.875, 122.8125, 121.0625, 111.8125, 108.625, 123.6875, 126.375, 126.4375, 124.875, 122.0625, 112.8125, 111.0625, 125.8125, 127.625, 127.25, 126.375, 123.5625, 114.125, 114.12656249999998, 129.6875, 130.0, 130.0, 129.0625, 126.8125, 117.125, 113.75156249999998, 129.1875, 129.9375, 129.25, 128.1875, 125.6875, 116.0, 110.125, 128.0625, 128.125, 127.1875, 124.75, 121.125, 111.375, 104.75, 122.81406249999998, 120.25, 116.4375, 113.875, 112.9375, 103.75, 96.1875, 111.25, 106.25, 104.5, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">106.5625, 108.9375, 100.5625, 92.5, 109.3125, 102.5625, 100.3125, 99.625]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.1875, 0.375, 0.6875, 1.0625, 1.5, 2.125, 2.9375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9375, 4.875, 5.75, 7.75, 9.4375, 11.310937500000007, 13.060937500000007, 15.625, 15.9375, 16.875, 20.3125, 23.3125, 25.125, 27.5625, 30.6875, 30.125, 29.875, 35.12343750000001, 38.12343750000001, 39.5, 41.9375, 44.1875, 42.25, 41.3125, 45.75, 49.125, 51.0, 52.06093750000001, 52.4375, 49.25, 46.8125, 52.125, 55.0, 56.3125, 56.5, 55.375, 51.4375, 48.375, 53.75, 56.9375, 58.0, 57.5625, 56.0, 51.8125, 48.8125, 55.8125, 58.8125, 59.3125, 59.0, 57.0625, 52.8125, 48.875, 54.75, 57.1875, 57.75, 56.9375, 54.75, 50.4375, 46.9375, 52.0, 53.8125, 53.1875, 51.9375, 49.5, 45.875, 42.5, 46.3125, 46.0625, 43.6875, 42.375, 40.75, 38.0, 35.3125, 37.375, 36.0, 35.1875, 35.375, 36.75, 34.5, 32.25, 35.375, 33.75, 32.875, 31.875], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.1875, 0.375, 0.625, 0.8125, 1.3125, 1.9375, 2.6875, 3.6875, 5.0, 6.6875, 7.625, 8.75, 11.4375, 13.6875, 15.8125, 18.0625, 21.0625, 21.25, 22.1875, 26.3125, 29.5, 31.6875, 34.0625, 37.4375, 36.25, 36.0, 41.4375, 44.5625, 45.8125, 47.6875, 49.8125, 47.125, 45.5625, 49.875, 53.1875, 55.0, 55.4375, 55.125, 51.3125, 48.375, 53.5, 56.625, 57.9375, 57.75, 56.125, 52.0, 49.0, 54.25, 57.375, 58.5, 58.0, 56.375, 52.1875, 49.5, 56.125, 58.9375, 59.5625, 59.0625, 57.4375, 53.1875, 49.5, 55.0625, 57.4375, 57.9375, 57.1875, 55.25, 50.9375, 47.5, 52.5625, 54.4375, 54.1875, 52.875, 50.5, 46.6875, 43.375, 47.5, 47.375, 45.375, 43.875, 42.4375, 39.5625, 36.6875, 39.0625, 37.8125, 36.6875, 37.0, 38.0625, 35.6875, 33.375, 36.75, 35.3125, 34.25, 33.375], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.375, 0.75, 1.125, 1.3125, 2.125, 3.0, 4.125, 5.5625, 7.375, 9.75, 10.875, 12.1875, 15.4375, 18.25, 20.4375, 23.25, 26.439062499999977, 26.4375, 27.1875, 31.875, 35.25, 37.25, 40.0, 43.375, 41.375, 41.0625, 46.8125, 49.9375, 51.0, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">52.4375, 54.0625, 50.9375, 48.8125, 53.0625, 56.1875, 58.125, 57.9375, 57.0625, 52.875, 49.4375, 54.5625, 57.875, 59.125, 58.6875, 56.8125, 52.5625, 49.5625, 54.6875, 57.75, 58.9375, 58.375, 56.75, 52.5, 50.25, 56.4375, 59.0, 59.8125, 59.1875, 57.8125, 53.5625, 50.25, 55.4375, 57.6875, 58.125, 57.4375, 55.75, 51.5, 48.125, 53.125, 54.9375, 55.0, 53.8125, 51.5, 47.5625, 44.3125, 48.625, 48.6875, 47.1875, 45.5, 44.1875, 41.125, 38.12656249999998, 40.875, 39.8125, 38.375, </t>
+  </si>
+  <si>
+    <t>38.75, 39.43906249999998, 37.0625, 34.62656249999998, 38.3125, 37.0625, 35.75, 34.9375]), ([0.0, 0.1875, 0.4375, 1.0, 2.25, 4.060937500000007, 4.75, 6.125, 9.5, 13.875, 19.8125, 28.3125, 38.62343750000001, 44.24843750000001, 51.8125, 70.74843750000001, 95.56093750000001, 123.18437500000002, 152.1859375, 193.11875000000003, 217.24375000000003, 251.61562500000005, 294.875, 343.1828125, 400.8109375, 462.5578125, 530.5578125000001, 581.4296875, 639.8109375, 743.184375, 818.0500000000001, 920.7484375, 1030.3046875, 1147.11875, 1251.7375, 1346.18125, 1485.746875, 1629.0343750000002, 1771.4875, 1914.1781250000001, 2077.746875, 2217.30625, 2325.4328125, 2535.1453125000003, 2719.9984375000004, 2884.9609375, 3085.1875, 3280.428125, 3439.8578125, 3563.8078125, 3763.4890625000003, 3987.6796875, 4217.4953125, 4430.15625, 4632.475, 4758.2359375, 4881.8578125, 5079.828125, 5329.0828125, 5574.9640625, 5788.684375, 5993.1828125, 6081.053125, 6205.121875, 6434.74375, 6684.109375, 6937.6078125, 7136.1, 7322.0390625, 7412.684375, 7546.43125, 7898.846875, 8311.8953125, 8667.3578125, 8978.0515625, 9155.2375, 9264.234375, 9367.0546875, 9629.4921875, 9983.515625, 10277.6015625, 10505.609375, 10669.303125, 10746.573437500001, 10816.6703125, 11023.5578125, 11241.925, 11453.43125, 11607.4984375, 11716.603125, 11789.8015625, 11850.28125, 12000.559375, 12127.125, 12237.7359375, 12333.809375, 12437.7296875, 12483.934375, 12531.0625, 12635.28125, 12709.4359375, 12790.8, 12882.6828125, 12971.9984375, 13015.4984375, 13054.75, 13151.2984375, 13231.678125, 13303.1859375, 13374.8703125, 13447.059375, 13484.9953125], [0.0, 0.625, 1.25, 2.25, 4.0625, 6.625, 8.125, 10.0625, 15.125, 21.5625, 30.3125, 42.0, 57.0, 65.1875, 76.4375, 102.625, 134.9375, 171.125, 211.375, 265.3125, 301.3125, 341.3125, 400.3125, 465.4375, 536.5, 612.375, 700.25, 770.9375, 844.9375, 954.3125, 1062.0625, 1180.9375, 1310.625, 1452.0, 1556.5, 1667.6875, 1827.875, 1990.9375, 2154.1875, 2323.625, 2509.25, 2641.5625, 2778.25, 2979.5625, 3180.875, 3375.0, 3579.125, 3790.4375, 3931.5625, 4067.6875, 4272.3125, 4500.125, 4733.25, 4951.6875, 5147.9375, 5265.0, 5383.6875, 5594.25, 5841.0625, 6086.625, 6300.1875, 6478.0, 6581.625, 6691.125, 6905.125, 7160.25, 7407.8125, 7622.625, 7794.4375, 7888.375, 7995.4375, 8349.6875, 8749.4375, 9111.6875, 9389.4375, 9578.75, 9665.25, 9752.75, 10011.875, 10345.625, 10620.0625, 10828.5625, 10982.3125, 11049.625, 11118.8125, 11316.625, 11519.1875, 11695.75, 11840.9375, 11958.875, 12015.125, 12075.5625, 12209.1875, 12326.125, 12425.0625, 12517.5, 12607.6875, 12658.0, 12702.875, 12791.6875, 12865.25, 12938.1875, 13016.5, 13102.375, 13144.4375, 13183.9375, 13272.8125, 13340.625, 13409.125, 13476.4375, 13543.6875, 13576.5], [0.0, 1.125, 2.25, 3.75, 6.1875, 9.8125, 12.1875, 14.6875, 21.625, 30.8125, 42.68906249999998, 58.8125, 77.43906249999998, 87.875, 104.375, 137.43906249999998, 178.00156249999998, 222.9437499999999, 272.1875, 344.6265625, 387.57343749999984, 436.5078124999999, 511.81718749999993, 599.0093749999999, 677.503125, 776.753125, 877.6999999999998, 965.4437499999999, 1055.0671874999998, 1174.6359374999997, 1309.0749999999998, 1438.5078125, 1581.1343749999999, 1737.2546874999998, 1869.125, 1981.253125, 2153.9796874999993, 2351.4421875, 2518.94375, 2689.139062499999, 2893.8312499999997, 3026.0703125, 3184.7671874999996, 3394.565625, 3596.448437499999, 3815.1968749999996, 4031.590625, 4244.765625, 4382.2671875, 4512.459374999999, 4714.278125, 4956.5875, 5185.328125, 5413.090625, 5599.065625, 5727.206249999999, 5818.821875, 6028.5078125, 6281.8140625, 6530.8765625, 6747.464062499999, 6893.5359375, 6984.964062499999, 7106.078125, 7320.946875, 7571.4078125, 7824.659374999999, 8036.0046875, 8207.9421875, 8277.1984375, 8381.321875, 8731.0796875, 9121.4515625, 9484.1390625, 9736.787499999999, 9921.509375, 10009.19375, 10083.0734375, 10328.6890625, 10641.834375, 10907.2515625, 11101.715624999999, 11241.457812499999, 11306.8765625, 11378.203125, 11559.1296875, 11753.690625, 11908.13125, 12042.134375, 12150.0046875, 12204.94375, 12260.00625, 12386.5015625, 12493.5046875, 12578.5671875, 12668.1265625, 12755.5640625, 12798.9375, 12842.4375, 12926.75625, 12990.190625, 13058.3765625, 13136.63125, 13216.2546875, 13258.9390625, 13292.5015625, 13374.8765625, 13433.9421875, 13499.321875, 13565.1890625, 13622.5640625, 13653.5671875]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.125, 0.3125, 0.3125, 0.4375, 0.8125, 1.0625, 1.25, 1.9375, 2.6875, 3.0625, 3.9375, 5.4375, 7.0, 9.5, 11.8125, 14.9375, 17.0625, 19.25, 24.625, 28.68593750000001, 33.25, 37.5, 43.24843750000001, 39.87343750000001, 43.25, 53.25, 57.43593750000001, 61.75, 66.4375, 72.3125, 67.9375, 70.62343750000001, 83.68593750000001, 85.5625, 87.62343750000001, 91.875, 98.125, 91.375, 91.9375, 103.6875, 105.625, 108.625, 110.125, 112.8125, 105.375, 102.625, 117.0625, 119.25, 119.4375, 119.8125, 120.25, 111.875, 107.9375, 122.6875, 124.5625, 124.8125, 124.1875, 122.0, 113.125, 111.4375, 129.0625, 130.0, 129.5, 128.375, 126.4375, 116.25, 111.0, 128.6875, 129.6875, 129.0625, 128.3125, 125.5, 115.5625, 109.3125, 127.5625, 127.9375, 126.5, 125.5, 121.125, 111.3125, 104.0625, 122.6875, 119.875, 116.75, 116.5625, 113.5, 104.3125, 96.9375, 110.1875, 105.0625, 104.625, 106.1875, 107.4375, 99.125, 92.125, 108.375, 102.75, 98.9375, 98.0], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.125, 0.1875, 0.3125, 0.375, 0.625, 0.625, 0.8125, 1.25, 1.625, 1.9375, 3.0, 3.9375, 4.875, 6.25, 8.5625, 11.25, 14.6875, 18.4375, 23.0625, 23.9375, 26.75, 33.6875, 37.8125, 43.125, 47.5625, 53.4375, 50.1875, 52.875, 64.25, 67.75, 71.1875, 76.0625, 81.6875, 76.5, 78.5625, 92.1875, 93.1875, 95.4375, 99.125, 104.1875, 97.0, 96.875, 108.5, 111.125, 113.3125, 114.0, 115.875, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">107.9375, 105.8125, 119.5, 121.0625, 121.625, 121.0625, 121.3125, 112.625, 109.4375, 123.25, 125.3125, 125.6875, 124.625, 122.8125, 113.6875, 113.0, 129.25, 130.0, 129.75, 128.625, 126.9375, 116.8125, 112.75, 128.875, 129.875, 129.375, 128.625, 126.25, 116.4375, 110.8125, 128.0, 128.5, 127.375, 126.125, 122.5625, 112.625, 105.75, 123.9375, 121.8125, 119.25, 118.4375, 115.375, 106.1875, 98.6875, 112.8125, 108.625, 107.5625, 108.9375, 110.0, 101.4375, 93.9375, 110.4375, 104.75, 101.4375, 101.0625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.3125, 0.375, 0.5625, 0.625, 0.9375, 0.9375, 1.25, 1.6875, 2.25, 2.6875, 4.1875, 5.4375, 6.9375, 8.9375, 12.125, 15.9375, 20.375, 26.25, 31.625, 31.5625, 35.0, 43.125, 47.375, 53.0, 57.62656249999998, 63.875, 60.0, 62.5625, 74.31406249999998, 77.56406249999998, 80.0625, 85.5625, 90.0625, 84.125, 86.3125, 99.9375, 100.0625, 102.5625, 105.75, 109.75, 101.875, 101.125, 112.75, 115.875, 117.375, 117.375, 118.375, 110.125, 108.4375, 121.5625, 122.6875, 123.5, 122.1875, 122.3125, 113.3125, 111.0625, 123.8125, 126.0, 126.5, 125.125, 123.5625, 114.25, 114.5625, 129.5, 130.0, 129.9375, 128.875, 127.4375, 117.3125, 114.4375, 129.0, 130.0, 129.6875, 128.875, 126.875, 117.3125, 112.4375, 128.375, 129.0625, 128.0625, 126.75, 123.875, 113.875, 107.5625, 125.1875, 123.625, 121.5, 120.1875, 117.1875, 107.9375, 100.5, 115.375, 112.1875, 110.375, 111.43906249999998, 112.4375, 103.68906249999998, 95.8125, 112.43906249999998, 106.75, 103.87656249999998, 104.0625]), ([0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.0625, 0.125, 0.3125, 0.4375, 0.875, 1.1875, 1.5625, 2.125, 3.0625, 3.5625, 4.25, 5.625, 7.0625, 8.4375, 10.3125, 12.25, 12.4375, 13.125, 16.1875, 18.375, 19.9375, 22.0, 25.0625, 24.5625, 25.3125, 29.6875, 32.12343750000001, 33.3125, 35.5, 38.8125, 37.3125, 36.99843750000001, 41.3125, 43.75, 45.8125, 47.0, 48.9375, 46.3125, 44.0625, 49.375, 52.1875, 53.3125, 54.0625, 54.4375, 50.8125, 48.125, 52.8125, 55.5625, 56.5, 56.6875, 55.4375, 51.125, 48.5625, 55.8125, 58.6875, 59.25, 59.0, 57.5625, 53.125, 49.5, 54.6875, 57.375, 57.8125, 57.5, 55.625, 51.5, 47.625, 52.875, 54.9375, 54.8125, 53.9375, 52.0, 47.9375, 44.375, 48.5625, 48.625, 47.5625, 46.8125, 44.99843750000001, 41.75, 38.75, 40.625, 39.25, 38.3125, 38.75, 39.5, 36.625, 34.375, 38.0, 37.0, 35.4375, 34.3125], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0625, 0.25, 0.25, 0.5, 0.75, 0.9375, 1.5625, 2.0625, 2.75, 3.75, 5.1875, 5.75, 6.75, 8.6875, 10.4375, 12.125, 14.0625, 16.5, 16.625, 17.25, 20.8125, 23.125, 24.6875, 26.9375, 29.9375, 29.125, 29.5625, 34.4375, 36.75, 38.1875, 40.25, 43.25, 41.25, 40.375, 44.625, 47.5, 49.375, 50.1875, 51.5625, 48.4375, 46.25, 51.25, 53.9375, 55.125, 55.375, 55.3125, 51.5, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">48.6875, 53.25, 56.125, 57.125, 57.0, 55.875, 51.4375, 49.1875, 56.125, 58.875, 59.5, 59.0, 57.875, 53.4375, 49.9375, 54.9375, 57.625, 57.9375, 57.75, 56.0625, 51.875, 48.125, 53.1875, 55.3125, 55.3125, 54.4375, 52.6875, 48.5625, 45.0, 49.3125, 49.75, 48.9375, 48.0, 46.1875, 42.875, 39.75, 42.0, 41.1875, 40.125, 40.3125, 40.875, 37.9375, 35.4375, 39.0625, 38.0, 36.5625, 35.625], [0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.1875, 0.5, 0.5, 0.875, 1.25, 1.5, 2.25, 3.0, 4.064062499999977, 5.5625, 7.6875, 8.25, 9.4375, 12.0, 14.125, 16.0, 18.0625, 20.875, 20.75, 21.4375, 25.375, 28.0, 29.501562499999977, 32.0625, 34.8125, 33.375, 33.6875, 39.125, 41.375, 42.9375, 44.9375, 47.25, 44.875, 43.4375, 47.625, 50.8125, 52.625, 52.9375, 53.75, 50.1875, 48.0, 52.8125, 55.4375, 56.625, 56.4375, 56.125, 52.125, 49.1875, 53.6875, 56.625, 57.625, 57.3125, 56.25, 51.8125, 49.8125, 56.4375, 59.0, 59.75, 59.0, 58.1875, 53.75, 50.375, 55.1875, 57.875, 58.0, 57.9375, 56.4375, 52.25, 48.625, 53.5, 55.6875, 55.75, 54.9375, 53.375, 49.1875, 45.625, 50.0625, 50.8125, 50.3125, 49.25, 47.4375, 43.93906249999998, 40.75, 43.25, 43.1875, 41.9375, 41.875, 42.3125, 39.1875, 36.5625, 40.18906249999998, 39.125, 37.6875, 37.06406249999998]), ([0.0, 0.25, 0.9375, 1.8125, 3.5, 5.375, 6.3125, 8.1875, 11.8125, 17.625, 22.74843750000001, 29.5, 39.43593750000001, 45.1875, 52.5625, 72.8125, 92.43593750000001, 113.3125, 141.5609375, 176.9953125, 201.9984375, 229.49375000000003, 270.0625, 309.371875, 364.9359375, 412.11406250000005, 475.24218750000006, 523.9984375, 578.434375, 652.6859375, 729.303125, 815.3000000000001, 914.60625, 1021.3703125000001, 1090.4828125000001, 1170.0968750000002, 1290.7828125, 1418.4531250000002, 1536.4265625, 1682.18125, 1821.1171875, 1931.425, 2038.5125000000003, 2208.990625, 2370.934375, 2520.228125, 2673.3578125, 2866.6828125, 3003.1234375, 3134.5546875, 3313.4359375, 3497.7453125, 3689.184375, 3889.890625, 4076.58125, 4232.2484375, 4350.490625, 4552.2375, 4779.1078125, 4997.4328125, 5202.871875, 5404.40625, 5540.4359375, 5659.4515625, 5873.6234375, 6113.8734375, 6343.7453125, 6565.689062500001, 6755.46875, 6871.7296875, 6978.9296875, 7339.9359375, 7738.587500000001, 8109.93125, 8388.471875, 8598.3953125, 8707.353125, 8809.4921875, 9068.2296875, 9417.8109375, 9732.73125, 9981.8046875, 10165.0484375, 10257.3109375, 10342.525, 10556.68125, 10810.4984375, 11019.309375, 11196.4828125, 11350.559375, 11404.8109375, 11477.4796875, 11641.6046875, 11780.9921875, 11918.6234375, 12042.8734375, 12149.68125, 12203.615625, 12254.109375, 12360.121875, 12460.3703125, 12550.8046875, 12645.25, 12746.54375, 12796.3734375, 12843.3125, 12945.1828125, 13027.1875, 13104.6875, 13185.121875, 13267.18125, 13303.684375], [0.0, 0.875, 1.875, 3.3125, 5.6875, 8.6875, 9.8125, 12.625, 18.625, 26.1875, 33.5625, 44.1875, 58.3125, 66.3125, 77.0, 101.25, 129.5625, 158.1875, 195.1875, 243.625, 275.875, 310.8125, 362.125, 417.5625, 480.5, 545.375, 621.875, 682.0, 744.6875, 835.5, 924.625, 1026.9375, 1133.875, 1253.75, 1338.9375, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1433.0, 1569.3125, 1703.0625, 1838.75, 1982.9375, 2139.25, 2254.25, 2375.875, 2551.125, 2718.9375, 2885.3125, 3060.1875, 3249.75, 3381.5625, 3516.9375, 3703.125, 3901.6875, 4104.9375, 4301.375, 4500.625, 4635.8125, 4765.1875, 4974.5625, </t>
+  </si>
+  <si>
+    <t>5194.3125, 5414.4375, 5619.0625, 5818.9375, 5939.3125, 6057.5625, 6262.9375, 6497.625, 6734.125, 6942.5625, 7124.3125, 7227.5625, 7342.8125, 7690.5, 8080.6875, 8441.0, 8716.3125, 8924.0, 9011.25, 9104.1875, 9365.1875, 9710.8125, 10011.875, 10247.6875, 10421.8125, 10499.4375, 10576.9375, 10788.4375, 11026.75, 11226.5, 11396.8125, 11533.8125, 11594.625, 11658.875, 11811.0, 11947.9375, 12070.375, 12187.5625, 12292.4375, 12342.5, 12394.0, 12493.6875, 12581.9375, 12667.1875, 12757.1875, 12851.375, 12897.625, 12940.375, 13038.125, 13116.375, 13190.125, 13265.0, 13340.5625, 13377.875], [0.0, 1.5625, 2.9375, 4.9375, 8.0625, 12.5625, 13.75, 17.75, 25.9375, 36.12656249999998, 45.56406249999998, 59.315624999999955, 78.56562499999995, 89.87656249999998, 103.56874999999991, 132.6875, 170.625, 207.12656249999998, 255.25312499999995, 315.6937499999999, 357.4499999999998, 399.5062499999999, 459.75937499999986, 526.753125, 605.3140625, 687.3171874999999, 773.2515625, 844.5640625, 921.5640625, 1028.0718749999999, 1128.0734374999997, 1245.6875, 1374.1296874999998, 1500.5781249999998, 1601.5109374999997, 1710.9468749999999, 1850.5171874999996, 1989.0156249999998, 2141.5, 2300.88125, 2470.13125, 2590.1359374999997, 2716.5265624999997, 2893.0671875, 3071.568749999999, 3252.1875, 3439.575, 3638.9453125, 3770.315625, 3901.7906249999996, 4087.2546875, 4297.071875, 4517.4421875, 4705.440624999999, 4908.8484375, 5034.5953125, 5168.4625, 5370.065625, 5592.5046875, 5830.537499999999, 6006.075, 6204.9375, 6314.4484375, 6425.3796875, 6627.75, 6871.8171875, 7096.393749999999, 7307.3765625, 7494.828125, 7575.639062499999, 7678.259375, 8036.6921875, 8422.75, 8771.45625, 9035.828125, 9235.125, 9307.6875, 9418.253125, 9664.5671875, 9988.7046875, 10265.895312499999, 10511.7, 10667.8890625, 10745.8171875, 10811.9421875, 11012.2515625, 11235.75625, 11413.196875, 11584.6875, 11723.2546875, 11775.2578125, 11843.4015625, 11979.5671875, 12105.6921875, 12217.5, 12328.69375, 12434.3875, 12477.81875, 12527.2515625, 12615.821875, 12696.75, 12779.89375, 12862.3765625, 12950.5703125, 12992.6953125, 13032.6890625, 13129.440625, 13202.628125, 13274.2515625, 13343.375, 13414.9421875, 13447.071875]))</t>
   </si>
 </sst>
 </file>
@@ -3715,6 +4128,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>77147</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>10164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AEBFF72-445A-442B-952D-C1BB51FFB22B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="22679025"/>
+          <a:ext cx="6782747" cy="4582164"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>115252</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>133980</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7A7504F-FEF5-491A-9D26-E1F2DA41F26B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="27632025"/>
+          <a:ext cx="6820852" cy="4515480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8369,6 +8875,379 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13180C0C-3E73-485D-BB5E-B98AD41D6776}">
+  <dimension ref="A1:C72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="C13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="C17" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="C20" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22">
+        <v>1.2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="C23" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="C24" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="C25" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="C26" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="C27" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>443</v>
+      </c>
+      <c r="C29" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="C30" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="C31" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="C32" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="C33" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="C36" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="C37" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="C38" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="C39" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="C42" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="C43" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="C44" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="C45" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="C46" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="C47" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="C50" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="C51" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="C52" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="C53" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="C54" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="C55" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>50</v>
+      </c>
+      <c r="C57" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="C58" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>-5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="C62" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="C63" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="C64" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="C65" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="C66" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>-10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="C69" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="C70" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="C71" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="C72" t="s">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3AD7C4-874C-4686-AAC5-4658CBE0AE83}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A28FB15-96AC-4A27-8F42-1357F430FE8B}">
   <dimension ref="A1:M174"/>
@@ -12549,7 +13428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7305D22-1091-4105-A4AF-50E66E4E5D50}">
   <dimension ref="A1:AI412"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A381" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB385" sqref="AB385"/>
     </sheetView>
   </sheetViews>
@@ -13293,10 +14172,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61788BDA-4C45-44A2-BFF7-0EB5F25B5DC0}">
-  <dimension ref="A1:DI152"/>
+  <dimension ref="A1:DI168"/>
   <sheetViews>
-    <sheetView topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:DI15"/>
+    <sheetView topLeftCell="X139" zoomScale="105" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AF108" sqref="AF108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14276,7 +15155,7 @@
     </row>
     <row r="15" spans="1:113">
       <c r="A15">
-        <f t="shared" ref="A14:P15" si="4">AVERAGE(A25,A32,A39,A46,A53,A74,A60,A81,A67)</f>
+        <f t="shared" ref="A15:P15" si="4">AVERAGE(A25,A32,A39,A46,A53,A74,A60,A81,A67)</f>
         <v>0</v>
       </c>
       <c r="B15">
@@ -16800,7 +17679,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:112">
+    <row r="34" spans="1:112" ht="90">
       <c r="A34" s="3" t="s">
         <v>205</v>
       </c>
@@ -17143,7 +18022,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:112">
+    <row r="36" spans="1:112" ht="75">
       <c r="A36" s="3" t="s">
         <v>206</v>
       </c>
@@ -17486,7 +18365,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:112">
+    <row r="38" spans="1:112" ht="90">
       <c r="A38" s="3" t="s">
         <v>207</v>
       </c>
@@ -18868,7 +19747,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:112">
+    <row r="48" spans="1:112" ht="90">
       <c r="A48" s="3" t="s">
         <v>211</v>
       </c>
@@ -19211,7 +20090,7 @@
         <v>34.875</v>
       </c>
     </row>
-    <row r="50" spans="1:112">
+    <row r="50" spans="1:112" ht="75">
       <c r="A50" s="3" t="s">
         <v>212</v>
       </c>
@@ -20936,7 +21815,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:112">
+    <row r="62" spans="1:112" ht="90">
       <c r="A62" s="3" t="s">
         <v>218</v>
       </c>
@@ -21279,7 +22158,7 @@
         <v>33.375</v>
       </c>
     </row>
-    <row r="64" spans="1:112">
+    <row r="64" spans="1:112" ht="75">
       <c r="A64" s="3" t="s">
         <v>219</v>
       </c>
@@ -24141,7 +25020,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:24">
       <c r="A98" t="s">
         <v>244</v>
       </c>
@@ -24149,7 +25028,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:24">
       <c r="A99" t="s">
         <v>245</v>
       </c>
@@ -24157,7 +25036,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:24">
       <c r="A100" t="s">
         <v>246</v>
       </c>
@@ -24165,7 +25044,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:24">
       <c r="A101" t="s">
         <v>247</v>
       </c>
@@ -24173,214 +25052,412 @@
         <v>251</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="102" spans="1:24">
+      <c r="K102" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24">
       <c r="A103" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:24">
       <c r="A104" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:24">
       <c r="A105" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:24">
       <c r="A106" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:24">
       <c r="A107" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:24">
       <c r="A108" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:24">
       <c r="A110" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:24">
       <c r="A111" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:24">
       <c r="A112" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="X112" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24">
+      <c r="X113" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24">
       <c r="A114" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="X114" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24">
       <c r="A115" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="X115" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24">
       <c r="A116" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="X116" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24">
       <c r="A117" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="X117" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24">
+      <c r="X118" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24">
       <c r="A119" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="X119" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24">
       <c r="A120" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="X120" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24">
       <c r="A121" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="X121" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24">
       <c r="A122" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="X122" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24">
       <c r="A123" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="X123" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24">
       <c r="A124" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="X124" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24">
+      <c r="X125" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24">
       <c r="A126" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="X126" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="127" spans="1:24">
       <c r="A127" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="X127" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24">
       <c r="A128" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="K128" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24">
+      <c r="X129" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24">
       <c r="A130" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="X130" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24">
       <c r="A131" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="X131" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24">
       <c r="A132" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:24">
       <c r="A133" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="X133" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24">
+      <c r="X134" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24">
       <c r="A135" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="X135" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24">
       <c r="A136" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="X136" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="137" spans="1:24">
       <c r="A137" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:24">
       <c r="A138" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="X138" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24">
       <c r="A139" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="X139" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="140" spans="1:24">
       <c r="A140" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="X140" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24">
+      <c r="X141" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24">
       <c r="A142" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="X142" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="143" spans="1:24">
       <c r="A143" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
+      <c r="X143" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="144" spans="1:24">
       <c r="A144" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="145" spans="1:24">
+      <c r="X145" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24">
       <c r="A146" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="X146" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24">
       <c r="A147" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="X147" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24">
       <c r="A148" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:24">
       <c r="A149" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="X149" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24">
+      <c r="X150" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24">
       <c r="A151" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="X151" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24">
       <c r="A152" t="s">
         <v>335</v>
+      </c>
+      <c r="X152" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="154" spans="1:24">
+      <c r="X154" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="155" spans="1:24">
+      <c r="X155" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="156" spans="1:24">
+      <c r="X156" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="157" spans="1:24">
+      <c r="X157" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="158" spans="1:24">
+      <c r="X158" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="159" spans="1:24">
+      <c r="X159" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="161" spans="24:24">
+      <c r="X161" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="162" spans="24:24">
+      <c r="X162" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="163" spans="24:24">
+      <c r="X163" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="165" spans="24:24">
+      <c r="X165" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="166" spans="24:24">
+      <c r="X166" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="167" spans="24:24">
+      <c r="X167" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="168" spans="24:24">
+      <c r="X168" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -24388,8 +25465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D9806C-BE2C-4454-9916-82735BC390F4}">
   <dimension ref="A1:DH102"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30021,7 +31098,7 @@
     </row>
     <row r="40" spans="1:112">
       <c r="A40">
-        <f t="shared" ref="A39:P40" si="2">AVERAGE(A5,A12,A19,A26,A32)</f>
+        <f t="shared" ref="A40:P40" si="2">AVERAGE(A5,A12,A19,A26,A32)</f>
         <v>0</v>
       </c>
       <c r="B40">
@@ -30931,6 +32008,15 @@
       <c r="G44" t="s">
         <v>340</v>
       </c>
+      <c r="O44" t="s">
+        <v>366</v>
+      </c>
+      <c r="R44" t="s">
+        <v>378</v>
+      </c>
+      <c r="V44" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="45" spans="1:112">
       <c r="A45" t="s">
@@ -30939,6 +32025,12 @@
       <c r="G45" t="s">
         <v>265</v>
       </c>
+      <c r="O45" t="s">
+        <v>348</v>
+      </c>
+      <c r="V45" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="46" spans="1:112">
       <c r="A46" t="s">
@@ -30947,6 +32039,12 @@
       <c r="G46" t="s">
         <v>253</v>
       </c>
+      <c r="O46" t="s">
+        <v>367</v>
+      </c>
+      <c r="V46" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="47" spans="1:112">
       <c r="A47" t="s">
@@ -30955,6 +32053,12 @@
       <c r="G47" t="s">
         <v>163</v>
       </c>
+      <c r="O47" t="s">
+        <v>368</v>
+      </c>
+      <c r="V47" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="48" spans="1:112">
       <c r="A48" t="s">
@@ -30963,66 +32067,114 @@
       <c r="G48" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="O48" t="s">
+        <v>351</v>
+      </c>
+      <c r="V48" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>290</v>
       </c>
       <c r="G49" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="O49" t="s">
+        <v>369</v>
+      </c>
+      <c r="V49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>291</v>
       </c>
       <c r="G50" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="O50" t="s">
+        <v>370</v>
+      </c>
+      <c r="V50" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="O51" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
         <v>293</v>
       </c>
       <c r="G52" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="O52" t="s">
+        <v>371</v>
+      </c>
+      <c r="V52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
       <c r="A53" t="s">
         <v>294</v>
       </c>
       <c r="G53" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="O53" t="s">
+        <v>372</v>
+      </c>
+      <c r="V53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>295</v>
       </c>
       <c r="G54" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="O54" t="s">
+        <v>252</v>
+      </c>
+      <c r="V54" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="O55" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>252</v>
       </c>
       <c r="G56" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="O56" t="s">
+        <v>163</v>
+      </c>
+      <c r="V56" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" t="s">
         <v>253</v>
       </c>
@@ -31032,16 +32184,28 @@
       <c r="H57" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="O57" t="s">
+        <v>254</v>
+      </c>
+      <c r="V57" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22">
       <c r="A58" t="s">
         <v>163</v>
       </c>
       <c r="G58" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="O58" t="s">
+        <v>255</v>
+      </c>
+      <c r="V58" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -31051,178 +32215,299 @@
       <c r="H59" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="O59" t="s">
+        <v>357</v>
+      </c>
+      <c r="V59" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="O61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="O62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="O63" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="O65" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="O66" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="O67" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="O68" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="O70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="O71" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="O72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="O73" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="O74" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="O75" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="O77" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="O78" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="O79" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="O81" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="O82" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="O83" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="O84" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="O86" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="O87" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="O88" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="O89" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="O90" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="O91" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="O93" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="O94" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="O95" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="O97" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
+      <c r="O98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="O99" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="O100" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>260</v>
       </c>
@@ -31234,10 +32519,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B815A55-507A-49C8-AFFB-C13029AB3631}">
-  <dimension ref="A1:DH24"/>
+  <dimension ref="A1:DH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32280,6 +33565,12 @@
       <c r="A9" t="s">
         <v>344</v>
       </c>
+      <c r="G9" t="s">
+        <v>383</v>
+      </c>
+      <c r="L9" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="10" spans="1:112">
       <c r="A10" t="s">
@@ -32290,66 +33581,318 @@
       <c r="A11" t="s">
         <v>253</v>
       </c>
+      <c r="G11" t="s">
+        <v>384</v>
+      </c>
+      <c r="L11" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="12" spans="1:112">
       <c r="A12" t="s">
         <v>163</v>
       </c>
+      <c r="G12" t="s">
+        <v>306</v>
+      </c>
+      <c r="L12" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="13" spans="1:112">
       <c r="A13" t="s">
         <v>254</v>
       </c>
+      <c r="G13" t="s">
+        <v>385</v>
+      </c>
+      <c r="L13" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:112">
       <c r="A14" t="s">
         <v>255</v>
       </c>
+      <c r="G14" t="s">
+        <v>386</v>
+      </c>
+      <c r="L14" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="15" spans="1:112">
       <c r="A15" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="G15" t="s">
+        <v>387</v>
+      </c>
+      <c r="L15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:112">
+      <c r="G16" t="s">
+        <v>388</v>
+      </c>
+      <c r="L16" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="G18" t="s">
+        <v>389</v>
+      </c>
+      <c r="L18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="G19" t="s">
+        <v>390</v>
+      </c>
+      <c r="L19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="G20" t="s">
+        <v>252</v>
+      </c>
+      <c r="L20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="G21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>323</v>
       </c>
       <c r="B22" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="G22" t="s">
+        <v>163</v>
+      </c>
+      <c r="L22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="G23" t="s">
+        <v>254</v>
+      </c>
+      <c r="L23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>326</v>
       </c>
       <c r="B24" t="s">
         <v>327</v>
+      </c>
+      <c r="G24" t="s">
+        <v>255</v>
+      </c>
+      <c r="L24" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="G25" t="s">
+        <v>357</v>
+      </c>
+      <c r="L25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="G27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="G28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="G29" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="G31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="G32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7">
+      <c r="G34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7">
+      <c r="G36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7">
+      <c r="G37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7">
+      <c r="G38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7">
+      <c r="G39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7">
+      <c r="G40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7">
+      <c r="G41" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7">
+      <c r="G43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7">
+      <c r="G44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7">
+      <c r="G45" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7">
+      <c r="G47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7">
+      <c r="G48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7">
+      <c r="G49" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7">
+      <c r="G50" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7">
+      <c r="G52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7">
+      <c r="G53" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7">
+      <c r="G54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7">
+      <c r="G55" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7">
+      <c r="G56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7">
+      <c r="G57" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="59" spans="7:7">
+      <c r="G59" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7">
+      <c r="G60" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7">
+      <c r="G61" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7">
+      <c r="G63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7">
+      <c r="G64" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7">
+      <c r="G65" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7">
+      <c r="G66" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -32361,8 +33904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33E8C3A-FDA9-44C2-BD11-9FAB5F45F871}">
   <dimension ref="A1:DH66"/>
   <sheetViews>
-    <sheetView topLeftCell="CF1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView topLeftCell="K31" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49:M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33403,6 +34946,9 @@
       <c r="G8" t="s">
         <v>336</v>
       </c>
+      <c r="M8" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="9" spans="1:112">
       <c r="A9" t="s">
@@ -33411,6 +34957,9 @@
       <c r="G9" t="s">
         <v>265</v>
       </c>
+      <c r="M9" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="10" spans="1:112">
       <c r="A10" t="s">
@@ -33419,6 +34968,9 @@
       <c r="G10" t="s">
         <v>253</v>
       </c>
+      <c r="M10" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="11" spans="1:112">
       <c r="A11" t="s">
@@ -33427,6 +34979,9 @@
       <c r="G11" t="s">
         <v>163</v>
       </c>
+      <c r="M11" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="12" spans="1:112">
       <c r="A12" t="s">
@@ -33435,6 +34990,9 @@
       <c r="G12" t="s">
         <v>254</v>
       </c>
+      <c r="M12" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="13" spans="1:112">
       <c r="A13" t="s">
@@ -33443,6 +35001,9 @@
       <c r="G13" t="s">
         <v>255</v>
       </c>
+      <c r="M13" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="14" spans="1:112">
       <c r="A14" t="s">
@@ -33451,11 +35012,17 @@
       <c r="G14" t="s">
         <v>337</v>
       </c>
+      <c r="M14" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="15" spans="1:112">
       <c r="A15" t="s">
         <v>316</v>
       </c>
+      <c r="M15" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="16" spans="1:112">
       <c r="A16" t="s">
@@ -33464,37 +35031,52 @@
       <c r="G16" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="M16" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>318</v>
       </c>
       <c r="G17" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="M17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>319</v>
       </c>
       <c r="G18" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="M18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="M19" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>252</v>
       </c>
       <c r="G20" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="M20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>253</v>
       </c>
@@ -33504,16 +35086,22 @@
       <c r="H21" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="M21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>163</v>
       </c>
       <c r="G22" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="M22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -33523,180 +35111,340 @@
       <c r="H23" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="M23" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="M25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="M26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="M27" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="M29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="M30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="M31" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>323</v>
       </c>
       <c r="B32" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="M32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
         <v>326</v>
       </c>
       <c r="B34" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="M34" t="s">
+        <v>261</v>
+      </c>
+      <c r="S34" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="M35" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="M36" t="s">
+        <v>163</v>
+      </c>
+      <c r="S36" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="M37" t="s">
+        <v>254</v>
+      </c>
+      <c r="S37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="M38" t="s">
+        <v>255</v>
+      </c>
+      <c r="S38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="M39" t="s">
+        <v>408</v>
+      </c>
+      <c r="S39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="S40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="M41" t="s">
+        <v>164</v>
+      </c>
+      <c r="S41" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="M42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="M43" t="s">
+        <v>409</v>
+      </c>
+      <c r="S43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="S44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="M45" t="s">
+        <v>166</v>
+      </c>
+      <c r="S45" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="M46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="M47" t="s">
+        <v>410</v>
+      </c>
+      <c r="S47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" t="s">
         <v>323</v>
       </c>
       <c r="B48" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="M48" t="s">
+        <v>260</v>
+      </c>
+      <c r="S48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="M49" t="s">
+        <v>265</v>
+      </c>
+      <c r="S49" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>326</v>
       </c>
       <c r="B50" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="M50" t="s">
+        <v>253</v>
+      </c>
+      <c r="S50" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
+      <c r="M51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="M52" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="M53" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="M54" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="M56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="M57" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="M58" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="M60" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="M61" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="M62" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="M63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" t="s">
         <v>323</v>
       </c>

</xml_diff>